<commit_message>
Added MDM enrollment config
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616EE747-AA23-6441-BBA0-A864936673C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B5836A-86FD-6645-8253-DDA884E18F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-43300" yWindow="-20560" windowWidth="34960" windowHeight="18860" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="-82920" yWindow="-20700" windowWidth="34960" windowHeight="18860" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,7 @@
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
     <definedName name="Status">'Identity ✍️'!$AD$3:$AK$3</definedName>
+    <definedName name="Table_WindowsEnrollment">'Device ⚙️'!$D$56</definedName>
     <definedName name="WorkshopData" localSheetId="2">'Device ✍️'!$A$2:$AA$216</definedName>
     <definedName name="WorkshopData">'Identity ✍️'!$A$2:$AA$212</definedName>
   </definedNames>
@@ -1144,7 +1145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="256">
   <si>
     <t>Devices</t>
   </si>
@@ -1903,12 +1904,24 @@
   <si>
     <t>Intune Configuration Assessment</t>
   </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Applies to</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>📌</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="39">
+  <fonts count="43">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2155,6 +2168,32 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Segoe UI Semibold"/>
     </font>
   </fonts>
   <fills count="22">
@@ -2562,14 +2601,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2730,18 +2770,6 @@
     </xf>
     <xf numFmtId="0" fontId="32" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="34" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2868,10 +2896,30 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Per cent" xfId="1" builtinId="5"/>
@@ -42433,27 +42481,27 @@
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
+      <c r="F5" s="114"/>
+      <c r="G5" s="114"/>
+      <c r="H5" s="114"/>
       <c r="I5" s="33"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="73"/>
-      <c r="N5" s="73"/>
-      <c r="O5" s="73"/>
-      <c r="P5" s="73"/>
+      <c r="J5" s="115"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="115"/>
       <c r="Q5" s="34"/>
       <c r="R5" s="34"/>
       <c r="S5" s="34"/>
       <c r="T5" s="34"/>
       <c r="U5" s="34"/>
       <c r="V5" s="33"/>
-      <c r="W5" s="73"/>
-      <c r="X5" s="73"/>
-      <c r="Y5" s="73"/>
-      <c r="Z5" s="73"/>
+      <c r="W5" s="115"/>
+      <c r="X5" s="115"/>
+      <c r="Y5" s="115"/>
+      <c r="Z5" s="115"/>
       <c r="AA5" s="15"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -45875,9 +45923,9 @@
   </sheetPr>
   <dimension ref="A1:AK154"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="Y1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC3" sqref="AC3:AK3"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="30" customHeight="1"/>
@@ -45907,8 +45955,8 @@
     <col min="25" max="25" width="2" style="16" customWidth="1"/>
     <col min="26" max="26" width="22" style="16" customWidth="1"/>
     <col min="27" max="28" width="10.83203125" style="16"/>
-    <col min="29" max="29" width="10.83203125" style="16" customWidth="1"/>
-    <col min="30" max="37" width="25.83203125" style="16" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" style="16" hidden="1" customWidth="1"/>
+    <col min="30" max="37" width="25.83203125" style="16" hidden="1" customWidth="1"/>
     <col min="38" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
@@ -46043,27 +46091,27 @@
       <c r="C5" s="52"/>
       <c r="D5" s="52"/>
       <c r="E5" s="52"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="F5" s="116"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
       <c r="I5" s="59"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
-      <c r="M5" s="75"/>
-      <c r="N5" s="75"/>
-      <c r="O5" s="75"/>
-      <c r="P5" s="75"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
       <c r="Q5" s="60"/>
       <c r="R5" s="60"/>
       <c r="S5" s="60"/>
       <c r="T5" s="60"/>
       <c r="U5" s="60"/>
       <c r="V5" s="59"/>
-      <c r="W5" s="75"/>
-      <c r="X5" s="75"/>
-      <c r="Y5" s="75"/>
-      <c r="Z5" s="75"/>
+      <c r="W5" s="117"/>
+      <c r="X5" s="117"/>
+      <c r="Y5" s="117"/>
+      <c r="Z5" s="117"/>
       <c r="AA5" s="52"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -48676,9 +48724,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
-  <dimension ref="A1:AF50"/>
+  <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="N54" sqref="N54"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
   <cols>
@@ -49132,7 +49182,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="3:9">
+    <row r="49" spans="3:11">
       <c r="C49" s="5" t="s">
         <v>33</v>
       </c>
@@ -49147,7 +49197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="3:9">
+    <row r="50" spans="3:11">
       <c r="C50" s="5" t="s">
         <v>34</v>
       </c>
@@ -49162,10 +49212,51 @@
         <v>3</v>
       </c>
     </row>
+    <row r="54" spans="3:11" ht="28">
+      <c r="C54" s="118" t="s">
+        <v>255</v>
+      </c>
+      <c r="D54" s="119" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="55" spans="3:11">
+      <c r="D55" s="120" t="s">
+        <v>254</v>
+      </c>
+      <c r="E55" s="122" t="s">
+        <v>252</v>
+      </c>
+      <c r="F55" s="122"/>
+      <c r="G55" s="122"/>
+      <c r="H55" s="122"/>
+      <c r="I55" s="122"/>
+      <c r="J55" s="122" t="s">
+        <v>253</v>
+      </c>
+      <c r="K55" s="122"/>
+    </row>
+    <row r="56" spans="3:11">
+      <c r="D56" s="121"/>
+      <c r="E56" s="121"/>
+      <c r="F56" s="121"/>
+      <c r="G56" s="121"/>
+      <c r="H56" s="121"/>
+      <c r="I56" s="121"/>
+      <c r="J56" s="121"/>
+      <c r="K56" s="121"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E55:I55"/>
+    <mergeCell ref="J55:K55"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C54" r:id="rId1" location="view/Microsoft_AAD_IAM/MdmAppsListBlade" xr:uid="{7CC02CD1-5A3A-C841-B0E4-23769402B4DC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -49397,7 +49488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
   <dimension ref="A1:AF397"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -49557,1555 +49648,1555 @@
       <c r="T5" s="68"/>
       <c r="U5" s="68"/>
     </row>
-    <row r="8" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B8" s="77" t="s">
+    <row r="8" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B8" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="96" t="s">
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78" t="s">
+      <c r="G8" s="74"/>
+      <c r="H8" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="78" t="s">
+      <c r="I8" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="J8" s="78" t="s">
+      <c r="J8" s="74" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="79" t="s">
+      <c r="K8" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="80"/>
-      <c r="M8" s="80"/>
-    </row>
-    <row r="9" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B9" s="81" t="s">
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+    </row>
+    <row r="9" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B9" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="82"/>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="84"/>
-    </row>
-    <row r="10" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B10" s="85"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103" t="s">
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="93"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="10" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B10" s="81"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="99" t="s">
         <v>250</v>
       </c>
-      <c r="H10" s="103"/>
-      <c r="I10" s="103" t="s">
+      <c r="H10" s="99"/>
+      <c r="I10" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="103"/>
-      <c r="K10" s="104"/>
-    </row>
-    <row r="11" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B11" s="85"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106" t="s">
+      <c r="J10" s="99"/>
+      <c r="K10" s="100"/>
+    </row>
+    <row r="11" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B11" s="81"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="101"/>
+      <c r="G11" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="106"/>
-      <c r="I11" s="106" t="s">
+      <c r="H11" s="102"/>
+      <c r="I11" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="J11" s="106"/>
-      <c r="K11" s="107"/>
-    </row>
-    <row r="12" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B12" s="85"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="108"/>
-      <c r="G12" s="109" t="s">
+      <c r="J11" s="102"/>
+      <c r="K11" s="103"/>
+    </row>
+    <row r="12" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B12" s="81"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="104"/>
+      <c r="G12" s="105" t="s">
         <v>41</v>
       </c>
-      <c r="H12" s="109"/>
-      <c r="I12" s="109" t="s">
+      <c r="H12" s="105"/>
+      <c r="I12" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="J12" s="109"/>
-      <c r="K12" s="110"/>
-    </row>
-    <row r="13" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B13" s="81" t="s">
+      <c r="J12" s="105"/>
+      <c r="K12" s="106"/>
+    </row>
+    <row r="13" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B13" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="87"/>
-      <c r="K13" s="88"/>
-    </row>
-    <row r="14" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B14" s="89"/>
-      <c r="F14" s="102"/>
-      <c r="G14" s="103" t="s">
+      <c r="C13" s="77"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="77"/>
+      <c r="F13" s="94"/>
+      <c r="G13" s="77"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="83"/>
+      <c r="K13" s="84"/>
+    </row>
+    <row r="14" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B14" s="85"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="103"/>
-      <c r="I14" s="103" t="s">
+      <c r="H14" s="99"/>
+      <c r="I14" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="103"/>
-      <c r="K14" s="104"/>
-    </row>
-    <row r="15" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B15" s="89"/>
-      <c r="F15" s="105"/>
-      <c r="G15" s="106" t="s">
+      <c r="J14" s="99"/>
+      <c r="K14" s="100"/>
+    </row>
+    <row r="15" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B15" s="85"/>
+      <c r="F15" s="101"/>
+      <c r="G15" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="106"/>
-      <c r="I15" s="106" t="s">
+      <c r="H15" s="102"/>
+      <c r="I15" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="106"/>
-      <c r="K15" s="107"/>
-    </row>
-    <row r="16" spans="1:32" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B16" s="89"/>
-      <c r="F16" s="111"/>
-      <c r="G16" s="106" t="s">
+      <c r="J15" s="102"/>
+      <c r="K15" s="103"/>
+    </row>
+    <row r="16" spans="1:32" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B16" s="85"/>
+      <c r="F16" s="107"/>
+      <c r="G16" s="102" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="106"/>
-      <c r="I16" s="106" t="s">
+      <c r="H16" s="102"/>
+      <c r="I16" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="J16" s="106"/>
-      <c r="K16" s="107"/>
-    </row>
-    <row r="17" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B17" s="89"/>
-      <c r="F17" s="108"/>
-      <c r="G17" s="109" t="s">
+      <c r="J16" s="102"/>
+      <c r="K16" s="103"/>
+    </row>
+    <row r="17" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B17" s="85"/>
+      <c r="F17" s="104"/>
+      <c r="G17" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="109"/>
-      <c r="I17" s="109" t="s">
+      <c r="H17" s="105"/>
+      <c r="I17" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="J17" s="109"/>
-      <c r="K17" s="110"/>
-    </row>
-    <row r="18" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B18" s="81" t="s">
+      <c r="J17" s="105"/>
+      <c r="K17" s="106"/>
+    </row>
+    <row r="18" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B18" s="77" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="81"/>
-      <c r="D18" s="81"/>
-      <c r="E18" s="81"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="81"/>
-      <c r="H18" s="87"/>
-      <c r="I18" s="87"/>
-      <c r="J18" s="87"/>
-      <c r="K18" s="88"/>
-    </row>
-    <row r="19" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B19" s="81" t="s">
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="83"/>
+      <c r="I18" s="83"/>
+      <c r="J18" s="83"/>
+      <c r="K18" s="84"/>
+    </row>
+    <row r="19" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B19" s="77" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="81"/>
-      <c r="D19" s="81"/>
-      <c r="E19" s="81"/>
-      <c r="F19" s="98"/>
-      <c r="G19" s="81"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="87"/>
-      <c r="K19" s="88"/>
-    </row>
-    <row r="20" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B20" s="89"/>
-      <c r="F20" s="102"/>
-      <c r="G20" s="103" t="s">
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="83"/>
+      <c r="I19" s="83"/>
+      <c r="J19" s="83"/>
+      <c r="K19" s="84"/>
+    </row>
+    <row r="20" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B20" s="85"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="99" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="103"/>
-      <c r="I20" s="103" t="s">
+      <c r="H20" s="99"/>
+      <c r="I20" s="99" t="s">
         <v>75</v>
       </c>
-      <c r="J20" s="103"/>
-      <c r="K20" s="104"/>
-    </row>
-    <row r="21" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B21" s="89"/>
-      <c r="F21" s="111"/>
-      <c r="G21" s="106" t="s">
+      <c r="J20" s="99"/>
+      <c r="K20" s="100"/>
+    </row>
+    <row r="21" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B21" s="85"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106" t="s">
+      <c r="H21" s="102"/>
+      <c r="I21" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="J21" s="106"/>
-      <c r="K21" s="107"/>
-    </row>
-    <row r="22" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B22" s="89"/>
-      <c r="F22" s="111"/>
-      <c r="G22" s="106" t="s">
+      <c r="J21" s="102"/>
+      <c r="K21" s="103"/>
+    </row>
+    <row r="22" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B22" s="85"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="H22" s="106"/>
-      <c r="I22" s="106" t="s">
+      <c r="H22" s="102"/>
+      <c r="I22" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="J22" s="106"/>
-      <c r="K22" s="107"/>
-    </row>
-    <row r="23" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B23" s="89"/>
-      <c r="F23" s="112"/>
-      <c r="G23" s="106" t="s">
+      <c r="J22" s="102"/>
+      <c r="K22" s="103"/>
+    </row>
+    <row r="23" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B23" s="85"/>
+      <c r="F23" s="108"/>
+      <c r="G23" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="H23" s="106"/>
-      <c r="I23" s="106" t="s">
+      <c r="H23" s="102"/>
+      <c r="I23" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="J23" s="106"/>
-      <c r="K23" s="107"/>
-    </row>
-    <row r="24" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B24" s="89"/>
-      <c r="F24" s="111"/>
-      <c r="G24" s="106" t="s">
+      <c r="J23" s="102"/>
+      <c r="K23" s="103"/>
+    </row>
+    <row r="24" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B24" s="85"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="H24" s="106"/>
-      <c r="I24" s="106" t="s">
+      <c r="H24" s="102"/>
+      <c r="I24" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="J24" s="106"/>
-      <c r="K24" s="107"/>
-    </row>
-    <row r="25" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B25" s="89"/>
-      <c r="F25" s="113"/>
-      <c r="G25" s="109" t="s">
+      <c r="J24" s="102"/>
+      <c r="K24" s="103"/>
+    </row>
+    <row r="25" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B25" s="85"/>
+      <c r="F25" s="109"/>
+      <c r="G25" s="105" t="s">
         <v>57</v>
       </c>
-      <c r="H25" s="109"/>
-      <c r="I25" s="109" t="s">
+      <c r="H25" s="105"/>
+      <c r="I25" s="105" t="s">
         <v>76</v>
       </c>
-      <c r="J25" s="109"/>
-      <c r="K25" s="110"/>
-    </row>
-    <row r="26" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B26" s="81" t="s">
+      <c r="J25" s="105"/>
+      <c r="K25" s="106"/>
+    </row>
+    <row r="26" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B26" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="98"/>
-      <c r="G26" s="81"/>
-      <c r="H26" s="87"/>
-      <c r="I26" s="87"/>
-      <c r="J26" s="87"/>
-      <c r="K26" s="88"/>
-    </row>
-    <row r="27" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B27" s="89"/>
-      <c r="F27" s="102"/>
-      <c r="G27" s="103" t="s">
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="94"/>
+      <c r="G26" s="77"/>
+      <c r="H26" s="83"/>
+      <c r="I26" s="83"/>
+      <c r="J26" s="83"/>
+      <c r="K26" s="84"/>
+    </row>
+    <row r="27" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B27" s="85"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="99" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="103"/>
-      <c r="I27" s="103"/>
-      <c r="J27" s="103"/>
-      <c r="K27" s="104"/>
-    </row>
-    <row r="28" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B28" s="89"/>
-      <c r="F28" s="111"/>
-      <c r="G28" s="106" t="s">
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="100"/>
+    </row>
+    <row r="28" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B28" s="85"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="107"/>
-    </row>
-    <row r="29" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B29" s="89"/>
-      <c r="F29" s="114"/>
-      <c r="G29" s="109" t="s">
+      <c r="H28" s="102"/>
+      <c r="I28" s="102"/>
+      <c r="J28" s="102"/>
+      <c r="K28" s="103"/>
+    </row>
+    <row r="29" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B29" s="85"/>
+      <c r="F29" s="110"/>
+      <c r="G29" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="109"/>
-      <c r="I29" s="109"/>
-      <c r="J29" s="109"/>
-      <c r="K29" s="110"/>
-    </row>
-    <row r="30" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B30" s="81" t="s">
+      <c r="H29" s="105"/>
+      <c r="I29" s="105"/>
+      <c r="J29" s="105"/>
+      <c r="K29" s="106"/>
+    </row>
+    <row r="30" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B30" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="98"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="87"/>
-      <c r="I30" s="87"/>
-      <c r="J30" s="87"/>
-      <c r="K30" s="88"/>
-    </row>
-    <row r="31" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B31" s="89"/>
-      <c r="F31" s="115"/>
-      <c r="G31" s="103" t="s">
+      <c r="C30" s="86"/>
+      <c r="D30" s="86"/>
+      <c r="E30" s="86"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="83"/>
+      <c r="H30" s="83"/>
+      <c r="I30" s="83"/>
+      <c r="J30" s="83"/>
+      <c r="K30" s="84"/>
+    </row>
+    <row r="31" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B31" s="85"/>
+      <c r="F31" s="111"/>
+      <c r="G31" s="99" t="s">
         <v>66</v>
       </c>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="104"/>
-    </row>
-    <row r="32" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B32" s="89"/>
-      <c r="F32" s="116"/>
-      <c r="G32" s="106" t="s">
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="100"/>
+    </row>
+    <row r="32" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B32" s="85"/>
+      <c r="F32" s="112"/>
+      <c r="G32" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
-      <c r="K32" s="107"/>
-    </row>
-    <row r="33" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B33" s="89"/>
-      <c r="F33" s="105"/>
-      <c r="G33" s="106" t="s">
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
+      <c r="J32" s="102"/>
+      <c r="K32" s="103"/>
+    </row>
+    <row r="33" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B33" s="85"/>
+      <c r="F33" s="101"/>
+      <c r="G33" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="H33" s="106"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="107"/>
-    </row>
-    <row r="34" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B34" s="89"/>
-      <c r="F34" s="108"/>
-      <c r="G34" s="109" t="s">
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="103"/>
+    </row>
+    <row r="34" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B34" s="85"/>
+      <c r="F34" s="104"/>
+      <c r="G34" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
-      <c r="K34" s="110"/>
-    </row>
-    <row r="35" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B35" s="91" t="s">
+      <c r="H34" s="105"/>
+      <c r="I34" s="105"/>
+      <c r="J34" s="105"/>
+      <c r="K34" s="106"/>
+    </row>
+    <row r="35" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B35" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="92"/>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92"/>
-      <c r="F35" s="100"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="94"/>
-    </row>
-    <row r="36" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B36" s="81" t="s">
+      <c r="C35" s="88"/>
+      <c r="D35" s="88"/>
+      <c r="E35" s="88"/>
+      <c r="F35" s="96"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="90"/>
+    </row>
+    <row r="36" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B36" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="90"/>
-      <c r="D36" s="90"/>
-      <c r="E36" s="90"/>
-      <c r="F36" s="98"/>
-      <c r="G36" s="87"/>
-      <c r="H36" s="87"/>
-      <c r="I36" s="87"/>
-      <c r="J36" s="87"/>
-      <c r="K36" s="88"/>
-    </row>
-    <row r="37" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B37" s="89"/>
-      <c r="F37" s="102"/>
-      <c r="G37" s="103" t="s">
+      <c r="C36" s="86"/>
+      <c r="D36" s="86"/>
+      <c r="E36" s="86"/>
+      <c r="F36" s="94"/>
+      <c r="G36" s="83"/>
+      <c r="H36" s="83"/>
+      <c r="I36" s="83"/>
+      <c r="J36" s="83"/>
+      <c r="K36" s="84"/>
+    </row>
+    <row r="37" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B37" s="85"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="99" t="s">
         <v>74</v>
       </c>
-      <c r="H37" s="103"/>
-      <c r="I37" s="103"/>
-      <c r="J37" s="103"/>
-      <c r="K37" s="104"/>
-    </row>
-    <row r="38" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B38" s="89"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="106" t="s">
+      <c r="H37" s="99"/>
+      <c r="I37" s="99"/>
+      <c r="J37" s="99"/>
+      <c r="K37" s="100"/>
+    </row>
+    <row r="38" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B38" s="85"/>
+      <c r="F38" s="112"/>
+      <c r="G38" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="107"/>
-    </row>
-    <row r="39" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B39" s="89"/>
-      <c r="F39" s="116"/>
-      <c r="G39" s="106" t="s">
+      <c r="H38" s="102"/>
+      <c r="I38" s="102"/>
+      <c r="J38" s="102"/>
+      <c r="K38" s="103"/>
+    </row>
+    <row r="39" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B39" s="85"/>
+      <c r="F39" s="112"/>
+      <c r="G39" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="107"/>
-    </row>
-    <row r="40" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B40" s="89"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="106"/>
-      <c r="J40" s="106"/>
-      <c r="K40" s="107"/>
-    </row>
-    <row r="41" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B41" s="89"/>
-      <c r="F41" s="112"/>
-      <c r="G41" s="106"/>
-      <c r="H41" s="106"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="107"/>
-    </row>
-    <row r="42" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B42" s="89"/>
-      <c r="F42" s="112"/>
-      <c r="G42" s="106"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="106"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="107"/>
-    </row>
-    <row r="43" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B43" s="89"/>
-      <c r="F43" s="112"/>
-      <c r="G43" s="106"/>
-      <c r="H43" s="106"/>
-      <c r="I43" s="106"/>
-      <c r="J43" s="106"/>
-      <c r="K43" s="107"/>
-    </row>
-    <row r="44" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B44" s="89"/>
-      <c r="F44" s="112"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="106"/>
-      <c r="J44" s="106"/>
-      <c r="K44" s="107"/>
-    </row>
-    <row r="45" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="B45" s="95"/>
-      <c r="C45" s="83"/>
-      <c r="D45" s="83"/>
-      <c r="E45" s="83"/>
-      <c r="F45" s="117"/>
-      <c r="G45" s="109"/>
-      <c r="H45" s="109"/>
-      <c r="I45" s="109"/>
-      <c r="J45" s="109"/>
-      <c r="K45" s="110"/>
-    </row>
-    <row r="46" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F46" s="101"/>
-    </row>
-    <row r="47" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F47" s="101"/>
-    </row>
-    <row r="48" spans="2:11" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F48" s="101"/>
-    </row>
-    <row r="49" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F49" s="101"/>
-    </row>
-    <row r="50" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F50" s="101"/>
-    </row>
-    <row r="51" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F51" s="101"/>
-    </row>
-    <row r="52" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F52" s="101"/>
-    </row>
-    <row r="53" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F53" s="101"/>
-    </row>
-    <row r="54" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F54" s="101"/>
-    </row>
-    <row r="55" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F55" s="101"/>
-    </row>
-    <row r="56" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F56" s="101"/>
-    </row>
-    <row r="57" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F57" s="101"/>
-    </row>
-    <row r="58" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F58" s="101"/>
-    </row>
-    <row r="59" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F59" s="101"/>
-    </row>
-    <row r="60" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F60" s="101"/>
-    </row>
-    <row r="61" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F61" s="101"/>
-    </row>
-    <row r="62" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F62" s="101"/>
-    </row>
-    <row r="63" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F63" s="101"/>
-    </row>
-    <row r="64" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F64" s="101"/>
-    </row>
-    <row r="65" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F65" s="101"/>
-    </row>
-    <row r="66" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F66" s="101"/>
-    </row>
-    <row r="67" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F67" s="101"/>
-    </row>
-    <row r="68" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F68" s="101"/>
-    </row>
-    <row r="69" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F69" s="101"/>
-    </row>
-    <row r="70" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F70" s="101"/>
-    </row>
-    <row r="71" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F71" s="101"/>
-    </row>
-    <row r="72" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F72" s="101"/>
-    </row>
-    <row r="73" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F73" s="101"/>
-    </row>
-    <row r="74" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F74" s="101"/>
-    </row>
-    <row r="75" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F75" s="101"/>
-    </row>
-    <row r="76" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F76" s="101"/>
-    </row>
-    <row r="77" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F77" s="101"/>
-    </row>
-    <row r="78" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F78" s="101"/>
-    </row>
-    <row r="79" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F79" s="101"/>
-    </row>
-    <row r="80" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F80" s="101"/>
-    </row>
-    <row r="81" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F81" s="101"/>
-    </row>
-    <row r="82" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F82" s="101"/>
-    </row>
-    <row r="83" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F83" s="101"/>
-    </row>
-    <row r="84" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F84" s="101"/>
-    </row>
-    <row r="85" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F85" s="101"/>
-    </row>
-    <row r="86" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F86" s="101"/>
-    </row>
-    <row r="87" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F87" s="101"/>
-    </row>
-    <row r="88" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F88" s="101"/>
-    </row>
-    <row r="89" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F89" s="101"/>
-    </row>
-    <row r="90" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F90" s="101"/>
-    </row>
-    <row r="91" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F91" s="101"/>
-    </row>
-    <row r="92" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F92" s="101"/>
-    </row>
-    <row r="93" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F93" s="101"/>
-    </row>
-    <row r="94" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F94" s="101"/>
-    </row>
-    <row r="95" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F95" s="101"/>
-    </row>
-    <row r="96" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F96" s="101"/>
-    </row>
-    <row r="97" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F97" s="101"/>
-    </row>
-    <row r="98" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F98" s="101"/>
-    </row>
-    <row r="99" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F99" s="101"/>
-    </row>
-    <row r="100" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F100" s="101"/>
-    </row>
-    <row r="101" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F101" s="101"/>
-    </row>
-    <row r="102" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F102" s="101"/>
-    </row>
-    <row r="103" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F103" s="101"/>
-    </row>
-    <row r="104" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F104" s="101"/>
-    </row>
-    <row r="105" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F105" s="101"/>
-    </row>
-    <row r="106" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F106" s="101"/>
-    </row>
-    <row r="107" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F107" s="101"/>
-    </row>
-    <row r="108" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F108" s="101"/>
-    </row>
-    <row r="109" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F109" s="101"/>
-    </row>
-    <row r="110" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F110" s="101"/>
-    </row>
-    <row r="111" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F111" s="101"/>
-    </row>
-    <row r="112" spans="6:6" s="76" customFormat="1" ht="26" customHeight="1">
-      <c r="F112" s="101"/>
+      <c r="H39" s="102"/>
+      <c r="I39" s="102"/>
+      <c r="J39" s="102"/>
+      <c r="K39" s="103"/>
+    </row>
+    <row r="40" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B40" s="85"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="102"/>
+      <c r="H40" s="102"/>
+      <c r="I40" s="102"/>
+      <c r="J40" s="102"/>
+      <c r="K40" s="103"/>
+    </row>
+    <row r="41" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B41" s="85"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="102"/>
+      <c r="H41" s="102"/>
+      <c r="I41" s="102"/>
+      <c r="J41" s="102"/>
+      <c r="K41" s="103"/>
+    </row>
+    <row r="42" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B42" s="85"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="102"/>
+      <c r="I42" s="102"/>
+      <c r="J42" s="102"/>
+      <c r="K42" s="103"/>
+    </row>
+    <row r="43" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B43" s="85"/>
+      <c r="F43" s="108"/>
+      <c r="G43" s="102"/>
+      <c r="H43" s="102"/>
+      <c r="I43" s="102"/>
+      <c r="J43" s="102"/>
+      <c r="K43" s="103"/>
+    </row>
+    <row r="44" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B44" s="85"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="102"/>
+      <c r="H44" s="102"/>
+      <c r="I44" s="102"/>
+      <c r="J44" s="102"/>
+      <c r="K44" s="103"/>
+    </row>
+    <row r="45" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B45" s="91"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="113"/>
+      <c r="G45" s="105"/>
+      <c r="H45" s="105"/>
+      <c r="I45" s="105"/>
+      <c r="J45" s="105"/>
+      <c r="K45" s="106"/>
+    </row>
+    <row r="46" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F46" s="97"/>
+    </row>
+    <row r="47" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F47" s="97"/>
+    </row>
+    <row r="48" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F48" s="97"/>
+    </row>
+    <row r="49" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F49" s="97"/>
+    </row>
+    <row r="50" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F50" s="97"/>
+    </row>
+    <row r="51" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F51" s="97"/>
+    </row>
+    <row r="52" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F52" s="97"/>
+    </row>
+    <row r="53" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F53" s="97"/>
+    </row>
+    <row r="54" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F54" s="97"/>
+    </row>
+    <row r="55" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F55" s="97"/>
+    </row>
+    <row r="56" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F56" s="97"/>
+    </row>
+    <row r="57" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F57" s="97"/>
+    </row>
+    <row r="58" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F58" s="97"/>
+    </row>
+    <row r="59" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F59" s="97"/>
+    </row>
+    <row r="60" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F60" s="97"/>
+    </row>
+    <row r="61" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F61" s="97"/>
+    </row>
+    <row r="62" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F62" s="97"/>
+    </row>
+    <row r="63" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F63" s="97"/>
+    </row>
+    <row r="64" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F64" s="97"/>
+    </row>
+    <row r="65" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F65" s="97"/>
+    </row>
+    <row r="66" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F66" s="97"/>
+    </row>
+    <row r="67" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F67" s="97"/>
+    </row>
+    <row r="68" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F68" s="97"/>
+    </row>
+    <row r="69" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F69" s="97"/>
+    </row>
+    <row r="70" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F70" s="97"/>
+    </row>
+    <row r="71" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F71" s="97"/>
+    </row>
+    <row r="72" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F72" s="97"/>
+    </row>
+    <row r="73" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F73" s="97"/>
+    </row>
+    <row r="74" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F74" s="97"/>
+    </row>
+    <row r="75" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F75" s="97"/>
+    </row>
+    <row r="76" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F76" s="97"/>
+    </row>
+    <row r="77" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F77" s="97"/>
+    </row>
+    <row r="78" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F78" s="97"/>
+    </row>
+    <row r="79" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F79" s="97"/>
+    </row>
+    <row r="80" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F80" s="97"/>
+    </row>
+    <row r="81" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F81" s="97"/>
+    </row>
+    <row r="82" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F82" s="97"/>
+    </row>
+    <row r="83" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F83" s="97"/>
+    </row>
+    <row r="84" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F84" s="97"/>
+    </row>
+    <row r="85" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F85" s="97"/>
+    </row>
+    <row r="86" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F86" s="97"/>
+    </row>
+    <row r="87" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F87" s="97"/>
+    </row>
+    <row r="88" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F88" s="97"/>
+    </row>
+    <row r="89" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F89" s="97"/>
+    </row>
+    <row r="90" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F90" s="97"/>
+    </row>
+    <row r="91" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F91" s="97"/>
+    </row>
+    <row r="92" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F92" s="97"/>
+    </row>
+    <row r="93" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F93" s="97"/>
+    </row>
+    <row r="94" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F94" s="97"/>
+    </row>
+    <row r="95" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F95" s="97"/>
+    </row>
+    <row r="96" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F96" s="97"/>
+    </row>
+    <row r="97" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F97" s="97"/>
+    </row>
+    <row r="98" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F98" s="97"/>
+    </row>
+    <row r="99" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F99" s="97"/>
+    </row>
+    <row r="100" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F100" s="97"/>
+    </row>
+    <row r="101" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F101" s="97"/>
+    </row>
+    <row r="102" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F102" s="97"/>
+    </row>
+    <row r="103" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F103" s="97"/>
+    </row>
+    <row r="104" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F104" s="97"/>
+    </row>
+    <row r="105" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F105" s="97"/>
+    </row>
+    <row r="106" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F106" s="97"/>
+    </row>
+    <row r="107" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F107" s="97"/>
+    </row>
+    <row r="108" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F108" s="97"/>
+    </row>
+    <row r="109" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F109" s="97"/>
+    </row>
+    <row r="110" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F110" s="97"/>
+    </row>
+    <row r="111" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F111" s="97"/>
+    </row>
+    <row r="112" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="F112" s="97"/>
     </row>
     <row r="113" spans="6:6">
-      <c r="F113" s="101"/>
+      <c r="F113" s="97"/>
     </row>
     <row r="114" spans="6:6">
-      <c r="F114" s="101"/>
+      <c r="F114" s="97"/>
     </row>
     <row r="115" spans="6:6">
-      <c r="F115" s="101"/>
+      <c r="F115" s="97"/>
     </row>
     <row r="116" spans="6:6">
-      <c r="F116" s="101"/>
+      <c r="F116" s="97"/>
     </row>
     <row r="117" spans="6:6">
-      <c r="F117" s="101"/>
+      <c r="F117" s="97"/>
     </row>
     <row r="118" spans="6:6">
-      <c r="F118" s="101"/>
+      <c r="F118" s="97"/>
     </row>
     <row r="119" spans="6:6">
-      <c r="F119" s="101"/>
+      <c r="F119" s="97"/>
     </row>
     <row r="120" spans="6:6">
-      <c r="F120" s="101"/>
+      <c r="F120" s="97"/>
     </row>
     <row r="121" spans="6:6">
-      <c r="F121" s="101"/>
+      <c r="F121" s="97"/>
     </row>
     <row r="122" spans="6:6">
-      <c r="F122" s="101"/>
+      <c r="F122" s="97"/>
     </row>
     <row r="123" spans="6:6">
-      <c r="F123" s="101"/>
+      <c r="F123" s="97"/>
     </row>
     <row r="124" spans="6:6">
-      <c r="F124" s="101"/>
+      <c r="F124" s="97"/>
     </row>
     <row r="125" spans="6:6">
-      <c r="F125" s="101"/>
+      <c r="F125" s="97"/>
     </row>
     <row r="126" spans="6:6">
-      <c r="F126" s="101"/>
+      <c r="F126" s="97"/>
     </row>
     <row r="127" spans="6:6">
-      <c r="F127" s="101"/>
+      <c r="F127" s="97"/>
     </row>
     <row r="128" spans="6:6">
-      <c r="F128" s="101"/>
+      <c r="F128" s="97"/>
     </row>
     <row r="129" spans="6:6">
-      <c r="F129" s="101"/>
+      <c r="F129" s="97"/>
     </row>
     <row r="130" spans="6:6">
-      <c r="F130" s="101"/>
+      <c r="F130" s="97"/>
     </row>
     <row r="131" spans="6:6">
-      <c r="F131" s="101"/>
+      <c r="F131" s="97"/>
     </row>
     <row r="132" spans="6:6">
-      <c r="F132" s="101"/>
+      <c r="F132" s="97"/>
     </row>
     <row r="133" spans="6:6">
-      <c r="F133" s="101"/>
+      <c r="F133" s="97"/>
     </row>
     <row r="134" spans="6:6">
-      <c r="F134" s="101"/>
+      <c r="F134" s="97"/>
     </row>
     <row r="135" spans="6:6">
-      <c r="F135" s="101"/>
+      <c r="F135" s="97"/>
     </row>
     <row r="136" spans="6:6">
-      <c r="F136" s="101"/>
+      <c r="F136" s="97"/>
     </row>
     <row r="137" spans="6:6">
-      <c r="F137" s="101"/>
+      <c r="F137" s="97"/>
     </row>
     <row r="138" spans="6:6">
-      <c r="F138" s="101"/>
+      <c r="F138" s="97"/>
     </row>
     <row r="139" spans="6:6">
-      <c r="F139" s="101"/>
+      <c r="F139" s="97"/>
     </row>
     <row r="140" spans="6:6">
-      <c r="F140" s="101"/>
+      <c r="F140" s="97"/>
     </row>
     <row r="141" spans="6:6">
-      <c r="F141" s="101"/>
+      <c r="F141" s="97"/>
     </row>
     <row r="142" spans="6:6">
-      <c r="F142" s="101"/>
+      <c r="F142" s="97"/>
     </row>
     <row r="143" spans="6:6">
-      <c r="F143" s="101"/>
+      <c r="F143" s="97"/>
     </row>
     <row r="144" spans="6:6">
-      <c r="F144" s="101"/>
+      <c r="F144" s="97"/>
     </row>
     <row r="145" spans="6:6">
-      <c r="F145" s="101"/>
+      <c r="F145" s="97"/>
     </row>
     <row r="146" spans="6:6">
-      <c r="F146" s="101"/>
+      <c r="F146" s="97"/>
     </row>
     <row r="147" spans="6:6">
-      <c r="F147" s="101"/>
+      <c r="F147" s="97"/>
     </row>
     <row r="148" spans="6:6">
-      <c r="F148" s="101"/>
+      <c r="F148" s="97"/>
     </row>
     <row r="149" spans="6:6">
-      <c r="F149" s="101"/>
+      <c r="F149" s="97"/>
     </row>
     <row r="150" spans="6:6">
-      <c r="F150" s="101"/>
+      <c r="F150" s="97"/>
     </row>
     <row r="151" spans="6:6">
-      <c r="F151" s="101"/>
+      <c r="F151" s="97"/>
     </row>
     <row r="152" spans="6:6">
-      <c r="F152" s="101"/>
+      <c r="F152" s="97"/>
     </row>
     <row r="153" spans="6:6">
-      <c r="F153" s="101"/>
+      <c r="F153" s="97"/>
     </row>
     <row r="154" spans="6:6">
-      <c r="F154" s="101"/>
+      <c r="F154" s="97"/>
     </row>
     <row r="155" spans="6:6">
-      <c r="F155" s="101"/>
+      <c r="F155" s="97"/>
     </row>
     <row r="156" spans="6:6">
-      <c r="F156" s="101"/>
+      <c r="F156" s="97"/>
     </row>
     <row r="157" spans="6:6">
-      <c r="F157" s="101"/>
+      <c r="F157" s="97"/>
     </row>
     <row r="158" spans="6:6">
-      <c r="F158" s="101"/>
+      <c r="F158" s="97"/>
     </row>
     <row r="159" spans="6:6">
-      <c r="F159" s="101"/>
+      <c r="F159" s="97"/>
     </row>
     <row r="160" spans="6:6">
-      <c r="F160" s="101"/>
+      <c r="F160" s="97"/>
     </row>
     <row r="161" spans="6:6">
-      <c r="F161" s="101"/>
+      <c r="F161" s="97"/>
     </row>
     <row r="162" spans="6:6">
-      <c r="F162" s="101"/>
+      <c r="F162" s="97"/>
     </row>
     <row r="163" spans="6:6">
-      <c r="F163" s="101"/>
+      <c r="F163" s="97"/>
     </row>
     <row r="164" spans="6:6">
-      <c r="F164" s="101"/>
+      <c r="F164" s="97"/>
     </row>
     <row r="165" spans="6:6">
-      <c r="F165" s="101"/>
+      <c r="F165" s="97"/>
     </row>
     <row r="166" spans="6:6">
-      <c r="F166" s="101"/>
+      <c r="F166" s="97"/>
     </row>
     <row r="167" spans="6:6">
-      <c r="F167" s="101"/>
+      <c r="F167" s="97"/>
     </row>
     <row r="168" spans="6:6">
-      <c r="F168" s="101"/>
+      <c r="F168" s="97"/>
     </row>
     <row r="169" spans="6:6">
-      <c r="F169" s="101"/>
+      <c r="F169" s="97"/>
     </row>
     <row r="170" spans="6:6">
-      <c r="F170" s="101"/>
+      <c r="F170" s="97"/>
     </row>
     <row r="171" spans="6:6">
-      <c r="F171" s="101"/>
+      <c r="F171" s="97"/>
     </row>
     <row r="172" spans="6:6">
-      <c r="F172" s="101"/>
+      <c r="F172" s="97"/>
     </row>
     <row r="173" spans="6:6">
-      <c r="F173" s="101"/>
+      <c r="F173" s="97"/>
     </row>
     <row r="174" spans="6:6">
-      <c r="F174" s="101"/>
+      <c r="F174" s="97"/>
     </row>
     <row r="175" spans="6:6">
-      <c r="F175" s="101"/>
+      <c r="F175" s="97"/>
     </row>
     <row r="176" spans="6:6">
-      <c r="F176" s="101"/>
+      <c r="F176" s="97"/>
     </row>
     <row r="177" spans="6:6">
-      <c r="F177" s="101"/>
+      <c r="F177" s="97"/>
     </row>
     <row r="178" spans="6:6">
-      <c r="F178" s="101"/>
+      <c r="F178" s="97"/>
     </row>
     <row r="179" spans="6:6">
-      <c r="F179" s="101"/>
+      <c r="F179" s="97"/>
     </row>
     <row r="180" spans="6:6">
-      <c r="F180" s="101"/>
+      <c r="F180" s="97"/>
     </row>
     <row r="181" spans="6:6">
-      <c r="F181" s="101"/>
+      <c r="F181" s="97"/>
     </row>
     <row r="182" spans="6:6">
-      <c r="F182" s="101"/>
+      <c r="F182" s="97"/>
     </row>
     <row r="183" spans="6:6">
-      <c r="F183" s="101"/>
+      <c r="F183" s="97"/>
     </row>
     <row r="184" spans="6:6">
-      <c r="F184" s="101"/>
+      <c r="F184" s="97"/>
     </row>
     <row r="185" spans="6:6">
-      <c r="F185" s="101"/>
+      <c r="F185" s="97"/>
     </row>
     <row r="186" spans="6:6">
-      <c r="F186" s="101"/>
+      <c r="F186" s="97"/>
     </row>
     <row r="187" spans="6:6">
-      <c r="F187" s="101"/>
+      <c r="F187" s="97"/>
     </row>
     <row r="188" spans="6:6">
-      <c r="F188" s="101"/>
+      <c r="F188" s="97"/>
     </row>
     <row r="189" spans="6:6">
-      <c r="F189" s="101"/>
+      <c r="F189" s="97"/>
     </row>
     <row r="190" spans="6:6">
-      <c r="F190" s="101"/>
+      <c r="F190" s="97"/>
     </row>
     <row r="191" spans="6:6">
-      <c r="F191" s="101"/>
+      <c r="F191" s="97"/>
     </row>
     <row r="192" spans="6:6">
-      <c r="F192" s="101"/>
+      <c r="F192" s="97"/>
     </row>
     <row r="193" spans="6:6">
-      <c r="F193" s="101"/>
+      <c r="F193" s="97"/>
     </row>
     <row r="194" spans="6:6">
-      <c r="F194" s="101"/>
+      <c r="F194" s="97"/>
     </row>
     <row r="195" spans="6:6">
-      <c r="F195" s="101"/>
+      <c r="F195" s="97"/>
     </row>
     <row r="196" spans="6:6">
-      <c r="F196" s="101"/>
+      <c r="F196" s="97"/>
     </row>
     <row r="197" spans="6:6">
-      <c r="F197" s="101"/>
+      <c r="F197" s="97"/>
     </row>
     <row r="198" spans="6:6">
-      <c r="F198" s="101"/>
+      <c r="F198" s="97"/>
     </row>
     <row r="199" spans="6:6">
-      <c r="F199" s="101"/>
+      <c r="F199" s="97"/>
     </row>
     <row r="200" spans="6:6">
-      <c r="F200" s="101"/>
+      <c r="F200" s="97"/>
     </row>
     <row r="201" spans="6:6">
-      <c r="F201" s="101"/>
+      <c r="F201" s="97"/>
     </row>
     <row r="202" spans="6:6">
-      <c r="F202" s="101"/>
+      <c r="F202" s="97"/>
     </row>
     <row r="203" spans="6:6">
-      <c r="F203" s="101"/>
+      <c r="F203" s="97"/>
     </row>
     <row r="204" spans="6:6">
-      <c r="F204" s="101"/>
+      <c r="F204" s="97"/>
     </row>
     <row r="205" spans="6:6">
-      <c r="F205" s="101"/>
+      <c r="F205" s="97"/>
     </row>
     <row r="206" spans="6:6">
-      <c r="F206" s="101"/>
+      <c r="F206" s="97"/>
     </row>
     <row r="207" spans="6:6">
-      <c r="F207" s="101"/>
+      <c r="F207" s="97"/>
     </row>
     <row r="208" spans="6:6">
-      <c r="F208" s="101"/>
+      <c r="F208" s="97"/>
     </row>
     <row r="209" spans="6:6">
-      <c r="F209" s="101"/>
+      <c r="F209" s="97"/>
     </row>
     <row r="210" spans="6:6">
-      <c r="F210" s="101"/>
+      <c r="F210" s="97"/>
     </row>
     <row r="211" spans="6:6">
-      <c r="F211" s="101"/>
+      <c r="F211" s="97"/>
     </row>
     <row r="212" spans="6:6">
-      <c r="F212" s="101"/>
+      <c r="F212" s="97"/>
     </row>
     <row r="213" spans="6:6">
-      <c r="F213" s="101"/>
+      <c r="F213" s="97"/>
     </row>
     <row r="214" spans="6:6">
-      <c r="F214" s="101"/>
+      <c r="F214" s="97"/>
     </row>
     <row r="215" spans="6:6">
-      <c r="F215" s="101"/>
+      <c r="F215" s="97"/>
     </row>
     <row r="216" spans="6:6">
-      <c r="F216" s="101"/>
+      <c r="F216" s="97"/>
     </row>
     <row r="217" spans="6:6">
-      <c r="F217" s="101"/>
+      <c r="F217" s="97"/>
     </row>
     <row r="218" spans="6:6">
-      <c r="F218" s="101"/>
+      <c r="F218" s="97"/>
     </row>
     <row r="219" spans="6:6">
-      <c r="F219" s="101"/>
+      <c r="F219" s="97"/>
     </row>
     <row r="220" spans="6:6">
-      <c r="F220" s="101"/>
+      <c r="F220" s="97"/>
     </row>
     <row r="221" spans="6:6">
-      <c r="F221" s="101"/>
+      <c r="F221" s="97"/>
     </row>
     <row r="222" spans="6:6">
-      <c r="F222" s="101"/>
+      <c r="F222" s="97"/>
     </row>
     <row r="223" spans="6:6">
-      <c r="F223" s="101"/>
+      <c r="F223" s="97"/>
     </row>
     <row r="224" spans="6:6">
-      <c r="F224" s="101"/>
+      <c r="F224" s="97"/>
     </row>
     <row r="225" spans="6:6">
-      <c r="F225" s="101"/>
+      <c r="F225" s="97"/>
     </row>
     <row r="226" spans="6:6">
-      <c r="F226" s="101"/>
+      <c r="F226" s="97"/>
     </row>
     <row r="227" spans="6:6">
-      <c r="F227" s="101"/>
+      <c r="F227" s="97"/>
     </row>
     <row r="228" spans="6:6">
-      <c r="F228" s="101"/>
+      <c r="F228" s="97"/>
     </row>
     <row r="229" spans="6:6">
-      <c r="F229" s="101"/>
+      <c r="F229" s="97"/>
     </row>
     <row r="230" spans="6:6">
-      <c r="F230" s="101"/>
+      <c r="F230" s="97"/>
     </row>
     <row r="231" spans="6:6">
-      <c r="F231" s="101"/>
+      <c r="F231" s="97"/>
     </row>
     <row r="232" spans="6:6">
-      <c r="F232" s="101"/>
+      <c r="F232" s="97"/>
     </row>
     <row r="233" spans="6:6">
-      <c r="F233" s="101"/>
+      <c r="F233" s="97"/>
     </row>
     <row r="234" spans="6:6">
-      <c r="F234" s="101"/>
+      <c r="F234" s="97"/>
     </row>
     <row r="235" spans="6:6">
-      <c r="F235" s="101"/>
+      <c r="F235" s="97"/>
     </row>
     <row r="236" spans="6:6">
-      <c r="F236" s="101"/>
+      <c r="F236" s="97"/>
     </row>
     <row r="237" spans="6:6">
-      <c r="F237" s="101"/>
+      <c r="F237" s="97"/>
     </row>
     <row r="238" spans="6:6">
-      <c r="F238" s="101"/>
+      <c r="F238" s="97"/>
     </row>
     <row r="239" spans="6:6">
-      <c r="F239" s="101"/>
+      <c r="F239" s="97"/>
     </row>
     <row r="240" spans="6:6">
-      <c r="F240" s="101"/>
+      <c r="F240" s="97"/>
     </row>
     <row r="241" spans="6:6">
-      <c r="F241" s="101"/>
+      <c r="F241" s="97"/>
     </row>
     <row r="242" spans="6:6">
-      <c r="F242" s="101"/>
+      <c r="F242" s="97"/>
     </row>
     <row r="243" spans="6:6">
-      <c r="F243" s="101"/>
+      <c r="F243" s="97"/>
     </row>
     <row r="244" spans="6:6">
-      <c r="F244" s="101"/>
+      <c r="F244" s="97"/>
     </row>
     <row r="245" spans="6:6">
-      <c r="F245" s="101"/>
+      <c r="F245" s="97"/>
     </row>
     <row r="246" spans="6:6">
-      <c r="F246" s="101"/>
+      <c r="F246" s="97"/>
     </row>
     <row r="247" spans="6:6">
-      <c r="F247" s="101"/>
+      <c r="F247" s="97"/>
     </row>
     <row r="248" spans="6:6">
-      <c r="F248" s="101"/>
+      <c r="F248" s="97"/>
     </row>
     <row r="249" spans="6:6">
-      <c r="F249" s="101"/>
+      <c r="F249" s="97"/>
     </row>
     <row r="250" spans="6:6">
-      <c r="F250" s="101"/>
+      <c r="F250" s="97"/>
     </row>
     <row r="251" spans="6:6">
-      <c r="F251" s="101"/>
+      <c r="F251" s="97"/>
     </row>
     <row r="252" spans="6:6">
-      <c r="F252" s="101"/>
+      <c r="F252" s="97"/>
     </row>
     <row r="253" spans="6:6">
-      <c r="F253" s="101"/>
+      <c r="F253" s="97"/>
     </row>
     <row r="254" spans="6:6">
-      <c r="F254" s="101"/>
+      <c r="F254" s="97"/>
     </row>
     <row r="255" spans="6:6">
-      <c r="F255" s="101"/>
+      <c r="F255" s="97"/>
     </row>
     <row r="256" spans="6:6">
-      <c r="F256" s="101"/>
+      <c r="F256" s="97"/>
     </row>
     <row r="257" spans="6:6">
-      <c r="F257" s="101"/>
+      <c r="F257" s="97"/>
     </row>
     <row r="258" spans="6:6">
-      <c r="F258" s="101"/>
+      <c r="F258" s="97"/>
     </row>
     <row r="259" spans="6:6">
-      <c r="F259" s="101"/>
+      <c r="F259" s="97"/>
     </row>
     <row r="260" spans="6:6">
-      <c r="F260" s="101"/>
+      <c r="F260" s="97"/>
     </row>
     <row r="261" spans="6:6">
-      <c r="F261" s="101"/>
+      <c r="F261" s="97"/>
     </row>
     <row r="262" spans="6:6">
-      <c r="F262" s="101"/>
+      <c r="F262" s="97"/>
     </row>
     <row r="263" spans="6:6">
-      <c r="F263" s="101"/>
+      <c r="F263" s="97"/>
     </row>
     <row r="264" spans="6:6">
-      <c r="F264" s="101"/>
+      <c r="F264" s="97"/>
     </row>
     <row r="265" spans="6:6">
-      <c r="F265" s="101"/>
+      <c r="F265" s="97"/>
     </row>
     <row r="266" spans="6:6">
-      <c r="F266" s="101"/>
+      <c r="F266" s="97"/>
     </row>
     <row r="267" spans="6:6">
-      <c r="F267" s="101"/>
+      <c r="F267" s="97"/>
     </row>
     <row r="268" spans="6:6">
-      <c r="F268" s="101"/>
+      <c r="F268" s="97"/>
     </row>
     <row r="269" spans="6:6">
-      <c r="F269" s="101"/>
+      <c r="F269" s="97"/>
     </row>
     <row r="270" spans="6:6">
-      <c r="F270" s="101"/>
+      <c r="F270" s="97"/>
     </row>
     <row r="271" spans="6:6">
-      <c r="F271" s="101"/>
+      <c r="F271" s="97"/>
     </row>
     <row r="272" spans="6:6">
-      <c r="F272" s="101"/>
+      <c r="F272" s="97"/>
     </row>
     <row r="273" spans="6:6">
-      <c r="F273" s="101"/>
+      <c r="F273" s="97"/>
     </row>
     <row r="274" spans="6:6">
-      <c r="F274" s="101"/>
+      <c r="F274" s="97"/>
     </row>
     <row r="275" spans="6:6">
-      <c r="F275" s="101"/>
+      <c r="F275" s="97"/>
     </row>
     <row r="276" spans="6:6">
-      <c r="F276" s="101"/>
+      <c r="F276" s="97"/>
     </row>
     <row r="277" spans="6:6">
-      <c r="F277" s="101"/>
+      <c r="F277" s="97"/>
     </row>
     <row r="278" spans="6:6">
-      <c r="F278" s="101"/>
+      <c r="F278" s="97"/>
     </row>
     <row r="279" spans="6:6">
-      <c r="F279" s="101"/>
+      <c r="F279" s="97"/>
     </row>
     <row r="280" spans="6:6">
-      <c r="F280" s="101"/>
+      <c r="F280" s="97"/>
     </row>
     <row r="281" spans="6:6">
-      <c r="F281" s="101"/>
+      <c r="F281" s="97"/>
     </row>
     <row r="282" spans="6:6">
-      <c r="F282" s="101"/>
+      <c r="F282" s="97"/>
     </row>
     <row r="283" spans="6:6">
-      <c r="F283" s="101"/>
+      <c r="F283" s="97"/>
     </row>
     <row r="284" spans="6:6">
-      <c r="F284" s="101"/>
+      <c r="F284" s="97"/>
     </row>
     <row r="285" spans="6:6">
-      <c r="F285" s="101"/>
+      <c r="F285" s="97"/>
     </row>
     <row r="286" spans="6:6">
-      <c r="F286" s="101"/>
+      <c r="F286" s="97"/>
     </row>
     <row r="287" spans="6:6">
-      <c r="F287" s="101"/>
+      <c r="F287" s="97"/>
     </row>
     <row r="288" spans="6:6">
-      <c r="F288" s="101"/>
+      <c r="F288" s="97"/>
     </row>
     <row r="289" spans="6:6">
-      <c r="F289" s="101"/>
+      <c r="F289" s="97"/>
     </row>
     <row r="290" spans="6:6">
-      <c r="F290" s="101"/>
+      <c r="F290" s="97"/>
     </row>
     <row r="291" spans="6:6">
-      <c r="F291" s="101"/>
+      <c r="F291" s="97"/>
     </row>
     <row r="292" spans="6:6">
-      <c r="F292" s="101"/>
+      <c r="F292" s="97"/>
     </row>
     <row r="293" spans="6:6">
-      <c r="F293" s="101"/>
+      <c r="F293" s="97"/>
     </row>
     <row r="294" spans="6:6">
-      <c r="F294" s="101"/>
+      <c r="F294" s="97"/>
     </row>
     <row r="295" spans="6:6">
-      <c r="F295" s="101"/>
+      <c r="F295" s="97"/>
     </row>
     <row r="296" spans="6:6">
-      <c r="F296" s="101"/>
+      <c r="F296" s="97"/>
     </row>
     <row r="297" spans="6:6">
-      <c r="F297" s="101"/>
+      <c r="F297" s="97"/>
     </row>
     <row r="298" spans="6:6">
-      <c r="F298" s="101"/>
+      <c r="F298" s="97"/>
     </row>
     <row r="299" spans="6:6">
-      <c r="F299" s="101"/>
+      <c r="F299" s="97"/>
     </row>
     <row r="300" spans="6:6">
-      <c r="F300" s="101"/>
+      <c r="F300" s="97"/>
     </row>
     <row r="301" spans="6:6">
-      <c r="F301" s="101"/>
+      <c r="F301" s="97"/>
     </row>
     <row r="302" spans="6:6">
-      <c r="F302" s="101"/>
+      <c r="F302" s="97"/>
     </row>
     <row r="303" spans="6:6">
-      <c r="F303" s="101"/>
+      <c r="F303" s="97"/>
     </row>
     <row r="304" spans="6:6">
-      <c r="F304" s="101"/>
+      <c r="F304" s="97"/>
     </row>
     <row r="305" spans="6:6">
-      <c r="F305" s="101"/>
+      <c r="F305" s="97"/>
     </row>
     <row r="306" spans="6:6">
-      <c r="F306" s="101"/>
+      <c r="F306" s="97"/>
     </row>
     <row r="307" spans="6:6">
-      <c r="F307" s="101"/>
+      <c r="F307" s="97"/>
     </row>
     <row r="308" spans="6:6">
-      <c r="F308" s="101"/>
+      <c r="F308" s="97"/>
     </row>
     <row r="309" spans="6:6">
-      <c r="F309" s="101"/>
+      <c r="F309" s="97"/>
     </row>
     <row r="310" spans="6:6">
-      <c r="F310" s="101"/>
+      <c r="F310" s="97"/>
     </row>
     <row r="311" spans="6:6">
-      <c r="F311" s="101"/>
+      <c r="F311" s="97"/>
     </row>
     <row r="312" spans="6:6">
-      <c r="F312" s="101"/>
+      <c r="F312" s="97"/>
     </row>
     <row r="313" spans="6:6">
-      <c r="F313" s="101"/>
+      <c r="F313" s="97"/>
     </row>
     <row r="314" spans="6:6">
-      <c r="F314" s="101"/>
+      <c r="F314" s="97"/>
     </row>
     <row r="315" spans="6:6">
-      <c r="F315" s="101"/>
+      <c r="F315" s="97"/>
     </row>
     <row r="316" spans="6:6">
-      <c r="F316" s="101"/>
+      <c r="F316" s="97"/>
     </row>
     <row r="317" spans="6:6">
-      <c r="F317" s="101"/>
+      <c r="F317" s="97"/>
     </row>
     <row r="318" spans="6:6">
-      <c r="F318" s="101"/>
+      <c r="F318" s="97"/>
     </row>
     <row r="319" spans="6:6">
-      <c r="F319" s="101"/>
+      <c r="F319" s="97"/>
     </row>
     <row r="320" spans="6:6">
-      <c r="F320" s="101"/>
+      <c r="F320" s="97"/>
     </row>
     <row r="321" spans="6:6">
-      <c r="F321" s="101"/>
+      <c r="F321" s="97"/>
     </row>
     <row r="322" spans="6:6">
-      <c r="F322" s="101"/>
+      <c r="F322" s="97"/>
     </row>
     <row r="323" spans="6:6">
-      <c r="F323" s="101"/>
+      <c r="F323" s="97"/>
     </row>
     <row r="324" spans="6:6">
-      <c r="F324" s="101"/>
+      <c r="F324" s="97"/>
     </row>
     <row r="325" spans="6:6">
-      <c r="F325" s="101"/>
+      <c r="F325" s="97"/>
     </row>
     <row r="326" spans="6:6">
-      <c r="F326" s="101"/>
+      <c r="F326" s="97"/>
     </row>
     <row r="327" spans="6:6">
-      <c r="F327" s="101"/>
+      <c r="F327" s="97"/>
     </row>
     <row r="328" spans="6:6">
-      <c r="F328" s="101"/>
+      <c r="F328" s="97"/>
     </row>
     <row r="329" spans="6:6">
-      <c r="F329" s="101"/>
+      <c r="F329" s="97"/>
     </row>
     <row r="330" spans="6:6">
-      <c r="F330" s="101"/>
+      <c r="F330" s="97"/>
     </row>
     <row r="331" spans="6:6">
-      <c r="F331" s="101"/>
+      <c r="F331" s="97"/>
     </row>
     <row r="332" spans="6:6">
-      <c r="F332" s="101"/>
+      <c r="F332" s="97"/>
     </row>
     <row r="333" spans="6:6">
-      <c r="F333" s="101"/>
+      <c r="F333" s="97"/>
     </row>
     <row r="334" spans="6:6">
-      <c r="F334" s="101"/>
+      <c r="F334" s="97"/>
     </row>
     <row r="335" spans="6:6">
-      <c r="F335" s="101"/>
+      <c r="F335" s="97"/>
     </row>
     <row r="336" spans="6:6">
-      <c r="F336" s="101"/>
+      <c r="F336" s="97"/>
     </row>
     <row r="337" spans="6:6">
-      <c r="F337" s="101"/>
+      <c r="F337" s="97"/>
     </row>
     <row r="338" spans="6:6">
-      <c r="F338" s="101"/>
+      <c r="F338" s="97"/>
     </row>
     <row r="339" spans="6:6">
-      <c r="F339" s="101"/>
+      <c r="F339" s="97"/>
     </row>
     <row r="340" spans="6:6">
-      <c r="F340" s="101"/>
+      <c r="F340" s="97"/>
     </row>
     <row r="341" spans="6:6">
-      <c r="F341" s="101"/>
+      <c r="F341" s="97"/>
     </row>
     <row r="342" spans="6:6">
-      <c r="F342" s="101"/>
+      <c r="F342" s="97"/>
     </row>
     <row r="343" spans="6:6">
-      <c r="F343" s="101"/>
+      <c r="F343" s="97"/>
     </row>
     <row r="344" spans="6:6">
-      <c r="F344" s="101"/>
+      <c r="F344" s="97"/>
     </row>
     <row r="345" spans="6:6">
-      <c r="F345" s="101"/>
+      <c r="F345" s="97"/>
     </row>
     <row r="346" spans="6:6">
-      <c r="F346" s="101"/>
+      <c r="F346" s="97"/>
     </row>
     <row r="347" spans="6:6">
-      <c r="F347" s="101"/>
+      <c r="F347" s="97"/>
     </row>
     <row r="348" spans="6:6">
-      <c r="F348" s="101"/>
+      <c r="F348" s="97"/>
     </row>
     <row r="349" spans="6:6">
-      <c r="F349" s="101"/>
+      <c r="F349" s="97"/>
     </row>
     <row r="350" spans="6:6">
-      <c r="F350" s="101"/>
+      <c r="F350" s="97"/>
     </row>
     <row r="351" spans="6:6">
-      <c r="F351" s="101"/>
+      <c r="F351" s="97"/>
     </row>
     <row r="352" spans="6:6">
-      <c r="F352" s="101"/>
+      <c r="F352" s="97"/>
     </row>
     <row r="353" spans="6:6">
-      <c r="F353" s="101"/>
+      <c r="F353" s="97"/>
     </row>
     <row r="354" spans="6:6">
-      <c r="F354" s="101"/>
+      <c r="F354" s="97"/>
     </row>
     <row r="355" spans="6:6">
-      <c r="F355" s="101"/>
+      <c r="F355" s="97"/>
     </row>
     <row r="356" spans="6:6">
-      <c r="F356" s="101"/>
+      <c r="F356" s="97"/>
     </row>
     <row r="357" spans="6:6">
-      <c r="F357" s="101"/>
+      <c r="F357" s="97"/>
     </row>
     <row r="358" spans="6:6">
-      <c r="F358" s="101"/>
+      <c r="F358" s="97"/>
     </row>
     <row r="359" spans="6:6">
-      <c r="F359" s="101"/>
+      <c r="F359" s="97"/>
     </row>
     <row r="360" spans="6:6">
-      <c r="F360" s="101"/>
+      <c r="F360" s="97"/>
     </row>
     <row r="361" spans="6:6">
-      <c r="F361" s="101"/>
+      <c r="F361" s="97"/>
     </row>
     <row r="362" spans="6:6">
-      <c r="F362" s="101"/>
+      <c r="F362" s="97"/>
     </row>
     <row r="363" spans="6:6">
-      <c r="F363" s="101"/>
+      <c r="F363" s="97"/>
     </row>
     <row r="364" spans="6:6">
-      <c r="F364" s="101"/>
+      <c r="F364" s="97"/>
     </row>
     <row r="365" spans="6:6">
-      <c r="F365" s="101"/>
+      <c r="F365" s="97"/>
     </row>
     <row r="366" spans="6:6">
-      <c r="F366" s="101"/>
+      <c r="F366" s="97"/>
     </row>
     <row r="367" spans="6:6">
-      <c r="F367" s="101"/>
+      <c r="F367" s="97"/>
     </row>
     <row r="368" spans="6:6">
-      <c r="F368" s="101"/>
+      <c r="F368" s="97"/>
     </row>
     <row r="369" spans="6:6">
-      <c r="F369" s="101"/>
+      <c r="F369" s="97"/>
     </row>
     <row r="370" spans="6:6">
-      <c r="F370" s="101"/>
+      <c r="F370" s="97"/>
     </row>
     <row r="371" spans="6:6">
-      <c r="F371" s="101"/>
+      <c r="F371" s="97"/>
     </row>
     <row r="372" spans="6:6">
-      <c r="F372" s="101"/>
+      <c r="F372" s="97"/>
     </row>
     <row r="373" spans="6:6">
-      <c r="F373" s="101"/>
+      <c r="F373" s="97"/>
     </row>
     <row r="374" spans="6:6">
-      <c r="F374" s="101"/>
+      <c r="F374" s="97"/>
     </row>
     <row r="375" spans="6:6">
-      <c r="F375" s="101"/>
+      <c r="F375" s="97"/>
     </row>
     <row r="376" spans="6:6">
-      <c r="F376" s="101"/>
+      <c r="F376" s="97"/>
     </row>
     <row r="377" spans="6:6">
-      <c r="F377" s="101"/>
+      <c r="F377" s="97"/>
     </row>
     <row r="378" spans="6:6">
-      <c r="F378" s="101"/>
+      <c r="F378" s="97"/>
     </row>
     <row r="379" spans="6:6">
-      <c r="F379" s="101"/>
+      <c r="F379" s="97"/>
     </row>
     <row r="380" spans="6:6">
-      <c r="F380" s="101"/>
+      <c r="F380" s="97"/>
     </row>
     <row r="381" spans="6:6">
-      <c r="F381" s="101"/>
+      <c r="F381" s="97"/>
     </row>
     <row r="382" spans="6:6">
-      <c r="F382" s="101"/>
+      <c r="F382" s="97"/>
     </row>
     <row r="383" spans="6:6">
-      <c r="F383" s="101"/>
+      <c r="F383" s="97"/>
     </row>
     <row r="384" spans="6:6">
-      <c r="F384" s="101"/>
+      <c r="F384" s="97"/>
     </row>
     <row r="385" spans="6:6">
-      <c r="F385" s="101"/>
+      <c r="F385" s="97"/>
     </row>
     <row r="386" spans="6:6">
-      <c r="F386" s="101"/>
+      <c r="F386" s="97"/>
     </row>
     <row r="387" spans="6:6">
-      <c r="F387" s="101"/>
+      <c r="F387" s="97"/>
     </row>
     <row r="388" spans="6:6">
-      <c r="F388" s="101"/>
+      <c r="F388" s="97"/>
     </row>
     <row r="389" spans="6:6">
-      <c r="F389" s="101"/>
+      <c r="F389" s="97"/>
     </row>
     <row r="390" spans="6:6">
-      <c r="F390" s="101"/>
+      <c r="F390" s="97"/>
     </row>
     <row r="391" spans="6:6">
-      <c r="F391" s="101"/>
+      <c r="F391" s="97"/>
     </row>
     <row r="392" spans="6:6">
-      <c r="F392" s="101"/>
+      <c r="F392" s="97"/>
     </row>
     <row r="393" spans="6:6">
-      <c r="F393" s="101"/>
+      <c r="F393" s="97"/>
     </row>
     <row r="394" spans="6:6">
-      <c r="F394" s="101"/>
+      <c r="F394" s="97"/>
     </row>
     <row r="395" spans="6:6">
-      <c r="F395" s="101"/>
+      <c r="F395" s="97"/>
     </row>
     <row r="396" spans="6:6">
-      <c r="F396" s="101"/>
+      <c r="F396" s="97"/>
     </row>
     <row r="397" spans="6:6">
-      <c r="F397" s="101"/>
+      <c r="F397" s="97"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F8:F101">
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
-      <formula>$AB$3</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
+      <formula>$Y$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
       <formula>$AA$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
-      <formula>$Y$3</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+      <formula>$AB$3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Eenrollment restriction check
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B5836A-86FD-6645-8253-DDA884E18F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE0262D9-6617-4046-81D4-54331A8D2497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-82920" yWindow="-20700" windowWidth="34960" windowHeight="18860" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="-82920" yWindow="-20700" windowWidth="34960" windowHeight="18860" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,10 @@
   </sheets>
   <definedNames>
     <definedName name="CH00001_WindowsEnrollment">'Device ☑️'!$F$10</definedName>
+    <definedName name="CH00002_DeviceEnrollment_Android">'Device ☑️'!$F$27</definedName>
+    <definedName name="CH00003_DeviceEnrollment_Windows">'Device ☑️'!$F$28</definedName>
+    <definedName name="CH00004_DeviceEnrollment_iOS">'Device ☑️'!$F$29</definedName>
+    <definedName name="CH00005_DeviceEnrollment_macOS">'Device ☑️'!$F$30</definedName>
     <definedName name="HeaderAssessedOn">Home!$E$7</definedName>
     <definedName name="HeaderTenantId">Home!$E$5</definedName>
     <definedName name="HeaderTitle">Home!$E$3</definedName>
@@ -1145,7 +1149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="258">
   <si>
     <t>Devices</t>
   </si>
@@ -1908,13 +1912,19 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Applies to</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
     <t>📌</t>
+  </si>
+  <si>
+    <t>User scope</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Configure enrollment restrictions for macOS devices</t>
   </si>
 </sst>
 </file>
@@ -2321,7 +2331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -2600,6 +2610,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2609,7 +2639,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2915,6 +2945,12 @@
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -48726,8 +48762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
   <dimension ref="A1:AF56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="N54" sqref="N54"/>
+    <sheetView showGridLines="0" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -49182,7 +49218,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="3:11">
+    <row r="49" spans="3:12">
       <c r="C49" s="5" t="s">
         <v>33</v>
       </c>
@@ -49197,7 +49233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="3:11">
+    <row r="50" spans="3:12">
       <c r="C50" s="5" t="s">
         <v>34</v>
       </c>
@@ -49212,17 +49248,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="3:11" ht="28">
+    <row r="54" spans="3:12" ht="28">
       <c r="C54" s="118" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D54" s="119" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="55" spans="3:11">
+    <row r="55" spans="3:12">
       <c r="D55" s="120" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E55" s="122" t="s">
         <v>252</v>
@@ -49231,12 +49267,15 @@
       <c r="G55" s="122"/>
       <c r="H55" s="122"/>
       <c r="I55" s="122"/>
-      <c r="J55" s="122" t="s">
-        <v>253</v>
-      </c>
-      <c r="K55" s="122"/>
-    </row>
-    <row r="56" spans="3:11">
+      <c r="J55" s="120" t="s">
+        <v>255</v>
+      </c>
+      <c r="K55" s="120"/>
+      <c r="L55" s="120" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12">
       <c r="D56" s="121"/>
       <c r="E56" s="121"/>
       <c r="F56" s="121"/>
@@ -49247,9 +49286,8 @@
       <c r="K56" s="121"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="E55:I55"/>
-    <mergeCell ref="J55:K55"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C54" r:id="rId1" location="view/Microsoft_AAD_IAM/MdmAppsListBlade" xr:uid="{7CC02CD1-5A3A-C841-B0E4-23769402B4DC}"/>
@@ -49486,10 +49524,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
-  <dimension ref="A1:AF397"/>
+  <dimension ref="A1:AF398"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -49810,7 +49848,7 @@
       <c r="D18" s="77"/>
       <c r="E18" s="77"/>
       <c r="F18" s="95"/>
-      <c r="G18" s="77"/>
+      <c r="G18" s="86"/>
       <c r="H18" s="83"/>
       <c r="I18" s="83"/>
       <c r="J18" s="83"/>
@@ -49916,7 +49954,7 @@
       <c r="D26" s="77"/>
       <c r="E26" s="77"/>
       <c r="F26" s="94"/>
-      <c r="G26" s="77"/>
+      <c r="G26" s="86"/>
       <c r="H26" s="83"/>
       <c r="I26" s="83"/>
       <c r="J26" s="83"/>
@@ -49926,7 +49964,7 @@
       <c r="B27" s="85"/>
       <c r="F27" s="98"/>
       <c r="G27" s="99" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H27" s="99"/>
       <c r="I27" s="99"/>
@@ -49941,61 +49979,61 @@
       </c>
       <c r="H28" s="102"/>
       <c r="I28" s="102"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="103"/>
+      <c r="J28" s="123"/>
+      <c r="K28" s="124"/>
     </row>
     <row r="29" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B29" s="85"/>
-      <c r="F29" s="110"/>
-      <c r="G29" s="105" t="s">
-        <v>64</v>
-      </c>
-      <c r="H29" s="105"/>
-      <c r="I29" s="105"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="106"/>
+      <c r="F29" s="107"/>
+      <c r="G29" s="102" t="s">
+        <v>62</v>
+      </c>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="103"/>
     </row>
     <row r="30" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="85"/>
+      <c r="F30" s="110"/>
+      <c r="G30" s="105" t="s">
+        <v>257</v>
+      </c>
+      <c r="H30" s="105"/>
+      <c r="I30" s="105"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="106"/>
+    </row>
+    <row r="31" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B31" s="77" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="86"/>
-      <c r="D30" s="86"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="83"/>
-      <c r="H30" s="83"/>
-      <c r="I30" s="83"/>
-      <c r="J30" s="83"/>
-      <c r="K30" s="84"/>
-    </row>
-    <row r="31" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B31" s="85"/>
-      <c r="F31" s="111"/>
-      <c r="G31" s="99" t="s">
-        <v>66</v>
-      </c>
-      <c r="H31" s="99"/>
-      <c r="I31" s="99"/>
-      <c r="J31" s="99"/>
-      <c r="K31" s="100"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="86"/>
+      <c r="E31" s="86"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="83"/>
+      <c r="H31" s="83"/>
+      <c r="I31" s="83"/>
+      <c r="J31" s="83"/>
+      <c r="K31" s="84"/>
     </row>
     <row r="32" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B32" s="85"/>
-      <c r="F32" s="112"/>
-      <c r="G32" s="102" t="s">
-        <v>67</v>
-      </c>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="102"/>
-      <c r="K32" s="103"/>
+      <c r="F32" s="111"/>
+      <c r="G32" s="99" t="s">
+        <v>66</v>
+      </c>
+      <c r="H32" s="99"/>
+      <c r="I32" s="99"/>
+      <c r="J32" s="99"/>
+      <c r="K32" s="100"/>
     </row>
     <row r="33" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B33" s="85"/>
-      <c r="F33" s="101"/>
+      <c r="F33" s="112"/>
       <c r="G33" s="102" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H33" s="102"/>
       <c r="I33" s="102"/>
@@ -50004,70 +50042,70 @@
     </row>
     <row r="34" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B34" s="85"/>
-      <c r="F34" s="104"/>
-      <c r="G34" s="105" t="s">
+      <c r="F34" s="101"/>
+      <c r="G34" s="102" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="102"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="103"/>
+    </row>
+    <row r="35" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B35" s="85"/>
+      <c r="F35" s="104"/>
+      <c r="G35" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="106"/>
-    </row>
-    <row r="35" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B35" s="87" t="s">
+      <c r="H35" s="105"/>
+      <c r="I35" s="105"/>
+      <c r="J35" s="105"/>
+      <c r="K35" s="106"/>
+    </row>
+    <row r="36" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B36" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="96"/>
-      <c r="G35" s="89"/>
-      <c r="H35" s="89"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="90"/>
-    </row>
-    <row r="36" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B36" s="77" t="s">
+      <c r="C36" s="88"/>
+      <c r="D36" s="88"/>
+      <c r="E36" s="88"/>
+      <c r="F36" s="96"/>
+      <c r="G36" s="89"/>
+      <c r="H36" s="89"/>
+      <c r="I36" s="89"/>
+      <c r="J36" s="89"/>
+      <c r="K36" s="90"/>
+    </row>
+    <row r="37" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
+      <c r="B37" s="77" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="86"/>
-      <c r="D36" s="86"/>
-      <c r="E36" s="86"/>
-      <c r="F36" s="94"/>
-      <c r="G36" s="83"/>
-      <c r="H36" s="83"/>
-      <c r="I36" s="83"/>
-      <c r="J36" s="83"/>
-      <c r="K36" s="84"/>
-    </row>
-    <row r="37" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B37" s="85"/>
-      <c r="F37" s="98"/>
-      <c r="G37" s="99" t="s">
-        <v>74</v>
-      </c>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="100"/>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="94"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="84"/>
     </row>
     <row r="38" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B38" s="85"/>
-      <c r="F38" s="112"/>
-      <c r="G38" s="102" t="s">
-        <v>72</v>
-      </c>
-      <c r="H38" s="102"/>
-      <c r="I38" s="102"/>
-      <c r="J38" s="102"/>
-      <c r="K38" s="103"/>
+      <c r="F38" s="98"/>
+      <c r="G38" s="99" t="s">
+        <v>74</v>
+      </c>
+      <c r="H38" s="99"/>
+      <c r="I38" s="99"/>
+      <c r="J38" s="99"/>
+      <c r="K38" s="100"/>
     </row>
     <row r="39" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B39" s="85"/>
       <c r="F39" s="112"/>
       <c r="G39" s="102" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H39" s="102"/>
       <c r="I39" s="102"/>
@@ -50076,8 +50114,10 @@
     </row>
     <row r="40" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="B40" s="85"/>
-      <c r="F40" s="108"/>
-      <c r="G40" s="102"/>
+      <c r="F40" s="112"/>
+      <c r="G40" s="102" t="s">
+        <v>73</v>
+      </c>
       <c r="H40" s="102"/>
       <c r="I40" s="102"/>
       <c r="J40" s="102"/>
@@ -50120,19 +50160,25 @@
       <c r="K44" s="103"/>
     </row>
     <row r="45" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="B45" s="91"/>
-      <c r="C45" s="79"/>
-      <c r="D45" s="79"/>
-      <c r="E45" s="79"/>
-      <c r="F45" s="113"/>
-      <c r="G45" s="105"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="105"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="106"/>
+      <c r="B45" s="85"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="102"/>
+      <c r="H45" s="102"/>
+      <c r="I45" s="102"/>
+      <c r="J45" s="102"/>
+      <c r="K45" s="103"/>
     </row>
     <row r="46" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
-      <c r="F46" s="97"/>
+      <c r="B46" s="91"/>
+      <c r="C46" s="79"/>
+      <c r="D46" s="79"/>
+      <c r="E46" s="79"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="105"/>
+      <c r="J46" s="105"/>
+      <c r="K46" s="106"/>
     </row>
     <row r="47" spans="2:11" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="F47" s="97"/>
@@ -50332,7 +50378,7 @@
     <row r="112" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="F112" s="97"/>
     </row>
-    <row r="113" spans="6:6">
+    <row r="113" spans="6:6" s="72" customFormat="1" ht="26" customHeight="1">
       <c r="F113" s="97"/>
     </row>
     <row r="114" spans="6:6">
@@ -51187,8 +51233,11 @@
     <row r="397" spans="6:6">
       <c r="F397" s="97"/>
     </row>
+    <row r="398" spans="6:6">
+      <c r="F398" s="97"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F101">
+  <conditionalFormatting sqref="F8:F102">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>$Y$3</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added displaying device platform restrictions
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10604"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10607"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5D4BE8-30B0-5949-A5BE-4F7ADE583618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FC902-9A94-E04D-A831-CDC3F70DFEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38240" yWindow="-21140" windowWidth="27320" windowHeight="19980" tabRatio="710" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="5220" yWindow="-19160" windowWidth="27320" windowHeight="19980" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -34,6 +34,7 @@
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
     <definedName name="Status">'Identity ✍️'!$AD$3:$AK$3</definedName>
+    <definedName name="Table_EnrollmentDevicePlatformRestrictions">'Device ⚙️'!$D$66</definedName>
     <definedName name="Table_WindowsEnrollment">'Device ⚙️'!$D$58</definedName>
     <definedName name="WorkshopData" localSheetId="2">'Device ✍️'!$A$2:$AA$216</definedName>
     <definedName name="WorkshopData">'Identity ✍️'!$A$2:$AA$212</definedName>
@@ -1149,7 +1150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="266">
   <si>
     <t>Devices</t>
   </si>
@@ -1861,9 +1862,6 @@
     <t>Native update management</t>
   </si>
   <si>
-    <t>Zero Trust Assessment for Australian Unity</t>
-  </si>
-  <si>
     <t>Assessed on: 24 Mar 2024</t>
   </si>
   <si>
@@ -1915,9 +1913,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>📌</t>
-  </si>
-  <si>
     <t>User scope</t>
   </si>
   <si>
@@ -1928,6 +1923,33 @@
   </si>
   <si>
     <t>🚦</t>
+  </si>
+  <si>
+    <t>Zero Trust Assessment for …</t>
+  </si>
+  <si>
+    <t>Enrollment device platform restrictions</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>MDM</t>
+  </si>
+  <si>
+    <t>Min Ver</t>
+  </si>
+  <si>
+    <t>Max Ver</t>
+  </si>
+  <si>
+    <t>Personally owned</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
   </si>
 </sst>
 </file>
@@ -2649,7 +2671,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2963,6 +2985,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -4701,7 +4726,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm flipH="1">
-          <a:off x="6617691" y="7229985"/>
+          <a:off x="6617691" y="7661785"/>
           <a:ext cx="2854903" cy="333186"/>
           <a:chOff x="3355655" y="5890375"/>
           <a:chExt cx="2854902" cy="333186"/>
@@ -5338,7 +5363,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2729802" y="6059148"/>
+          <a:off x="2729802" y="6490948"/>
           <a:ext cx="881119" cy="882707"/>
           <a:chOff x="3532169" y="4490816"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -6178,7 +6203,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2729802" y="3116300"/>
+          <a:off x="2729802" y="3548100"/>
           <a:ext cx="881119" cy="881120"/>
           <a:chOff x="3532169" y="1564391"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -7655,7 +7680,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9833375" y="5324626"/>
+          <a:off x="9833375" y="5756426"/>
           <a:ext cx="881121" cy="881120"/>
           <a:chOff x="8046234" y="3992399"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -9668,7 +9693,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9833375" y="6796844"/>
+          <a:off x="9833375" y="7228644"/>
           <a:ext cx="881121" cy="879532"/>
           <a:chOff x="7017394" y="5358871"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -11543,7 +11568,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9833375" y="3852408"/>
+          <a:off x="9833375" y="4284208"/>
           <a:ext cx="881121" cy="881120"/>
           <a:chOff x="8046234" y="2294010"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -12344,7 +12369,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="9833375" y="2375427"/>
+          <a:off x="9833375" y="2807227"/>
           <a:ext cx="881121" cy="885882"/>
           <a:chOff x="7017394" y="966860"/>
           <a:chExt cx="1002445" cy="1002445"/>
@@ -13973,7 +13998,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5734780" y="4076371"/>
+          <a:off x="5734780" y="4508171"/>
           <a:ext cx="1974739" cy="1905408"/>
           <a:chOff x="6252798" y="2498464"/>
           <a:chExt cx="1980312" cy="1905677"/>
@@ -14426,7 +14451,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4005511" y="7231119"/>
+          <a:off x="4005511" y="7662919"/>
           <a:ext cx="2849610" cy="333186"/>
           <a:chOff x="3355655" y="5890375"/>
           <a:chExt cx="2854902" cy="333186"/>
@@ -40524,10 +40549,10 @@
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -40543,7 +40568,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1727200" y="12344400"/>
-          <a:ext cx="5994400" cy="609600"/>
+          <a:ext cx="6362700" cy="698500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -40605,23 +40630,24 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
+      <xdr:colOff>377100</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>262800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Graphic 19">
+        <xdr:cNvPr id="31" name="Graphic 30">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D80A7EB0-CCFB-FA16-0ED8-43FCA8EEF844}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A03F631-602F-FBC9-7350-E40DB2D397F9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -40630,10 +40656,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20">
           <a:extLst>
             <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId20"/>
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId21"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -40643,8 +40669,139 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1244600" y="12407900"/>
-          <a:ext cx="381000" cy="381000"/>
+          <a:off x="673100" y="12217400"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B27E34B-B877-804F-AEBB-8C9090EC6E63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1727200" y="14427200"/>
+          <a:ext cx="6362700" cy="711200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Device enrollment restrictions let you restrict devices from enrolling in Intune based on certain device attributes. Device platform restrictions restrict devices based on device platform, version, manufacturer, or ownership type.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:br>
+            <a:rPr lang="en-AU" sz="1200"/>
+          </a:br>
+          <a:endParaRPr lang="en-GB" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>241300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>415200</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>250100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Graphic 21">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3D6996-745B-E4BF-1726-878A4DCC4812}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId24"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="711200" y="14287500"/>
+          <a:ext cx="720000" cy="720000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -42328,7 +42485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6C57C3-010E-3649-B978-A4ACB529691A}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -42407,7 +42564,7 @@
       <c r="C3" s="68"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
@@ -42467,7 +42624,7 @@
       <c r="C5" s="68"/>
       <c r="D5" s="68"/>
       <c r="E5" s="71" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F5" s="68"/>
       <c r="G5" s="68"/>
@@ -42527,7 +42684,7 @@
       <c r="C7" s="68"/>
       <c r="D7" s="68"/>
       <c r="E7" s="71" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F7" s="68"/>
       <c r="G7" s="68"/>
@@ -42581,7 +42738,7 @@
       <c r="Z8" s="68"/>
       <c r="AA8" s="68"/>
     </row>
-    <row r="9" spans="1:27">
+    <row r="9" spans="1:27" ht="50">
       <c r="D9" s="1"/>
     </row>
   </sheetData>
@@ -42934,17 +43091,17 @@
       </c>
       <c r="J11" s="39"/>
       <c r="L11" s="47" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N11" s="47" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="P11" s="47" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q11" s="42"/>
       <c r="R11" s="47" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="S11" s="42"/>
       <c r="T11" s="42"/>
@@ -43894,11 +44051,11 @@
         <v>153</v>
       </c>
       <c r="P62" s="46" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="Q62"/>
       <c r="R62" s="51" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="V62" s="39"/>
     </row>
@@ -46238,7 +46395,7 @@
   <dimension ref="A1:AK154"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="7" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -46319,7 +46476,7 @@
       <c r="D3" s="54"/>
       <c r="E3" s="53"/>
       <c r="F3" s="55" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G3" s="56"/>
       <c r="H3" s="53"/>
@@ -47479,7 +47636,7 @@
         <v>187</v>
       </c>
       <c r="P72" s="50" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R72"/>
       <c r="V72" s="39"/>
@@ -48897,7 +49054,7 @@
       <c r="C3" s="68"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
@@ -49038,10 +49195,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
-  <dimension ref="A1:AF57"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -49091,7 +49248,7 @@
       <c r="C3" s="68"/>
       <c r="D3" s="69"/>
       <c r="E3" s="69" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
@@ -49223,12 +49380,12 @@
       <c r="AE6" s="68"/>
       <c r="AF6" s="68"/>
     </row>
-    <row r="10" spans="1:32">
+    <row r="10" spans="1:32" ht="50">
       <c r="C10" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" ht="28">
       <c r="C12" s="9" t="s">
         <v>18</v>
       </c>
@@ -49241,7 +49398,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:32">
+    <row r="15" spans="1:32" ht="17">
       <c r="C15" s="7" t="s">
         <v>3</v>
       </c>
@@ -49300,7 +49457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="3:7">
+    <row r="23" spans="3:7" ht="17">
       <c r="C23" s="7" t="s">
         <v>15</v>
       </c>
@@ -49396,12 +49553,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="3:9">
+    <row r="38" spans="3:9" ht="28">
       <c r="C38" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="3:9">
+    <row r="39" spans="3:9" ht="17">
       <c r="C39" s="7" t="s">
         <v>26</v>
       </c>
@@ -49461,12 +49618,12 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="3:9">
+    <row r="46" spans="3:9" ht="28">
       <c r="C46" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="3:9">
+    <row r="47" spans="3:9" ht="17">
       <c r="C47" s="7" t="s">
         <v>26</v>
       </c>
@@ -49526,51 +49683,97 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="3:12">
-      <c r="C54" s="114" t="s">
-        <v>254</v>
-      </c>
+    <row r="54" spans="3:12" ht="28">
+      <c r="C54"/>
       <c r="D54" s="115" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="55" spans="3:12">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" ht="28">
       <c r="C55" s="114"/>
       <c r="D55" s="115"/>
     </row>
-    <row r="56" spans="3:12">
+    <row r="56" spans="3:12" ht="28">
       <c r="C56" s="114"/>
       <c r="D56" s="115"/>
     </row>
     <row r="57" spans="3:12">
       <c r="D57" s="116" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E57" s="124" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F57" s="124"/>
       <c r="G57" s="124"/>
       <c r="H57" s="124"/>
       <c r="I57" s="124"/>
       <c r="J57" s="116" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K57" s="116"/>
       <c r="L57" s="116" t="s">
-        <v>256</v>
-      </c>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" ht="28">
+      <c r="C62"/>
+      <c r="D62" s="115" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" ht="28">
+      <c r="C63" s="114"/>
+      <c r="D63" s="115"/>
+    </row>
+    <row r="64" spans="3:12" ht="28">
+      <c r="C64" s="114"/>
+      <c r="D64" s="115"/>
+    </row>
+    <row r="65" spans="4:20" ht="51">
+      <c r="D65" s="116" t="s">
+        <v>35</v>
+      </c>
+      <c r="E65" s="116" t="s">
+        <v>259</v>
+      </c>
+      <c r="F65" s="116" t="s">
+        <v>251</v>
+      </c>
+      <c r="G65" s="116"/>
+      <c r="H65" s="116"/>
+      <c r="I65" s="116"/>
+      <c r="J65" s="116" t="s">
+        <v>260</v>
+      </c>
+      <c r="K65" s="116" t="s">
+        <v>261</v>
+      </c>
+      <c r="L65" s="116" t="s">
+        <v>262</v>
+      </c>
+      <c r="M65" s="125" t="s">
+        <v>263</v>
+      </c>
+      <c r="N65" s="116" t="s">
+        <v>264</v>
+      </c>
+      <c r="O65" s="116" t="s">
+        <v>265</v>
+      </c>
+      <c r="P65" s="116"/>
+      <c r="Q65" s="116"/>
+      <c r="R65" s="116"/>
+      <c r="S65" s="116"/>
+      <c r="T65" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E57:I57"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="C54" r:id="rId1" location="view/Microsoft_AAD_IAM/MdmAppsListBlade" xr:uid="{7CC02CD1-5A3A-C841-B0E4-23769402B4DC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -49658,7 +49861,7 @@
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
       <c r="D3" s="69" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E3" s="68"/>
       <c r="F3" s="69"/>
@@ -49802,7 +50005,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
   <dimension ref="A1:AF398"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
   <cols>
@@ -49870,7 +50075,7 @@
       <c r="E3" s="68"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H3" s="69"/>
       <c r="I3" s="68"/>
@@ -50005,11 +50210,11 @@
       <c r="C10" s="82"/>
       <c r="D10" s="82"/>
       <c r="E10" s="119" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F10" s="98"/>
       <c r="G10" s="99" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H10" s="99"/>
       <c r="I10" s="99" t="s">
@@ -50273,7 +50478,7 @@
       <c r="B30" s="85"/>
       <c r="F30" s="110"/>
       <c r="G30" s="105" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H30" s="105"/>
       <c r="I30" s="105"/>

</xml_diff>

<commit_message>
Added scope look up
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FC902-9A94-E04D-A831-CDC3F70DFEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34824D3-D09D-4B46-A3A9-83C6B139F6D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="-19160" windowWidth="27320" windowHeight="19980" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
@@ -1150,7 +1150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="267">
   <si>
     <t>Devices</t>
   </si>
@@ -1950,6 +1950,9 @@
   </si>
   <si>
     <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Blocked manuf.</t>
   </si>
 </sst>
 </file>
@@ -2985,9 +2988,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -3025,706 +3026,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3803,195 +3104,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
           <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4010,48 +3123,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
           <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4081,94 +3153,7 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
           <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFB6A7D8"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4192,40 +3177,13 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
-        <color rgb="FFFF0000"/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FFF7F3DC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
+          <bgColor rgb="FF0096FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4244,18 +3202,45 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FF74D6FE"/>
+          <bgColor rgb="FFDBD2E9"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <color theme="0"/>
+        <color rgb="FFFF0000"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FF0096FF"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4356,7 +3341,53 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor theme="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4372,10 +3403,24 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FFD6FD78"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4383,7 +3428,18 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FF74FC79"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4399,13 +3455,51 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="1"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
-          <bgColor rgb="FFDBD2E9"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4419,12 +3513,919 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="0"/>
       </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor auto="1"/>
           <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF0096FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFB6A7D8"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFDBD2E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFF7F3DC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FFD6FD78"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor rgb="FF74D6FE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -45960,29 +45961,29 @@
     <mergeCell ref="W5:Z5"/>
   </mergeCells>
   <conditionalFormatting sqref="A24:K25">
-    <cfRule type="cellIs" dxfId="144" priority="104" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="144" priority="97" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="103" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="98" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="99" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="100" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="101" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="139" priority="102" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="103" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="102" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="101" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="100" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="99" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="98" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="97" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="137" priority="104" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:O47 A67:AA73 A9:AA10 O11 Q11 A11:K12 M11:M12 S11:W12 AA11:AA12 L12 N12:R12 A13:AA13 Q14:AA14 A14:M15 O14:O15 N15 P15:Q15 S15 U15:AA15 A16:AA16 A17:K18 M17:M18 O17:O18 Q17:Q18 S17:S18 U17:AA18 L18 N18 P18 R18 T18 A19:AA19 M20 O20:Q20 R20:S21 A20:K22 U20:AA22 A23:AA23 O24:O25 S24:W25 Y24:Y25 AA24:AA25 A26:AA26 A27:W28 Y27:AA28 A29:AA29 A30:F31 H30:AA31 A32:AA32 A33:Q34 U33:AA34 A35:AA35 A36:F37 H36:AA37 A38:AA38 H39:O40 Q39:AA40 A39:F43 H41:AA43 A44:AA45 A48:AA48 A49:O50 Q49:AA50 A53:O54 Q53:AA54 A55:AA55 A56:O57 S56:AA57 A58:AA58 A59:M60 Q59:AA60 A61:AA61 A64:AA64 A65:F66 H65:M66 S65:AA66 AA74:AA115 A116:K207 S116:AA207 L124:R215">
@@ -45991,92 +45992,92 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:P63">
-    <cfRule type="cellIs" dxfId="135" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="9" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="10" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="11" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="12" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="13" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="14" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="15" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="16" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="9" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:AA10 O11 Q11 A11:K12 M11:M12 S11:W12 AA11:AA12 L12 N12:R12 A13:AA13 Q14:AA14 A14:M15 O14:O15 N15 P15:Q15 S15 U15:AA15 A16:AA16 A17:K18 M17:M18 O17:O18 Q17:Q18 S17:S18 U17:AA18 L18 N18 P18 R18 T18 A19:AA19 M20 O20:Q20 R20:S21 A20:K22 U20:AA22 A23:AA23 O24:O25 S24:W25 Y24:Y25 AA24:AA25 A26:AA26 A27:W28 Y27:AA28 A29:AA29 A30:F31 H30:AA31 A32:AA32 A33:Q34 U33:AA34 A35:AA35 A36:F37 H36:AA37 A38:AA38 H39:O40 Q39:AA40 A39:F43 H41:AA43 A44:AA45 A46:O47 A48:AA48 A49:O50 Q49:AA50 A53:O54 Q53:AA54 A55:AA55 A56:O57 S56:AA57 A58:AA58 A59:M60 Q59:AA60 A61:AA61 A64:AA64 A65:F66 H65:M66 S65:AA66 A67:AA73 AA74:AA115 A116:K207 S116:AA207 L124:R215">
-    <cfRule type="cellIs" dxfId="127" priority="127" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="121" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="121" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="126" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="122" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="125" priority="123" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="124" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="125" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="126" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="125" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="124" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="123" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="122" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="121" priority="127" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:AA52">
-    <cfRule type="cellIs" dxfId="120" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="17" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="119" priority="18" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="19" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="24" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="117" priority="20" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="21" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="115" priority="22" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="23" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="22" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="21" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="20" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="17" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="113" priority="24" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47 G69">
-    <cfRule type="cellIs" dxfId="112" priority="116" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
+    <cfRule type="cellIs" dxfId="112" priority="113" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="119" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="114" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="114" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="115" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="115" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="109" priority="116" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="108" priority="117" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
@@ -46084,120 +46085,120 @@
     <cfRule type="cellIs" dxfId="107" priority="118" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="113" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="106" priority="119" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="105" priority="95" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="105" priority="89" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="94" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="104" priority="90" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="93" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
+    <cfRule type="cellIs" dxfId="103" priority="91" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="102" priority="92" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="96" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="93" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="94" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="95" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="96" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="91" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="90" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="89" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:Q21">
-    <cfRule type="cellIs" dxfId="97" priority="112" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="97" priority="105" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="111" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="106" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="107" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="108" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="109" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="110" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="111" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="110" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="109" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="108" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="107" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="106" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="105" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="90" priority="112" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25">
-    <cfRule type="cellIs" dxfId="89" priority="79" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="89" priority="73" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="78" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="88" priority="74" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="77" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
+    <cfRule type="cellIs" dxfId="87" priority="75" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="86" priority="76" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="75" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="85" priority="77" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="74" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
+    <cfRule type="cellIs" dxfId="84" priority="78" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="73" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="83" priority="79" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="82" priority="80" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="cellIs" dxfId="81" priority="72" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="65" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="65" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="66" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="67" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="68" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="69" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="70" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="71" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="72" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P46:P47">
-    <cfRule type="cellIs" dxfId="73" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="33" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="34" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="33" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="71" priority="35" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
@@ -46219,159 +46220,159 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R46:AA47">
-    <cfRule type="cellIs" dxfId="65" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="25" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="26" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="32" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="63" priority="27" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="31" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="30" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="62" priority="28" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="61" priority="29" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="28" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
+    <cfRule type="cellIs" dxfId="60" priority="30" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="25" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="59" priority="31" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="27" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="58" priority="32" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R62:AA63">
     <cfRule type="cellIs" dxfId="57" priority="1" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="8" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="56" priority="2" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="55" priority="3" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="6" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="54" priority="4" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="53" priority="5" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
+    <cfRule type="cellIs" dxfId="52" priority="6" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="3" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="51" priority="7" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
+    <cfRule type="cellIs" dxfId="50" priority="8" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T21">
-    <cfRule type="cellIs" dxfId="49" priority="87" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="81" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="81" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="82" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="82" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="83" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="83" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="84" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="84" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="85" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="86" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="86" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="43" priority="87" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="42" priority="88" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X25">
-    <cfRule type="cellIs" dxfId="41" priority="64" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="57" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="63" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="40" priority="58" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="62" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="39" priority="59" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="60" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="37" priority="61" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="60" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
+    <cfRule type="cellIs" dxfId="36" priority="62" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="59" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="35" priority="63" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="58" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
+    <cfRule type="cellIs" dxfId="34" priority="64" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X28">
-    <cfRule type="cellIs" dxfId="33" priority="48" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="33" priority="41" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="42" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="43" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="44" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="45" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="46" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="47" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="46" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="45" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="44" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="43" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="42" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="41" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="26" priority="48" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="cellIs" dxfId="25" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="49" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="50" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="51" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="52" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="21" priority="53" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="54" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="19" priority="55" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="49" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="50" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="51" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="56" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="53" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="54" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="52" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -48905,26 +48906,26 @@
     <mergeCell ref="W5:Z5"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:AA11 A12:R12 U12:AA12 A13:AA15 A16:Q16 S16 U16:AA16 A17:AA29 A30:Q30 V30:AA30 A31:AA42 A43:Q43 S43:AA43 A44:T44 V44:AA44 A45:AA63 A64:S64 U64:AA64 A65:AA83 A84:T84 V84:AA84 A85:AA211">
-    <cfRule type="cellIs" dxfId="17" priority="15" stopIfTrue="1" operator="equal">
-      <formula>$AK$3</formula>
+    <cfRule type="cellIs" dxfId="17" priority="9" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="16" priority="10" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="13" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="15" priority="11" stopIfTrue="1" operator="equal">
+      <formula>$AG$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="12" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="11" stopIfTrue="1" operator="equal">
-      <formula>$AG$3</formula>
+    <cfRule type="cellIs" dxfId="13" priority="13" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="12" priority="14" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="9" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
+    <cfRule type="cellIs" dxfId="11" priority="15" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:AA63 A65:AA83 A84:T84 V84:AA84 A85:AA211 A9:AA11 A12:R12 U12:AA12 A13:AA15 A16:Q16 S16 U16:AA16 A17:AA29 A30:Q30 V30:AA30 A31:AA42 A43:Q43 S43:AA43 A44:T44 V44:AA44 A64:S64 U64:AA64">
@@ -48933,26 +48934,26 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50 G70 G73 L84 R84 X84 L87 N87 P87 R87 X87 G90 L90 N90 P90 R90 X90 G93 L93 N93 P93 R93 X93 G96 L96 N96 G99 G102 L105 N105 P105 R105 L108 N108">
-    <cfRule type="cellIs" dxfId="9" priority="7" stopIfTrue="1" operator="equal">
-      <formula>$AJ$3</formula>
+    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="equal">
+      <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" stopIfTrue="1" operator="equal">
-      <formula>$AI$3</formula>
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="equal">
+      <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" stopIfTrue="1" operator="equal">
-      <formula>$AH$3</formula>
+    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="equal">
+      <formula>$AF$3</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="4" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
-      <formula>$AF$3</formula>
+    <cfRule type="cellIs" dxfId="5" priority="5" stopIfTrue="1" operator="equal">
+      <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="equal">
-      <formula>$AE$3</formula>
+    <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="equal">
+      <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
-      <formula>$AD$3</formula>
+    <cfRule type="cellIs" dxfId="3" priority="7" stopIfTrue="1" operator="equal">
+      <formula>$AJ$3</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -49197,8 +49198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
   <dimension ref="A1:AF65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="P62" sqref="P62"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="Q66" sqref="Q66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -49730,42 +49731,40 @@
       <c r="C64" s="114"/>
       <c r="D64" s="115"/>
     </row>
-    <row r="65" spans="4:20" ht="51">
+    <row r="65" spans="4:20">
       <c r="D65" s="116" t="s">
         <v>35</v>
       </c>
-      <c r="E65" s="116" t="s">
+      <c r="G65" s="116" t="s">
         <v>259</v>
       </c>
-      <c r="F65" s="116" t="s">
+      <c r="H65" s="116" t="s">
         <v>251</v>
       </c>
-      <c r="G65" s="116"/>
-      <c r="H65" s="116"/>
       <c r="I65" s="116"/>
-      <c r="J65" s="116" t="s">
+      <c r="J65" s="116"/>
+      <c r="K65" s="116"/>
+      <c r="L65" s="116" t="s">
         <v>260</v>
       </c>
-      <c r="K65" s="116" t="s">
+      <c r="M65" s="116" t="s">
         <v>261</v>
       </c>
-      <c r="L65" s="116" t="s">
+      <c r="N65" s="116" t="s">
         <v>262</v>
       </c>
-      <c r="M65" s="125" t="s">
+      <c r="O65" s="125" t="s">
         <v>263</v>
       </c>
-      <c r="N65" s="116" t="s">
+      <c r="Q65" s="116" t="s">
+        <v>266</v>
+      </c>
+      <c r="S65" s="116" t="s">
         <v>264</v>
       </c>
-      <c r="O65" s="116" t="s">
+      <c r="T65" s="116" t="s">
         <v>265</v>
       </c>
-      <c r="P65" s="116"/>
-      <c r="Q65" s="116"/>
-      <c r="R65" s="116"/>
-      <c r="S65" s="116"/>
-      <c r="T65" s="116"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Added storage and jailbroken
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9DE677-20C3-654D-859E-CBE224FBD62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E374E0C8-A9CE-4349-843F-F7D2D24A890A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-23040" windowWidth="40960" windowHeight="23040" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
     <definedName name="Status">'Identity ✍️'!$AD$3:$AK$3</definedName>
-    <definedName name="Table_DeviceCompliancePolicies">'Device ⚙️'!$D$76</definedName>
+    <definedName name="Table_DeviceCompliancePolicies">'Device ⚙️'!$D$77</definedName>
     <definedName name="Table_EnrollmentDevicePlatformRestrictions">'Device ⚙️'!$D$66</definedName>
     <definedName name="Table_WindowsEnrollment">'Device ⚙️'!$D$58</definedName>
     <definedName name="WorkshopData" localSheetId="2">'Device ✍️'!$A$2:$AA$216</definedName>
@@ -1151,7 +1151,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="282">
   <si>
     <t>Devices</t>
   </si>
@@ -1968,9 +1968,6 @@
     <t>Max OS version</t>
   </si>
   <si>
-    <t>Rooted devices</t>
-  </si>
-  <si>
     <t>Included groups</t>
   </si>
   <si>
@@ -1996,6 +1993,12 @@
   </si>
   <si>
     <t># of previous pswds to prevent reuse</t>
+  </si>
+  <si>
+    <t>Require Firewall</t>
+  </si>
+  <si>
+    <t>Rooted / Jailbroken  devices</t>
   </si>
 </sst>
 </file>
@@ -40962,15 +40965,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>254000</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>292100</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -41000,7 +41003,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="723900" y="16383000"/>
+          <a:off x="685800" y="16167100"/>
           <a:ext cx="749300" cy="749300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -49395,9 +49398,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
-  <dimension ref="A1:AF76"/>
+  <dimension ref="A1:AF77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A51" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
@@ -49996,104 +49999,108 @@
       <c r="C74" s="88"/>
       <c r="D74" s="89"/>
     </row>
-    <row r="75" spans="3:30" s="96" customFormat="1" ht="119">
-      <c r="D75" s="127" t="s">
+    <row r="75" spans="3:30" ht="28">
+      <c r="C75" s="88"/>
+      <c r="D75" s="89"/>
+    </row>
+    <row r="76" spans="3:30" s="96" customFormat="1" ht="119">
+      <c r="D76" s="127" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="127"/>
-      <c r="F75" s="127"/>
-      <c r="G75" s="127" t="s">
+      <c r="E76" s="127"/>
+      <c r="F76" s="127"/>
+      <c r="G76" s="127" t="s">
         <v>26</v>
       </c>
-      <c r="H75" s="127"/>
-      <c r="I75" s="127"/>
-      <c r="J75" s="127"/>
-      <c r="K75" s="127"/>
-      <c r="L75" s="132" t="s">
+      <c r="H76" s="127"/>
+      <c r="I76" s="127"/>
+      <c r="J76" s="127"/>
+      <c r="K76" s="127"/>
+      <c r="L76" s="132" t="s">
         <v>268</v>
       </c>
-      <c r="M75" s="131" t="s">
+      <c r="M76" s="131" t="s">
         <v>269</v>
       </c>
-      <c r="N75" s="131" t="s">
+      <c r="N76" s="131" t="s">
         <v>270</v>
       </c>
-      <c r="O75" s="132" t="s">
+      <c r="O76" s="132" t="s">
+        <v>273</v>
+      </c>
+      <c r="P76" s="131" t="s">
         <v>274</v>
       </c>
-      <c r="P75" s="131" t="s">
+      <c r="Q76" s="134" t="s">
         <v>275</v>
       </c>
-      <c r="Q75" s="134" t="s">
+      <c r="R76" s="134"/>
+      <c r="S76" s="131" t="s">
         <v>276</v>
       </c>
-      <c r="R75" s="134"/>
-      <c r="S75" s="131" t="s">
+      <c r="T76" s="131" t="s">
+        <v>279</v>
+      </c>
+      <c r="U76" s="131" t="s">
         <v>277</v>
       </c>
-      <c r="T75" s="131" t="s">
+      <c r="V76" s="132" t="s">
+        <v>278</v>
+      </c>
+      <c r="W76" s="132" t="s">
+        <v>281</v>
+      </c>
+      <c r="X76" s="132" t="s">
         <v>280</v>
       </c>
-      <c r="U75" s="131" t="s">
-        <v>278</v>
-      </c>
-      <c r="V75" s="132" t="s">
-        <v>279</v>
-      </c>
-      <c r="W75" s="132" t="s">
+      <c r="Y76" s="95" t="s">
+        <v>264</v>
+      </c>
+      <c r="Z76" s="95"/>
+      <c r="AA76" s="127" t="s">
         <v>271</v>
       </c>
-      <c r="X75" s="132" t="s">
-        <v>230</v>
-      </c>
-      <c r="Y75" s="95" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z75" s="95"/>
-      <c r="AA75" s="127" t="s">
+      <c r="AB76" s="127"/>
+      <c r="AC76" s="127" t="s">
         <v>272</v>
       </c>
-      <c r="AB75" s="127"/>
-      <c r="AC75" s="127" t="s">
-        <v>273</v>
-      </c>
-      <c r="AD75" s="127"/>
-    </row>
-    <row r="76" spans="3:30">
-      <c r="L76" s="133"/>
-      <c r="M76" s="130"/>
-      <c r="N76" s="130"/>
-      <c r="O76" s="133"/>
-      <c r="P76" s="130"/>
-      <c r="Q76" s="135"/>
-      <c r="R76" s="135"/>
-      <c r="S76" s="130"/>
-      <c r="T76" s="130"/>
-      <c r="U76" s="130"/>
-      <c r="V76" s="133"/>
-      <c r="W76" s="133"/>
-      <c r="X76" s="133"/>
-      <c r="Y76" s="136"/>
-      <c r="Z76" s="136"/>
-      <c r="AA76" s="136"/>
-      <c r="AB76" s="136"/>
-      <c r="AC76" s="136"/>
-      <c r="AD76" s="136"/>
+      <c r="AD76" s="127"/>
+    </row>
+    <row r="77" spans="3:30">
+      <c r="L77" s="133"/>
+      <c r="M77" s="130"/>
+      <c r="N77" s="130"/>
+      <c r="O77" s="133"/>
+      <c r="P77" s="130"/>
+      <c r="Q77" s="135"/>
+      <c r="R77" s="135"/>
+      <c r="S77" s="130"/>
+      <c r="T77" s="130"/>
+      <c r="U77" s="130"/>
+      <c r="V77" s="133"/>
+      <c r="W77" s="133"/>
+      <c r="X77" s="133"/>
+      <c r="Y77" s="136"/>
+      <c r="Z77" s="136"/>
+      <c r="AA77" s="136"/>
+      <c r="AB77" s="136"/>
+      <c r="AC77" s="136"/>
+      <c r="AD77" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Y75:Z75"/>
     <mergeCell ref="Y76:Z76"/>
-    <mergeCell ref="AA75:AB75"/>
+    <mergeCell ref="Y77:Z77"/>
     <mergeCell ref="AA76:AB76"/>
-    <mergeCell ref="AC75:AD75"/>
+    <mergeCell ref="AA77:AB77"/>
     <mergeCell ref="AC76:AD76"/>
+    <mergeCell ref="AC77:AD77"/>
     <mergeCell ref="O65:P65"/>
     <mergeCell ref="Q65:R65"/>
-    <mergeCell ref="D75:F75"/>
-    <mergeCell ref="Q75:R75"/>
+    <mergeCell ref="D76:F76"/>
+    <mergeCell ref="Q76:R76"/>
     <mergeCell ref="E57:I57"/>
-    <mergeCell ref="G75:K75"/>
+    <mergeCell ref="G76:K76"/>
     <mergeCell ref="J57:K57"/>
     <mergeCell ref="D65:F65"/>
     <mergeCell ref="H65:K65"/>

</xml_diff>

<commit_message>
Added compliance policy check
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A63455D-7586-4D4E-9A79-0B62DCF6A8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B7C88C8-97F8-F845-99CB-8AB82A7896D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="-30780" yWindow="-18040" windowWidth="28800" windowHeight="18000" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,17 @@
   </sheets>
   <definedNames>
     <definedName name="CH00001_WindowsEnrollment">'Device ☑️'!$F$10</definedName>
-    <definedName name="CH00002_DeviceEnrollment_Android">'Device ☑️'!$F$27</definedName>
-    <definedName name="CH00003_DeviceEnrollment_Windows">'Device ☑️'!$F$28</definedName>
-    <definedName name="CH00004_DeviceEnrollment_iOS">'Device ☑️'!$F$29</definedName>
-    <definedName name="CH00005_DeviceEnrollment_macOS">'Device ☑️'!$F$30</definedName>
+    <definedName name="CH00002_DeviceEnrollment_Android">'Device ☑️'!$F$30</definedName>
+    <definedName name="CH00003_DeviceEnrollment_Windows">'Device ☑️'!$F$31</definedName>
+    <definedName name="CH00004_DeviceEnrollment_iOS">'Device ☑️'!$F$32</definedName>
+    <definedName name="CH00005_DeviceEnrollment_macOS">'Device ☑️'!$F$33</definedName>
+    <definedName name="CH00006_DeviceCompliance_Android_AOSP">'Device ☑️'!$F$20</definedName>
+    <definedName name="CH00007_DeviceCompliance_Android_DeviceAdmin">'Device ☑️'!$F$21</definedName>
+    <definedName name="CH00008_DeviceCompliance_Android_EntCorp">'Device ☑️'!$F$22</definedName>
+    <definedName name="CH00009_DeviceCompliance_Android_EntPersonal">'Device ☑️'!$F$23</definedName>
+    <definedName name="CH00009_DeviceCompliance_iOS">'Device ☑️'!$F$24</definedName>
+    <definedName name="CH00009_DeviceCompliance_macOS">'Device ☑️'!$F$25</definedName>
+    <definedName name="CH00009_DeviceCompliance_Windows">'Device ☑️'!$F$26</definedName>
     <definedName name="HeaderAssessedOn">Home!$E$7</definedName>
     <definedName name="HeaderTenantId">Home!$E$5</definedName>
     <definedName name="HeaderTitle">Home!$E$3</definedName>
@@ -1174,7 +1181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="254">
   <si>
     <t>Devices: Info</t>
   </si>
@@ -1233,22 +1240,10 @@
     <t>Device compliance policies to ensure devices meet minimum requirements</t>
   </si>
   <si>
-    <t>Configure compliance policies for Android Enterprise - Fully managed</t>
-  </si>
-  <si>
-    <t>Configure compliance policies for Android Enterprise - personally owned Work profile</t>
-  </si>
-  <si>
     <t>Configure actions for non-compliant devices</t>
   </si>
   <si>
-    <t>Compliance policies for iOS</t>
-  </si>
-  <si>
     <t>Compliance policies for macOS</t>
-  </si>
-  <si>
-    <t>Compliance policies for Windows</t>
   </si>
   <si>
     <t>Configure Enrollment restrictions</t>
@@ -2002,6 +1997,24 @@
       <t xml:space="preserve">
 Retire</t>
     </r>
+  </si>
+  <si>
+    <t>Compliance policies for iOS / iPadOS</t>
+  </si>
+  <si>
+    <t>Configure compliance policies for Android (AOSP)</t>
+  </si>
+  <si>
+    <t>Configure compliance policies for Android device administrator</t>
+  </si>
+  <si>
+    <t>Configure compliance policies for Android Enterprise (Fully managed and corporate owned work profile)</t>
+  </si>
+  <si>
+    <t>Configure compliance policies for Android Enterprise (Personally-owned work profile)</t>
+  </si>
+  <si>
+    <t>Compliance policies for Windows 10 and later</t>
   </si>
 </sst>
 </file>
@@ -42404,7 +42417,7 @@
       <c r="C3" s="58"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
@@ -42464,7 +42477,7 @@
       <c r="C5" s="58"/>
       <c r="D5" s="58"/>
       <c r="E5" s="61" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F5" s="58"/>
       <c r="G5" s="58"/>
@@ -42524,7 +42537,7 @@
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
       <c r="E7" s="61" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="58"/>
@@ -42706,7 +42719,7 @@
       <c r="D3" s="9"/>
       <c r="E3" s="8"/>
       <c r="F3" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="8"/>
@@ -42730,31 +42743,31 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="5"/>
       <c r="AC3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AH3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AE3" s="16" t="s">
+      <c r="AI3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AJ3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AG3" s="18" t="s">
+      <c r="AK3" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="AH3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI3" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:37" ht="11" customHeight="1">
@@ -42927,21 +42940,21 @@
       <c r="D11" s="28"/>
       <c r="E11" s="29"/>
       <c r="G11" s="30" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="J11" s="29"/>
       <c r="L11" s="37" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="N11" s="37" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="P11" s="37" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="Q11" s="32"/>
       <c r="R11" s="37" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="S11" s="32"/>
       <c r="T11" s="32"/>
@@ -42958,21 +42971,21 @@
       <c r="D12" s="28"/>
       <c r="E12" s="29"/>
       <c r="G12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J12" s="29"/>
       <c r="L12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="35"/>
       <c r="R12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S12" s="35"/>
       <c r="T12" s="35"/>
@@ -42998,17 +43011,17 @@
       <c r="D14" s="28"/>
       <c r="E14" s="29"/>
       <c r="G14" s="36" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="J14" s="29"/>
       <c r="L14" s="30" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N14" s="33" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="P14" s="37" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
@@ -43024,17 +43037,17 @@
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="G15" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J15" s="29"/>
       <c r="L15" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P15" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q15" s="35"/>
       <c r="R15"/>
@@ -43059,23 +43072,23 @@
       <c r="D17" s="28"/>
       <c r="E17" s="29"/>
       <c r="G17" s="30" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J17" s="29"/>
       <c r="L17" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="P17" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="R17" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="T17" s="31" t="s">
         <v>57</v>
-      </c>
-      <c r="N17" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="P17" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="R17" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="T17" s="31" t="s">
-        <v>61</v>
       </c>
       <c r="V17" s="29"/>
     </row>
@@ -43086,23 +43099,23 @@
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="G18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J18" s="29"/>
       <c r="L18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T18" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V18" s="29"/>
     </row>
@@ -43122,23 +43135,23 @@
       <c r="D20" s="28"/>
       <c r="E20" s="29"/>
       <c r="G20" s="30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="J20" s="29"/>
       <c r="L20" s="37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="N20" s="37" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="P20" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="R20" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="T20" s="37" t="s">
         <v>65</v>
-      </c>
-      <c r="R20" s="36" t="s">
-        <v>66</v>
-      </c>
-      <c r="T20" s="37" t="s">
-        <v>69</v>
       </c>
       <c r="V20" s="29"/>
     </row>
@@ -43149,23 +43162,23 @@
       <c r="D21" s="28"/>
       <c r="E21" s="29"/>
       <c r="G21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J21" s="29"/>
       <c r="L21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T21" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V21" s="29"/>
     </row>
@@ -43204,24 +43217,24 @@
       <c r="D24" s="28"/>
       <c r="E24" s="29"/>
       <c r="G24" s="40" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J24" s="29"/>
       <c r="L24" s="33" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="N24" s="37" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="P24" s="37" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="V24" s="29"/>
       <c r="X24" s="37" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="Z24" s="33" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="30" customHeight="1" thickBot="1">
@@ -43231,24 +43244,24 @@
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
       <c r="G25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J25" s="29"/>
       <c r="L25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V25" s="29"/>
       <c r="X25" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="Z25" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="30" customHeight="1" thickBot="1">
@@ -43267,28 +43280,28 @@
       <c r="D27" s="28"/>
       <c r="E27" s="29"/>
       <c r="G27" s="36" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="J27" s="29"/>
       <c r="L27" s="36" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="N27" s="40" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P27" s="36" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="Q27" s="38"/>
       <c r="R27" s="36" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="S27" s="38"/>
       <c r="T27" s="38"/>
       <c r="U27" s="38"/>
       <c r="V27" s="29"/>
       <c r="X27" s="37" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="30" customHeight="1" thickBot="1">
@@ -43298,28 +43311,28 @@
       <c r="D28" s="28"/>
       <c r="E28" s="29"/>
       <c r="G28" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J28" s="29"/>
       <c r="L28" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N28" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P28" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q28" s="35"/>
       <c r="R28" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S28" s="35"/>
       <c r="T28" s="35"/>
       <c r="U28" s="35"/>
       <c r="V28" s="29"/>
       <c r="X28" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="30" customHeight="1" thickBot="1">
@@ -43340,19 +43353,19 @@
       <c r="G30"/>
       <c r="J30" s="29"/>
       <c r="L30" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="N30" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="P30" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="R30" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="T30" s="40" t="s">
         <v>80</v>
-      </c>
-      <c r="N30" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="P30" s="40" t="s">
-        <v>82</v>
-      </c>
-      <c r="R30" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="T30" s="40" t="s">
-        <v>84</v>
       </c>
       <c r="V30" s="29"/>
     </row>
@@ -43365,19 +43378,19 @@
       <c r="G31"/>
       <c r="J31" s="29"/>
       <c r="L31" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N31" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P31" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R31" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T31" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V31" s="29"/>
     </row>
@@ -43398,13 +43411,13 @@
       <c r="E33" s="29"/>
       <c r="J33" s="29"/>
       <c r="L33" s="30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="N33" s="30" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="P33" s="40" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="R33"/>
       <c r="S33"/>
@@ -43419,13 +43432,13 @@
       <c r="E34" s="29"/>
       <c r="J34" s="29"/>
       <c r="L34" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N34" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P34" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R34"/>
       <c r="S34"/>
@@ -43450,20 +43463,20 @@
       <c r="G36"/>
       <c r="J36" s="29"/>
       <c r="L36" s="40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="N36" s="30" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="P36" s="30" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="R36" s="30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="V36" s="29"/>
       <c r="X36" s="30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -43475,20 +43488,20 @@
       <c r="G37"/>
       <c r="J37" s="29"/>
       <c r="L37" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N37" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P37" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R37" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V37" s="29"/>
       <c r="X37" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -43509,10 +43522,10 @@
       <c r="G39"/>
       <c r="J39" s="29"/>
       <c r="L39" s="36" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="N39" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="U39" s="38"/>
       <c r="V39" s="29"/>
@@ -43526,10 +43539,10 @@
       <c r="G40"/>
       <c r="J40" s="29"/>
       <c r="L40" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N40" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P40"/>
       <c r="U40" s="35"/>
@@ -43554,20 +43567,20 @@
       <c r="G42"/>
       <c r="J42" s="29"/>
       <c r="L42" s="40" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N42" s="30" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P42" s="30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R42" s="40" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="V42" s="29"/>
       <c r="X42" s="36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -43579,20 +43592,20 @@
       <c r="G43"/>
       <c r="J43" s="29"/>
       <c r="L43" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N43" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P43" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R43" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V43" s="29"/>
       <c r="X43" s="34" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="44" spans="1:24" ht="30" customHeight="1">
@@ -43620,21 +43633,21 @@
       <c r="D46" s="28"/>
       <c r="E46" s="29"/>
       <c r="G46" s="30" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J46" s="29"/>
       <c r="L46" s="30" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="N46" s="40" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="Q46"/>
       <c r="R46" s="40" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="V46" s="29"/>
     </row>
@@ -43645,21 +43658,21 @@
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="G47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J47" s="29"/>
       <c r="L47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q47"/>
       <c r="R47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V47" s="29"/>
     </row>
@@ -43684,10 +43697,10 @@
       <c r="G49"/>
       <c r="J49" s="29"/>
       <c r="L49" s="40" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="N49" s="30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="R49"/>
       <c r="V49" s="29"/>
@@ -43701,10 +43714,10 @@
       <c r="G50"/>
       <c r="J50" s="29"/>
       <c r="L50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R50"/>
       <c r="V50" s="29"/>
@@ -43734,14 +43747,14 @@
       <c r="D53" s="28"/>
       <c r="E53" s="29"/>
       <c r="G53" s="40" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J53" s="29"/>
       <c r="L53" s="40" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N53" s="36" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="P53"/>
       <c r="R53"/>
@@ -43754,14 +43767,14 @@
       <c r="D54" s="28"/>
       <c r="E54" s="29"/>
       <c r="G54" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J54" s="29"/>
       <c r="L54" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N54" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P54"/>
       <c r="R54"/>
@@ -43783,14 +43796,14 @@
       <c r="D56" s="28"/>
       <c r="E56" s="29"/>
       <c r="G56" s="40" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="J56" s="29"/>
       <c r="L56" s="36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="N56" s="30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="P56"/>
       <c r="Q56"/>
@@ -43804,14 +43817,14 @@
       <c r="D57" s="28"/>
       <c r="E57" s="29"/>
       <c r="G57" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J57" s="29"/>
       <c r="L57" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N57" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P57"/>
       <c r="Q57"/>
@@ -43834,11 +43847,11 @@
       <c r="D59" s="28"/>
       <c r="E59" s="29"/>
       <c r="G59" s="30" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="J59" s="29"/>
       <c r="L59" s="30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="N59"/>
       <c r="O59"/>
@@ -43853,11 +43866,11 @@
       <c r="D60" s="28"/>
       <c r="E60" s="29"/>
       <c r="G60" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J60" s="29"/>
       <c r="L60" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N60"/>
       <c r="O60"/>
@@ -43881,21 +43894,21 @@
       <c r="D62" s="28"/>
       <c r="E62" s="29"/>
       <c r="G62" s="36" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="J62" s="29"/>
       <c r="L62" s="41" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="N62" s="36" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="P62" s="36" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="Q62"/>
       <c r="R62" s="41" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="V62" s="29"/>
     </row>
@@ -43906,21 +43919,21 @@
       <c r="D63" s="28"/>
       <c r="E63" s="29"/>
       <c r="G63" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J63" s="29"/>
       <c r="L63" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N63" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P63" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q63"/>
       <c r="R63" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V63" s="29"/>
     </row>
@@ -43942,7 +43955,7 @@
       <c r="G65"/>
       <c r="J65" s="29"/>
       <c r="L65" s="40" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="N65"/>
       <c r="O65"/>
@@ -43960,7 +43973,7 @@
       <c r="G66"/>
       <c r="J66" s="29"/>
       <c r="L66" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N66"/>
       <c r="O66"/>
@@ -43988,17 +44001,17 @@
       <c r="E68" s="29"/>
       <c r="F68"/>
       <c r="G68" s="30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="J68" s="29"/>
       <c r="L68" s="30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="N68" s="40" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="P68" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="R68"/>
       <c r="V68" s="29"/>
@@ -44010,17 +44023,17 @@
       <c r="D69" s="28"/>
       <c r="E69" s="29"/>
       <c r="G69" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J69" s="29"/>
       <c r="L69" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N69" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P69" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R69"/>
       <c r="V69" s="29"/>
@@ -44042,13 +44055,13 @@
       <c r="E71" s="29"/>
       <c r="J71" s="29"/>
       <c r="L71" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="N71" s="40" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="P71" s="40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="R71"/>
       <c r="V71" s="29"/>
@@ -44061,13 +44074,13 @@
       <c r="E72" s="29"/>
       <c r="J72" s="29"/>
       <c r="L72" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N72" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P72" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R72"/>
       <c r="V72" s="29"/>
@@ -46316,7 +46329,7 @@
       <c r="D3" s="44"/>
       <c r="E3" s="43"/>
       <c r="F3" s="45" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G3" s="46"/>
       <c r="H3" s="43"/>
@@ -46340,31 +46353,31 @@
       <c r="Z3" s="43"/>
       <c r="AA3" s="42"/>
       <c r="AC3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AD3" s="15" t="s">
+      <c r="AH3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="AE3" s="16" t="s">
+      <c r="AI3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AF3" s="17" t="s">
+      <c r="AJ3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AG3" s="18" t="s">
+      <c r="AK3" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="AH3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI3" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="AK3" s="22" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:37" ht="11" customHeight="1">
@@ -46538,13 +46551,13 @@
       <c r="E11" s="29"/>
       <c r="J11" s="29"/>
       <c r="L11" s="52" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="N11" s="52" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="P11" s="52" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="Q11" s="32"/>
       <c r="R11" s="32"/>
@@ -46553,10 +46566,10 @@
       <c r="U11" s="32"/>
       <c r="V11" s="29"/>
       <c r="X11" s="40" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="Z11" s="52" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:37" ht="30" customHeight="1" thickBot="1">
@@ -46568,13 +46581,13 @@
       <c r="G12" s="35"/>
       <c r="J12" s="29"/>
       <c r="L12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="35"/>
       <c r="R12" s="35"/>
@@ -46583,10 +46596,10 @@
       <c r="U12" s="35"/>
       <c r="V12" s="29"/>
       <c r="X12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Z12" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:37" ht="30" customHeight="1">
@@ -46614,17 +46627,17 @@
       <c r="D15" s="28"/>
       <c r="E15" s="29"/>
       <c r="G15" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J15" s="29"/>
       <c r="L15" s="30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N15" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="P15" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
@@ -46640,17 +46653,17 @@
       <c r="D16" s="28"/>
       <c r="E16" s="29"/>
       <c r="G16" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J16" s="29"/>
       <c r="L16" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N16" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q16" s="35"/>
       <c r="R16"/>
@@ -46675,7 +46688,7 @@
       <c r="D18" s="28"/>
       <c r="E18" s="29"/>
       <c r="G18" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J18" s="29"/>
       <c r="V18" s="29"/>
@@ -46687,7 +46700,7 @@
       <c r="D19" s="28"/>
       <c r="E19" s="29"/>
       <c r="G19" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J19" s="29"/>
       <c r="V19" s="29"/>
@@ -46709,16 +46722,16 @@
       <c r="E21" s="29"/>
       <c r="J21" s="29"/>
       <c r="N21" s="40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P21" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R21" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="T21" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="V21" s="29"/>
     </row>
@@ -46730,16 +46743,16 @@
       <c r="E22" s="29"/>
       <c r="J22" s="29"/>
       <c r="N22" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R22" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T22" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V22" s="29"/>
     </row>
@@ -46759,11 +46772,11 @@
       <c r="D24" s="28"/>
       <c r="E24" s="29"/>
       <c r="G24" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J24" s="29"/>
       <c r="L24" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="V24" s="29"/>
     </row>
@@ -46774,11 +46787,11 @@
       <c r="D25" s="28"/>
       <c r="E25" s="29"/>
       <c r="G25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J25" s="29"/>
       <c r="L25" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V25" s="29"/>
     </row>
@@ -46816,17 +46829,17 @@
       <c r="D29" s="28"/>
       <c r="E29" s="29"/>
       <c r="G29" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J29" s="29"/>
       <c r="L29" s="30" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="N29" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="P29" s="30" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="Q29" s="38"/>
       <c r="R29" s="38"/>
@@ -46842,17 +46855,17 @@
       <c r="D30" s="28"/>
       <c r="E30" s="29"/>
       <c r="G30" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J30" s="29"/>
       <c r="L30" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N30" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P30" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q30" s="35"/>
       <c r="R30"/>
@@ -46877,7 +46890,7 @@
       <c r="D32" s="28"/>
       <c r="E32" s="29"/>
       <c r="G32" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J32" s="29"/>
       <c r="V32" s="29"/>
@@ -46889,7 +46902,7 @@
       <c r="D33" s="28"/>
       <c r="E33" s="29"/>
       <c r="G33" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J33" s="29"/>
       <c r="V33" s="29"/>
@@ -46911,16 +46924,16 @@
       <c r="E35" s="29"/>
       <c r="J35" s="29"/>
       <c r="N35" s="40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="P35" s="40" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="R35" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="T35" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="V35" s="29"/>
     </row>
@@ -46932,16 +46945,16 @@
       <c r="E36" s="29"/>
       <c r="J36" s="29"/>
       <c r="N36" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P36" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R36" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T36" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V36" s="29"/>
     </row>
@@ -46961,11 +46974,11 @@
       <c r="D38" s="28"/>
       <c r="E38" s="29"/>
       <c r="G38" s="40" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J38" s="29"/>
       <c r="L38" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="V38" s="29"/>
     </row>
@@ -46976,11 +46989,11 @@
       <c r="D39" s="28"/>
       <c r="E39" s="29"/>
       <c r="G39" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J39" s="29"/>
       <c r="L39" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V39" s="29"/>
     </row>
@@ -47018,14 +47031,14 @@
       <c r="D43" s="28"/>
       <c r="E43" s="29"/>
       <c r="G43" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J43" s="29"/>
       <c r="N43" s="30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P43" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U43" s="38"/>
       <c r="V43" s="29"/>
@@ -47037,14 +47050,14 @@
       <c r="D44" s="28"/>
       <c r="E44" s="29"/>
       <c r="G44" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J44" s="29"/>
       <c r="N44" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P44" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="U44"/>
       <c r="V44" s="29"/>
@@ -47065,17 +47078,17 @@
       <c r="D46" s="28"/>
       <c r="E46" s="29"/>
       <c r="G46" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J46" s="29"/>
       <c r="N46" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P46" s="30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R46" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V46" s="29"/>
     </row>
@@ -47086,17 +47099,17 @@
       <c r="D47" s="28"/>
       <c r="E47" s="29"/>
       <c r="G47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J47" s="29"/>
       <c r="N47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R47" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V47" s="29"/>
     </row>
@@ -47116,17 +47129,17 @@
       <c r="D49" s="28"/>
       <c r="E49" s="29"/>
       <c r="G49" s="40" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J49" s="29"/>
       <c r="N49" s="30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="P49" s="30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="R49" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V49" s="29"/>
     </row>
@@ -47137,17 +47150,17 @@
       <c r="D50" s="28"/>
       <c r="E50" s="29"/>
       <c r="G50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J50" s="29"/>
       <c r="N50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R50" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V50" s="29"/>
     </row>
@@ -47172,10 +47185,10 @@
       <c r="G52"/>
       <c r="J52" s="29"/>
       <c r="N52" s="30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P52" s="30" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="R52"/>
       <c r="V52" s="29"/>
@@ -47189,10 +47202,10 @@
       <c r="G53"/>
       <c r="J53" s="29"/>
       <c r="N53" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P53" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R53"/>
       <c r="V53" s="29"/>
@@ -47214,10 +47227,10 @@
       <c r="E55" s="29"/>
       <c r="J55" s="29"/>
       <c r="N55" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P55" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="R55"/>
       <c r="V55" s="29"/>
@@ -47230,10 +47243,10 @@
       <c r="E56" s="29"/>
       <c r="J56" s="29"/>
       <c r="N56" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P56" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R56"/>
       <c r="V56" s="29"/>
@@ -47255,13 +47268,13 @@
       <c r="E58" s="29"/>
       <c r="J58" s="29"/>
       <c r="N58" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P58" s="30" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="R58" s="40" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="V58" s="29"/>
     </row>
@@ -47273,13 +47286,13 @@
       <c r="E59" s="29"/>
       <c r="J59" s="29"/>
       <c r="N59" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P59" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R59" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V59" s="29"/>
     </row>
@@ -47317,14 +47330,14 @@
       <c r="D63" s="28"/>
       <c r="E63" s="29"/>
       <c r="G63" s="40" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J63" s="29"/>
       <c r="N63" s="30" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="P63" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="U63" s="38"/>
       <c r="V63" s="29"/>
@@ -47336,14 +47349,14 @@
       <c r="D64" s="28"/>
       <c r="E64" s="29"/>
       <c r="G64" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J64" s="29"/>
       <c r="N64" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P64" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="U64" s="35"/>
       <c r="V64" s="29"/>
@@ -47364,17 +47377,17 @@
       <c r="D66" s="28"/>
       <c r="E66" s="29"/>
       <c r="G66" s="41" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="J66" s="29"/>
       <c r="N66" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="P66" s="30" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="R66" s="30" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="V66" s="29"/>
     </row>
@@ -47385,17 +47398,17 @@
       <c r="D67" s="28"/>
       <c r="E67" s="29"/>
       <c r="G67" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J67" s="29"/>
       <c r="N67" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P67" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R67" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V67" s="29"/>
     </row>
@@ -47415,17 +47428,17 @@
       <c r="D69" s="28"/>
       <c r="E69" s="29"/>
       <c r="G69" s="30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J69" s="29"/>
       <c r="N69" s="30" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="P69" s="30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="R69" s="30" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="V69" s="29"/>
     </row>
@@ -47436,17 +47449,17 @@
       <c r="D70" s="28"/>
       <c r="E70" s="29"/>
       <c r="G70" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J70" s="29"/>
       <c r="N70" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P70" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R70" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V70" s="29"/>
     </row>
@@ -47469,14 +47482,14 @@
       <c r="E72" s="29"/>
       <c r="F72"/>
       <c r="G72" s="30" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="J72" s="29"/>
       <c r="N72" s="30" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="P72" s="40" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="R72"/>
       <c r="V72" s="29"/>
@@ -47488,14 +47501,14 @@
       <c r="D73" s="28"/>
       <c r="E73" s="29"/>
       <c r="G73" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J73" s="29"/>
       <c r="N73" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P73" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R73"/>
       <c r="V73" s="29"/>
@@ -47517,10 +47530,10 @@
       <c r="E75" s="29"/>
       <c r="J75" s="29"/>
       <c r="N75" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="P75" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="R75"/>
       <c r="V75" s="29"/>
@@ -47533,10 +47546,10 @@
       <c r="E76" s="29"/>
       <c r="J76" s="29"/>
       <c r="N76" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P76" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R76"/>
       <c r="V76" s="29"/>
@@ -47558,13 +47571,13 @@
       <c r="E78" s="29"/>
       <c r="J78" s="29"/>
       <c r="N78" s="30" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="P78" s="41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="R78" s="40" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="V78" s="29"/>
     </row>
@@ -47576,13 +47589,13 @@
       <c r="E79" s="29"/>
       <c r="J79" s="29"/>
       <c r="N79" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P79" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R79" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V79" s="29"/>
     </row>
@@ -47616,25 +47629,25 @@
       <c r="D83" s="28"/>
       <c r="E83" s="29"/>
       <c r="G83" s="30" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="J83" s="29"/>
       <c r="L83" s="30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="N83" s="30" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="P83" s="30" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="R83" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="U83" s="38"/>
       <c r="V83" s="29"/>
       <c r="X83" s="30" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="84" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47644,25 +47657,25 @@
       <c r="D84" s="28"/>
       <c r="E84" s="29"/>
       <c r="G84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J84" s="29"/>
       <c r="L84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="U84"/>
       <c r="V84" s="29"/>
       <c r="X84" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="85" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47681,24 +47694,24 @@
       <c r="D86" s="28"/>
       <c r="E86" s="29"/>
       <c r="G86" s="30" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="J86" s="29"/>
       <c r="L86" s="30" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="N86" s="40" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="P86" s="30" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="R86" s="30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="V86" s="29"/>
       <c r="X86" s="30" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47708,24 +47721,24 @@
       <c r="D87" s="28"/>
       <c r="E87" s="29"/>
       <c r="G87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J87" s="29"/>
       <c r="L87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V87" s="29"/>
       <c r="X87" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47744,24 +47757,24 @@
       <c r="D89" s="28"/>
       <c r="E89" s="29"/>
       <c r="G89" s="30" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="J89" s="29"/>
       <c r="L89" s="30" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="N89" s="40" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="P89" s="30" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="R89" s="30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="V89" s="29"/>
       <c r="X89" s="30" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="90" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47771,24 +47784,24 @@
       <c r="D90" s="28"/>
       <c r="E90" s="29"/>
       <c r="G90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J90" s="29"/>
       <c r="L90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V90" s="29"/>
       <c r="X90" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="91" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47810,24 +47823,24 @@
       <c r="E92" s="29"/>
       <c r="F92"/>
       <c r="G92" s="41" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="J92" s="29"/>
       <c r="L92" s="40" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="N92" s="30" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="P92" s="30" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="R92" s="30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="V92" s="29"/>
       <c r="X92" s="30" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="93" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47837,24 +47850,24 @@
       <c r="D93" s="28"/>
       <c r="E93" s="29"/>
       <c r="G93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J93" s="29"/>
       <c r="L93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V93" s="29"/>
       <c r="X93" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="94" spans="1:24" ht="30" customHeight="1" thickBot="1">
@@ -47873,14 +47886,14 @@
       <c r="D95" s="28"/>
       <c r="E95" s="29"/>
       <c r="G95" s="40" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="J95" s="29"/>
       <c r="L95" s="30" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="N95" s="30" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="P95"/>
       <c r="Q95"/>
@@ -47894,14 +47907,14 @@
       <c r="D96" s="28"/>
       <c r="E96" s="29"/>
       <c r="G96" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J96" s="29"/>
       <c r="L96" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N96" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P96"/>
       <c r="Q96"/>
@@ -47927,7 +47940,7 @@
       <c r="D98" s="28"/>
       <c r="E98" s="29"/>
       <c r="G98" s="30" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="J98" s="29"/>
       <c r="L98"/>
@@ -47946,7 +47959,7 @@
       <c r="D99" s="28"/>
       <c r="E99" s="29"/>
       <c r="G99" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J99" s="29"/>
       <c r="L99"/>
@@ -47971,7 +47984,7 @@
       <c r="E101" s="29"/>
       <c r="F101" s="53"/>
       <c r="G101" s="30" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J101" s="29"/>
       <c r="V101" s="29"/>
@@ -47979,7 +47992,7 @@
     <row r="102" spans="1:24" ht="30" customHeight="1" thickTop="1" thickBot="1">
       <c r="E102" s="29"/>
       <c r="G102" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J102" s="29"/>
       <c r="V102" s="29"/>
@@ -47995,16 +48008,16 @@
       <c r="G104" s="54"/>
       <c r="J104" s="29"/>
       <c r="L104" s="30" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="N104" s="40" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="P104" s="30" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="R104" s="30" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="V104" s="29"/>
     </row>
@@ -48012,16 +48025,16 @@
       <c r="E105" s="29"/>
       <c r="J105" s="29"/>
       <c r="L105" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N105" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P105" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R105" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V105" s="29"/>
     </row>
@@ -48034,10 +48047,10 @@
       <c r="E107" s="29"/>
       <c r="J107" s="29"/>
       <c r="L107" s="30" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="N107" s="30" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="V107" s="29"/>
     </row>
@@ -48045,10 +48058,10 @@
       <c r="E108" s="29"/>
       <c r="J108" s="29"/>
       <c r="L108" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N108" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V108" s="29"/>
     </row>
@@ -48078,30 +48091,30 @@
       <c r="D112" s="28"/>
       <c r="E112" s="29"/>
       <c r="G112" s="30" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J112" s="29"/>
       <c r="L112" s="30" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="N112" s="40" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="P112" s="30" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="Q112" s="38"/>
       <c r="R112" s="30" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="S112" s="38"/>
       <c r="T112" s="30" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="U112" s="38"/>
       <c r="V112" s="29"/>
       <c r="X112" s="30" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:29" ht="30" customHeight="1" thickBot="1">
@@ -48111,30 +48124,30 @@
       <c r="D113" s="28"/>
       <c r="E113" s="29"/>
       <c r="G113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J113" s="29"/>
       <c r="L113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="Q113" s="35"/>
       <c r="R113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="S113" s="35"/>
       <c r="T113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="U113" s="35"/>
       <c r="V113" s="29"/>
       <c r="X113" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="114" spans="1:29" ht="30" customHeight="1" thickBot="1">
@@ -48153,27 +48166,27 @@
       <c r="D115" s="28"/>
       <c r="E115" s="29"/>
       <c r="G115" s="40" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J115" s="29"/>
       <c r="L115" s="30" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="N115" s="30" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="P115" s="30" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="R115" s="30" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="T115" s="30" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="V115" s="29"/>
       <c r="X115" s="30" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="116" spans="1:29" ht="30" customHeight="1" thickBot="1">
@@ -48183,27 +48196,27 @@
       <c r="D116" s="28"/>
       <c r="E116" s="29"/>
       <c r="G116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="J116" s="29"/>
       <c r="L116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="P116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="R116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="T116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="V116" s="29"/>
       <c r="X116" s="34" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="117" spans="1:29" ht="30" customHeight="1">
@@ -48894,7 +48907,7 @@
       <c r="C3" s="58"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
@@ -49037,7 +49050,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
   <dimension ref="A1:AO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -49088,7 +49101,7 @@
       <c r="C3" s="58"/>
       <c r="D3" s="59"/>
       <c r="E3" s="59" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F3" s="58"/>
       <c r="G3" s="58"/>
@@ -49228,7 +49241,7 @@
     <row r="14" spans="1:32" ht="28">
       <c r="C14"/>
       <c r="D14" s="79" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="15" spans="1:32" ht="28">
@@ -49241,21 +49254,21 @@
     </row>
     <row r="17" spans="3:21">
       <c r="D17" s="139" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="E17" s="138" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F17" s="138"/>
       <c r="G17" s="138"/>
       <c r="H17" s="138"/>
       <c r="I17" s="138"/>
       <c r="J17" s="138" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="K17" s="138"/>
       <c r="L17" s="139" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="M17" s="140"/>
     </row>
@@ -49274,7 +49287,7 @@
     <row r="22" spans="3:21" ht="28">
       <c r="C22"/>
       <c r="D22" s="79" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="23" spans="3:21" ht="28">
@@ -49292,36 +49305,36 @@
       <c r="E25" s="138"/>
       <c r="F25" s="138"/>
       <c r="G25" s="139" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="H25" s="138" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I25" s="138"/>
       <c r="J25" s="138"/>
       <c r="K25" s="138"/>
       <c r="L25" s="139" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="M25" s="139" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="N25" s="139" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="O25" s="138" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="P25" s="138"/>
       <c r="Q25" s="138" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="R25" s="138"/>
       <c r="S25" s="139" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="T25" s="139" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="U25" s="140"/>
     </row>
@@ -49349,7 +49362,7 @@
     <row r="30" spans="3:21" ht="28">
       <c r="C30"/>
       <c r="D30" s="79" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="3:21" ht="16" customHeight="1">
@@ -49378,75 +49391,75 @@
       <c r="J34" s="124"/>
       <c r="K34" s="124"/>
       <c r="L34" s="111" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="M34" s="112" t="s">
+        <v>230</v>
+      </c>
+      <c r="N34" s="112" t="s">
+        <v>231</v>
+      </c>
+      <c r="O34" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="N34" s="112" t="s">
+      <c r="P34" s="112" t="s">
         <v>235</v>
       </c>
-      <c r="O34" s="113" t="s">
-        <v>238</v>
-      </c>
-      <c r="P34" s="112" t="s">
-        <v>239</v>
-      </c>
       <c r="Q34" s="126" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="R34" s="126"/>
       <c r="S34" s="112" t="s">
+        <v>236</v>
+      </c>
+      <c r="T34" s="112" t="s">
+        <v>242</v>
+      </c>
+      <c r="U34" s="112" t="s">
+        <v>241</v>
+      </c>
+      <c r="V34" s="114" t="s">
+        <v>237</v>
+      </c>
+      <c r="W34" s="114" t="s">
+        <v>239</v>
+      </c>
+      <c r="X34" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="T34" s="112" t="s">
-        <v>246</v>
-      </c>
-      <c r="U34" s="112" t="s">
-        <v>245</v>
-      </c>
-      <c r="V34" s="114" t="s">
-        <v>241</v>
-      </c>
-      <c r="W34" s="114" t="s">
+      <c r="Y34" s="114" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z34" s="135" t="s">
         <v>243</v>
-      </c>
-      <c r="X34" s="114" t="s">
-        <v>244</v>
-      </c>
-      <c r="Y34" s="114" t="s">
-        <v>242</v>
-      </c>
-      <c r="Z34" s="135" t="s">
-        <v>247</v>
       </c>
       <c r="AA34" s="135"/>
       <c r="AB34" s="135" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="AC34" s="135"/>
       <c r="AD34" s="135" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="AE34" s="135"/>
       <c r="AF34" s="135" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="AG34" s="135"/>
       <c r="AH34" s="135" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="AI34" s="135"/>
       <c r="AJ34" s="134" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AK34" s="134"/>
       <c r="AL34" s="133" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="AM34" s="133"/>
       <c r="AN34" s="133" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AO34" s="133"/>
     </row>
@@ -49619,7 +49632,7 @@
       <c r="B3" s="58"/>
       <c r="C3" s="58"/>
       <c r="D3" s="59" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E3" s="58"/>
       <c r="F3" s="59"/>
@@ -49761,10 +49774,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
-  <dimension ref="A1:AF398"/>
+  <dimension ref="A1:AF401"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
@@ -49833,7 +49846,7 @@
       <c r="E3" s="58"/>
       <c r="F3" s="59"/>
       <c r="G3" s="59" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="H3" s="59"/>
       <c r="I3" s="58"/>
@@ -49850,31 +49863,31 @@
       <c r="T3" s="58"/>
       <c r="U3" s="58"/>
       <c r="X3" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="AC3" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AD3" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AE3" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AF3" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="AC3" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE3" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF3" s="22" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:32">
@@ -49968,15 +49981,15 @@
       <c r="C10" s="87"/>
       <c r="D10" s="87"/>
       <c r="E10" s="88" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F10" s="70"/>
       <c r="G10" s="89" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H10" s="89"/>
       <c r="I10" s="89" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J10" s="89"/>
       <c r="K10" s="90"/>
@@ -49992,7 +50005,7 @@
       </c>
       <c r="H11" s="91"/>
       <c r="I11" s="91" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J11" s="91"/>
       <c r="K11" s="92"/>
@@ -50008,7 +50021,7 @@
       </c>
       <c r="H12" s="93"/>
       <c r="I12" s="93" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J12" s="93"/>
       <c r="K12" s="94"/>
@@ -50038,7 +50051,7 @@
       </c>
       <c r="H14" s="89"/>
       <c r="I14" s="89" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J14" s="89"/>
       <c r="K14" s="90"/>
@@ -50054,7 +50067,7 @@
       </c>
       <c r="H15" s="91"/>
       <c r="I15" s="91" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J15" s="91"/>
       <c r="K15" s="92"/>
@@ -50070,7 +50083,7 @@
       </c>
       <c r="H16" s="91"/>
       <c r="I16" s="91" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J16" s="91"/>
       <c r="K16" s="92"/>
@@ -50086,7 +50099,7 @@
       </c>
       <c r="H17" s="93"/>
       <c r="I17" s="93" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="J17" s="93"/>
       <c r="K17" s="94"/>
@@ -50126,11 +50139,11 @@
       <c r="E20" s="99"/>
       <c r="F20" s="70"/>
       <c r="G20" s="89" t="s">
-        <v>22</v>
+        <v>249</v>
       </c>
       <c r="H20" s="89"/>
       <c r="I20" s="89" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J20" s="89"/>
       <c r="K20" s="90"/>
@@ -50142,11 +50155,11 @@
       <c r="E21" s="99"/>
       <c r="F21" s="73"/>
       <c r="G21" s="91" t="s">
-        <v>23</v>
+        <v>250</v>
       </c>
       <c r="H21" s="91"/>
       <c r="I21" s="91" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J21" s="91"/>
       <c r="K21" s="92"/>
@@ -50158,11 +50171,11 @@
       <c r="E22" s="99"/>
       <c r="F22" s="73"/>
       <c r="G22" s="91" t="s">
-        <v>24</v>
+        <v>251</v>
       </c>
       <c r="H22" s="91"/>
       <c r="I22" s="91" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="J22" s="91"/>
       <c r="K22" s="92"/>
@@ -50174,11 +50187,11 @@
       <c r="E23" s="99"/>
       <c r="F23" s="101"/>
       <c r="G23" s="91" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="H23" s="91"/>
       <c r="I23" s="91" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J23" s="91"/>
       <c r="K23" s="92"/>
@@ -50188,13 +50201,13 @@
       <c r="C24" s="99"/>
       <c r="D24" s="99"/>
       <c r="E24" s="99"/>
-      <c r="F24" s="73"/>
+      <c r="F24" s="101"/>
       <c r="G24" s="91" t="s">
-        <v>20</v>
+        <v>248</v>
       </c>
       <c r="H24" s="91"/>
       <c r="I24" s="91" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J24" s="91"/>
       <c r="K24" s="92"/>
@@ -50204,246 +50217,252 @@
       <c r="C25" s="99"/>
       <c r="D25" s="99"/>
       <c r="E25" s="99"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="93" t="s">
-        <v>21</v>
-      </c>
-      <c r="H25" s="93"/>
-      <c r="I25" s="93" t="s">
-        <v>40</v>
-      </c>
-      <c r="J25" s="93"/>
-      <c r="K25" s="94"/>
+      <c r="F25" s="101"/>
+      <c r="G25" s="91" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="91"/>
+      <c r="I25" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="J25" s="91"/>
+      <c r="K25" s="92"/>
     </row>
     <row r="26" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B26" s="81" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="81"/>
-      <c r="D26" s="81"/>
-      <c r="E26" s="81"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="96"/>
-      <c r="I26" s="96"/>
-      <c r="J26" s="96"/>
-      <c r="K26" s="97"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="99"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="101"/>
+      <c r="G26" s="91" t="s">
+        <v>253</v>
+      </c>
+      <c r="H26" s="91"/>
+      <c r="I26" s="91" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="91"/>
+      <c r="K26" s="92"/>
     </row>
     <row r="27" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B27" s="98"/>
       <c r="C27" s="99"/>
       <c r="D27" s="99"/>
       <c r="E27" s="99"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="89" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="89"/>
-      <c r="I27" s="89"/>
-      <c r="J27" s="89"/>
-      <c r="K27" s="90"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="92"/>
     </row>
     <row r="28" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B28" s="98"/>
       <c r="C28" s="99"/>
       <c r="D28" s="99"/>
       <c r="E28" s="99"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="91" t="s">
-        <v>27</v>
-      </c>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="102"/>
-      <c r="K28" s="103"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="93" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="93"/>
+      <c r="I28" s="93" t="s">
+        <v>36</v>
+      </c>
+      <c r="J28" s="93"/>
+      <c r="K28" s="94"/>
     </row>
     <row r="29" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B29" s="98"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="99"/>
-      <c r="E29" s="99"/>
-      <c r="F29" s="73"/>
-      <c r="G29" s="91" t="s">
-        <v>26</v>
-      </c>
-      <c r="H29" s="91"/>
-      <c r="I29" s="91"/>
-      <c r="J29" s="91"/>
-      <c r="K29" s="92"/>
+      <c r="B29" s="81" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="81"/>
+      <c r="D29" s="81"/>
+      <c r="E29" s="81"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="100"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="97"/>
     </row>
     <row r="30" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B30" s="98"/>
       <c r="C30" s="99"/>
       <c r="D30" s="99"/>
       <c r="E30" s="99"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="93" t="s">
-        <v>219</v>
-      </c>
-      <c r="H30" s="93"/>
-      <c r="I30" s="93"/>
-      <c r="J30" s="93"/>
-      <c r="K30" s="94"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="89" t="s">
+        <v>24</v>
+      </c>
+      <c r="H30" s="89"/>
+      <c r="I30" s="89"/>
+      <c r="J30" s="89"/>
+      <c r="K30" s="90"/>
     </row>
     <row r="31" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B31" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="100"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="100"/>
-      <c r="F31" s="95"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="96"/>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="97"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="99"/>
+      <c r="E31" s="99"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="91" t="s">
+        <v>23</v>
+      </c>
+      <c r="H31" s="91"/>
+      <c r="I31" s="91"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="103"/>
     </row>
     <row r="32" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B32" s="98"/>
       <c r="C32" s="99"/>
       <c r="D32" s="99"/>
       <c r="E32" s="99"/>
-      <c r="F32" s="76"/>
-      <c r="G32" s="89" t="s">
-        <v>30</v>
-      </c>
-      <c r="H32" s="89"/>
-      <c r="I32" s="89"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="90"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="91" t="s">
+        <v>22</v>
+      </c>
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="91"/>
+      <c r="K32" s="92"/>
     </row>
     <row r="33" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B33" s="98"/>
       <c r="C33" s="99"/>
       <c r="D33" s="99"/>
       <c r="E33" s="99"/>
-      <c r="F33" s="77"/>
-      <c r="G33" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="92"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="93" t="s">
+        <v>215</v>
+      </c>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="94"/>
     </row>
     <row r="34" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B34" s="98"/>
-      <c r="C34" s="99"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="99"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="91" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="92"/>
+      <c r="B34" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" s="100"/>
+      <c r="D34" s="100"/>
+      <c r="E34" s="100"/>
+      <c r="F34" s="95"/>
+      <c r="G34" s="96"/>
+      <c r="H34" s="96"/>
+      <c r="I34" s="96"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="97"/>
     </row>
     <row r="35" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B35" s="98"/>
       <c r="C35" s="99"/>
       <c r="D35" s="99"/>
       <c r="E35" s="99"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="93" t="s">
-        <v>33</v>
-      </c>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="94"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="89" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="89"/>
+      <c r="I35" s="89"/>
+      <c r="J35" s="89"/>
+      <c r="K35" s="90"/>
     </row>
     <row r="36" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B36" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="105"/>
-      <c r="D36" s="105"/>
-      <c r="E36" s="105"/>
-      <c r="F36" s="106"/>
-      <c r="G36" s="107"/>
-      <c r="H36" s="107"/>
-      <c r="I36" s="107"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="108"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="99"/>
+      <c r="D36" s="99"/>
+      <c r="E36" s="99"/>
+      <c r="F36" s="77"/>
+      <c r="G36" s="91" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="91"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="91"/>
+      <c r="K36" s="92"/>
     </row>
     <row r="37" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B37" s="81" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" s="100"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="100"/>
-      <c r="F37" s="95"/>
-      <c r="G37" s="96"/>
-      <c r="H37" s="96"/>
-      <c r="I37" s="96"/>
-      <c r="J37" s="96"/>
-      <c r="K37" s="97"/>
+      <c r="B37" s="98"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="99"/>
+      <c r="E37" s="99"/>
+      <c r="F37" s="71"/>
+      <c r="G37" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="91"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="91"/>
+      <c r="K37" s="92"/>
     </row>
     <row r="38" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B38" s="98"/>
       <c r="C38" s="99"/>
       <c r="D38" s="99"/>
       <c r="E38" s="99"/>
-      <c r="F38" s="70"/>
-      <c r="G38" s="89" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" s="89"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="90"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="93" t="s">
+        <v>29</v>
+      </c>
+      <c r="H38" s="93"/>
+      <c r="I38" s="93"/>
+      <c r="J38" s="93"/>
+      <c r="K38" s="94"/>
     </row>
     <row r="39" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B39" s="98"/>
-      <c r="C39" s="99"/>
-      <c r="D39" s="99"/>
-      <c r="E39" s="99"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="91" t="s">
-        <v>36</v>
-      </c>
-      <c r="H39" s="91"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="92"/>
+      <c r="B39" s="104" t="s">
+        <v>30</v>
+      </c>
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="107"/>
+      <c r="H39" s="107"/>
+      <c r="I39" s="107"/>
+      <c r="J39" s="107"/>
+      <c r="K39" s="108"/>
     </row>
     <row r="40" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B40" s="98"/>
-      <c r="C40" s="99"/>
-      <c r="D40" s="99"/>
-      <c r="E40" s="99"/>
-      <c r="F40" s="77"/>
-      <c r="G40" s="91" t="s">
-        <v>37</v>
-      </c>
-      <c r="H40" s="91"/>
-      <c r="I40" s="91"/>
-      <c r="J40" s="91"/>
-      <c r="K40" s="92"/>
+      <c r="B40" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="C40" s="100"/>
+      <c r="D40" s="100"/>
+      <c r="E40" s="100"/>
+      <c r="F40" s="95"/>
+      <c r="G40" s="96"/>
+      <c r="H40" s="96"/>
+      <c r="I40" s="96"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="97"/>
     </row>
     <row r="41" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B41" s="98"/>
       <c r="C41" s="99"/>
       <c r="D41" s="99"/>
       <c r="E41" s="99"/>
-      <c r="F41" s="101"/>
-      <c r="G41" s="91"/>
-      <c r="H41" s="91"/>
-      <c r="I41" s="91"/>
-      <c r="J41" s="91"/>
-      <c r="K41" s="92"/>
+      <c r="F41" s="70"/>
+      <c r="G41" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="90"/>
     </row>
     <row r="42" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B42" s="98"/>
       <c r="C42" s="99"/>
       <c r="D42" s="99"/>
       <c r="E42" s="99"/>
-      <c r="F42" s="101"/>
-      <c r="G42" s="91"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="91" t="s">
+        <v>32</v>
+      </c>
       <c r="H42" s="91"/>
       <c r="I42" s="91"/>
       <c r="J42" s="91"/>
@@ -50454,8 +50473,10 @@
       <c r="C43" s="99"/>
       <c r="D43" s="99"/>
       <c r="E43" s="99"/>
-      <c r="F43" s="101"/>
-      <c r="G43" s="91"/>
+      <c r="F43" s="77"/>
+      <c r="G43" s="91" t="s">
+        <v>33</v>
+      </c>
       <c r="H43" s="91"/>
       <c r="I43" s="91"/>
       <c r="J43" s="91"/>
@@ -50486,69 +50507,96 @@
       <c r="K45" s="92"/>
     </row>
     <row r="46" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B46" s="109"/>
-      <c r="C46" s="84"/>
-      <c r="D46" s="84"/>
-      <c r="E46" s="84"/>
-      <c r="F46" s="110"/>
-      <c r="G46" s="93"/>
-      <c r="H46" s="93"/>
-      <c r="I46" s="93"/>
-      <c r="J46" s="93"/>
-      <c r="K46" s="94"/>
+      <c r="B46" s="98"/>
+      <c r="C46" s="99"/>
+      <c r="D46" s="99"/>
+      <c r="E46" s="99"/>
+      <c r="F46" s="101"/>
+      <c r="G46" s="91"/>
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="91"/>
+      <c r="K46" s="92"/>
     </row>
     <row r="47" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="F47" s="69"/>
+      <c r="B47" s="98"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="99"/>
+      <c r="E47" s="99"/>
+      <c r="F47" s="101"/>
+      <c r="G47" s="91"/>
+      <c r="H47" s="91"/>
+      <c r="I47" s="91"/>
+      <c r="J47" s="91"/>
+      <c r="K47" s="92"/>
     </row>
     <row r="48" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="F48" s="69"/>
-    </row>
-    <row r="49" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="F49" s="69"/>
-    </row>
-    <row r="50" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+      <c r="B48" s="98"/>
+      <c r="C48" s="99"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="99"/>
+      <c r="F48" s="101"/>
+      <c r="G48" s="91"/>
+      <c r="H48" s="91"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="91"/>
+      <c r="K48" s="92"/>
+    </row>
+    <row r="49" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
+      <c r="B49" s="109"/>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="84"/>
+      <c r="F49" s="110"/>
+      <c r="G49" s="93"/>
+      <c r="H49" s="93"/>
+      <c r="I49" s="93"/>
+      <c r="J49" s="93"/>
+      <c r="K49" s="94"/>
+    </row>
+    <row r="50" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F50" s="69"/>
     </row>
-    <row r="51" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="51" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F51" s="69"/>
     </row>
-    <row r="52" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="52" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F52" s="69"/>
     </row>
-    <row r="53" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="53" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F53" s="69"/>
     </row>
-    <row r="54" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="54" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F54" s="69"/>
     </row>
-    <row r="55" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="55" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F55" s="69"/>
     </row>
-    <row r="56" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="56" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F56" s="69"/>
     </row>
-    <row r="57" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="57" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F57" s="69"/>
     </row>
-    <row r="58" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="58" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F58" s="69"/>
     </row>
-    <row r="59" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="59" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F59" s="69"/>
     </row>
-    <row r="60" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="60" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F60" s="69"/>
     </row>
-    <row r="61" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="61" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F61" s="69"/>
     </row>
-    <row r="62" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="62" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F62" s="69"/>
     </row>
-    <row r="63" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="63" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F63" s="69"/>
     </row>
-    <row r="64" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="64" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F64" s="69"/>
     </row>
     <row r="65" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
@@ -50698,13 +50746,13 @@
     <row r="113" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F113" s="69"/>
     </row>
-    <row r="114" spans="6:6">
+    <row r="114" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F114" s="69"/>
     </row>
-    <row r="115" spans="6:6">
+    <row r="115" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F115" s="69"/>
     </row>
-    <row r="116" spans="6:6">
+    <row r="116" spans="6:6" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F116" s="69"/>
     </row>
     <row r="117" spans="6:6">
@@ -51553,8 +51601,17 @@
     <row r="398" spans="6:6">
       <c r="F398" s="69"/>
     </row>
+    <row r="399" spans="6:6">
+      <c r="F399" s="69"/>
+    </row>
+    <row r="400" spans="6:6">
+      <c r="F400" s="69"/>
+    </row>
+    <row r="401" spans="6:6">
+      <c r="F401" s="69"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F102">
+  <conditionalFormatting sqref="F8:F105">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>$Y$3</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added Android root detection
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10607"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10612"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44E8F80-FDBF-2E4D-B592-7085C4DCF923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EE3FD7B-5F21-C342-AE22-EECB8DE67A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34600" yWindow="-20500" windowWidth="28800" windowHeight="18000" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="0" yWindow="-23040" windowWidth="40960" windowHeight="23040" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -34,17 +34,18 @@
     <definedName name="CH00010_DeviceCompliance_iOS">'Device ☑️'!$F$24</definedName>
     <definedName name="CH00011_DeviceCompliance_macOS">'Device ☑️'!$F$25</definedName>
     <definedName name="CH00012_DeviceCompliance_Windows">'Device ☑️'!$F$26</definedName>
-    <definedName name="CH00013_DeviceCompliance_iOS_Jailbreak">'Device ☑️'!$F$39</definedName>
-    <definedName name="CH00014_DeviceCompliance_Windows_BitLocker">'Device ☑️'!$F$43</definedName>
-    <definedName name="CH00015_DeviceCompliance_DefenderEndPoint">'Device ☑️'!$F$40</definedName>
+    <definedName name="CH00013_DeviceCompliance_iOS_Jailbreak">'Device ☑️'!$F$40</definedName>
+    <definedName name="CH00014_DeviceCompliance_Windows_BitLocker">'Device ☑️'!$F$44</definedName>
+    <definedName name="CH00015_DeviceCompliance_AndroidRoot">'Device ☑️'!$F$39</definedName>
+    <definedName name="CH00015_DeviceCompliance_DefenderEndPoint">'Device ☑️'!$F$41</definedName>
     <definedName name="Device_CP">'Device ☑️'!$B$19</definedName>
-    <definedName name="Device_CP_ADA">'Device ☑️'!$C$72:$C$80</definedName>
-    <definedName name="Device_CP_AECorp">'Device ☑️'!$C$85:$C$93</definedName>
-    <definedName name="Device_CP_AEPersonal">'Device ☑️'!$C$98:$C$106</definedName>
-    <definedName name="Device_CP_AOSP">'Device ☑️'!$C$59:$C$68</definedName>
-    <definedName name="Device_CP_iOS">'Device ☑️'!$C$111:$C$119</definedName>
-    <definedName name="Device_CP_macOS">'Device ☑️'!$C$124:$C$139</definedName>
-    <definedName name="Device_CP_Windows">'Device ☑️'!$C$144:$C$160</definedName>
+    <definedName name="Device_CP_ADA">'Device ☑️'!$C$73:$C$81</definedName>
+    <definedName name="Device_CP_AECorp">'Device ☑️'!$C$86:$C$94</definedName>
+    <definedName name="Device_CP_AEPersonal">'Device ☑️'!$C$99:$C$107</definedName>
+    <definedName name="Device_CP_AOSP">'Device ☑️'!$C$60:$C$69</definedName>
+    <definedName name="Device_CP_iOS">'Device ☑️'!$C$112:$C$120</definedName>
+    <definedName name="Device_CP_macOS">'Device ☑️'!$C$125:$C$140</definedName>
+    <definedName name="Device_CP_Windows">'Device ☑️'!$C$145:$C$161</definedName>
     <definedName name="HeaderAssessedOn">Home!$E$7</definedName>
     <definedName name="HeaderTenantId">Home!$E$5</definedName>
     <definedName name="HeaderTitle">Home!$E$3</definedName>
@@ -1192,7 +1193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="263">
   <si>
     <t>Devices: Info</t>
   </si>
@@ -2050,6 +2051,9 @@
   </si>
   <si>
     <t>iOS Jailbreak detection is Enabled - App Protection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Android root detection is Enabled - Device Compliance Policy </t>
   </si>
 </sst>
 </file>
@@ -3169,47 +3173,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3242,6 +3205,47 @@
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -42136,7 +42140,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -42301,13 +42305,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -42368,13 +42372,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>491400</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>46900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -42418,7 +42422,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -42583,13 +42587,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -42650,7 +42654,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -42815,13 +42819,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>93</xdr:row>
+      <xdr:row>94</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -42882,7 +42886,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -43047,13 +43051,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>106</xdr:row>
+      <xdr:row>107</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -43114,7 +43118,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -43293,13 +43297,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>119</xdr:row>
+      <xdr:row>120</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -43360,13 +43364,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7742870</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>216064</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43410,7 +43414,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -43603,13 +43607,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>140</xdr:row>
       <xdr:rowOff>98200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -43670,13 +43674,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>232730</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>520930</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>72299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43720,13 +43724,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7772400</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>245594</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43770,13 +43774,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>181930</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>470130</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>84999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43820,13 +43824,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7721600</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>84</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>194794</xdr:colOff>
-      <xdr:row>84</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43870,13 +43874,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>194630</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>482830</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>72299</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43920,13 +43924,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7734300</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>97</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>207494</xdr:colOff>
-      <xdr:row>97</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -43970,13 +43974,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>194630</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>126999</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>482830</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>84999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44020,13 +44024,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>181930</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>101599</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>470130</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>186599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44070,13 +44074,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7696200</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>123</xdr:row>
       <xdr:rowOff>101601</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>123</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>186999</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44120,7 +44124,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -44314,13 +44318,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>158</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>160</xdr:row>
       <xdr:rowOff>161700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -44381,13 +44385,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>181930</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>165099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>470130</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>46899</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44431,13 +44435,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7708901</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>143</xdr:row>
       <xdr:rowOff>173376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>139701</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>61063</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44481,13 +44485,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7747001</xdr:colOff>
-      <xdr:row>109</xdr:row>
+      <xdr:row>110</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114301</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>50921</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44533,13 +44537,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7823200</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44587,13 +44591,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>317500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44641,13 +44645,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>92</xdr:row>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>94</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44695,13 +44699,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>105</xdr:row>
+      <xdr:row>106</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>107</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44749,13 +44753,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>119</xdr:row>
       <xdr:rowOff>215900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>120</xdr:row>
+      <xdr:row>121</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44803,13 +44807,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>12700</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>141</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -44857,13 +44861,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>7848600</xdr:colOff>
-      <xdr:row>158</xdr:row>
+      <xdr:row>159</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>161</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -45676,27 +45680,27 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="123"/>
-      <c r="G5" s="123"/>
-      <c r="H5" s="123"/>
+      <c r="F5" s="134"/>
+      <c r="G5" s="134"/>
+      <c r="H5" s="134"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="124"/>
-      <c r="K5" s="124"/>
-      <c r="L5" s="124"/>
-      <c r="M5" s="124"/>
-      <c r="N5" s="124"/>
-      <c r="O5" s="124"/>
-      <c r="P5" s="124"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="135"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="23"/>
-      <c r="W5" s="124"/>
-      <c r="X5" s="124"/>
-      <c r="Y5" s="124"/>
-      <c r="Z5" s="124"/>
+      <c r="W5" s="135"/>
+      <c r="X5" s="135"/>
+      <c r="Y5" s="135"/>
+      <c r="Z5" s="135"/>
       <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -49286,27 +49290,27 @@
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
-      <c r="H5" s="125"/>
+      <c r="F5" s="136"/>
+      <c r="G5" s="136"/>
+      <c r="H5" s="136"/>
       <c r="I5" s="49"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="126"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="126"/>
-      <c r="N5" s="126"/>
-      <c r="O5" s="126"/>
-      <c r="P5" s="126"/>
+      <c r="J5" s="137"/>
+      <c r="K5" s="137"/>
+      <c r="L5" s="137"/>
+      <c r="M5" s="137"/>
+      <c r="N5" s="137"/>
+      <c r="O5" s="137"/>
+      <c r="P5" s="137"/>
       <c r="Q5" s="50"/>
       <c r="R5" s="50"/>
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
       <c r="V5" s="49"/>
-      <c r="W5" s="126"/>
-      <c r="X5" s="126"/>
-      <c r="Y5" s="126"/>
-      <c r="Z5" s="126"/>
+      <c r="W5" s="137"/>
+      <c r="X5" s="137"/>
+      <c r="Y5" s="137"/>
+      <c r="Z5" s="137"/>
       <c r="AA5" s="42"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -51921,7 +51925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
   <dimension ref="A1:AO35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D35" sqref="D35:F35"/>
     </sheetView>
   </sheetViews>
@@ -52127,17 +52131,17 @@
       <c r="D17" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="E17" s="136" t="s">
+      <c r="E17" s="138" t="s">
         <v>207</v>
       </c>
-      <c r="F17" s="136"/>
-      <c r="G17" s="136"/>
-      <c r="H17" s="136"/>
-      <c r="I17" s="136"/>
-      <c r="J17" s="136" t="s">
+      <c r="F17" s="138"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="138"/>
+      <c r="I17" s="138"/>
+      <c r="J17" s="138" t="s">
         <v>209</v>
       </c>
-      <c r="K17" s="136"/>
+      <c r="K17" s="138"/>
       <c r="L17" s="119" t="s">
         <v>210</v>
       </c>
@@ -52145,15 +52149,15 @@
     </row>
     <row r="18" spans="3:21">
       <c r="D18" s="120"/>
-      <c r="E18" s="127"/>
-      <c r="F18" s="131"/>
-      <c r="G18" s="131"/>
-      <c r="H18" s="131"/>
-      <c r="I18" s="128"/>
-      <c r="J18" s="127"/>
-      <c r="K18" s="128"/>
-      <c r="L18" s="127"/>
-      <c r="M18" s="128"/>
+      <c r="E18" s="140"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="142"/>
+      <c r="J18" s="140"/>
+      <c r="K18" s="142"/>
+      <c r="L18" s="140"/>
+      <c r="M18" s="142"/>
     </row>
     <row r="22" spans="3:21" ht="28">
       <c r="C22"/>
@@ -52170,20 +52174,20 @@
       <c r="D24" s="79"/>
     </row>
     <row r="25" spans="3:21">
-      <c r="D25" s="136" t="s">
+      <c r="D25" s="138" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="136"/>
-      <c r="F25" s="136"/>
+      <c r="E25" s="138"/>
+      <c r="F25" s="138"/>
       <c r="G25" s="119" t="s">
         <v>215</v>
       </c>
-      <c r="H25" s="136" t="s">
+      <c r="H25" s="138" t="s">
         <v>207</v>
       </c>
-      <c r="I25" s="136"/>
-      <c r="J25" s="136"/>
-      <c r="K25" s="136"/>
+      <c r="I25" s="138"/>
+      <c r="J25" s="138"/>
+      <c r="K25" s="138"/>
       <c r="L25" s="119" t="s">
         <v>216</v>
       </c>
@@ -52193,14 +52197,14 @@
       <c r="N25" s="119" t="s">
         <v>218</v>
       </c>
-      <c r="O25" s="136" t="s">
+      <c r="O25" s="138" t="s">
         <v>219</v>
       </c>
-      <c r="P25" s="136"/>
-      <c r="Q25" s="136" t="s">
+      <c r="P25" s="138"/>
+      <c r="Q25" s="138" t="s">
         <v>222</v>
       </c>
-      <c r="R25" s="136"/>
+      <c r="R25" s="138"/>
       <c r="S25" s="119" t="s">
         <v>220</v>
       </c>
@@ -52210,24 +52214,24 @@
       <c r="U25" s="120"/>
     </row>
     <row r="26" spans="3:21">
-      <c r="D26" s="127"/>
-      <c r="E26" s="131"/>
-      <c r="F26" s="128"/>
+      <c r="D26" s="140"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="142"/>
       <c r="G26" s="121"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="131"/>
-      <c r="J26" s="131"/>
-      <c r="K26" s="128"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="141"/>
+      <c r="J26" s="141"/>
+      <c r="K26" s="142"/>
       <c r="L26" s="120"/>
       <c r="M26" s="122"/>
       <c r="N26" s="122"/>
-      <c r="O26" s="127"/>
-      <c r="P26" s="128"/>
-      <c r="Q26" s="127"/>
-      <c r="R26" s="128"/>
+      <c r="O26" s="140"/>
+      <c r="P26" s="142"/>
+      <c r="Q26" s="140"/>
+      <c r="R26" s="142"/>
       <c r="S26" s="120"/>
-      <c r="T26" s="127"/>
-      <c r="U26" s="128"/>
+      <c r="T26" s="140"/>
+      <c r="U26" s="142"/>
     </row>
     <row r="27" spans="3:21" ht="17" customHeight="1"/>
     <row r="30" spans="3:21" ht="28">
@@ -52249,18 +52253,18 @@
       <c r="D33" s="79"/>
     </row>
     <row r="34" spans="3:41" s="80" customFormat="1" ht="68">
-      <c r="D34" s="137" t="s">
+      <c r="D34" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="137"/>
-      <c r="F34" s="137"/>
-      <c r="G34" s="137" t="s">
+      <c r="E34" s="139"/>
+      <c r="F34" s="139"/>
+      <c r="G34" s="139" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="137"/>
-      <c r="I34" s="137"/>
-      <c r="J34" s="137"/>
-      <c r="K34" s="137"/>
+      <c r="H34" s="139"/>
+      <c r="I34" s="139"/>
+      <c r="J34" s="139"/>
+      <c r="K34" s="139"/>
       <c r="L34" s="110" t="s">
         <v>225</v>
       </c>
@@ -52276,10 +52280,10 @@
       <c r="P34" s="111" t="s">
         <v>231</v>
       </c>
-      <c r="Q34" s="138" t="s">
+      <c r="Q34" s="145" t="s">
         <v>224</v>
       </c>
-      <c r="R34" s="138"/>
+      <c r="R34" s="145"/>
       <c r="S34" s="111" t="s">
         <v>232</v>
       </c>
@@ -52301,48 +52305,48 @@
       <c r="Y34" s="113" t="s">
         <v>234</v>
       </c>
-      <c r="Z34" s="134" t="s">
+      <c r="Z34" s="143" t="s">
         <v>239</v>
       </c>
-      <c r="AA34" s="134"/>
-      <c r="AB34" s="134" t="s">
+      <c r="AA34" s="143"/>
+      <c r="AB34" s="143" t="s">
         <v>240</v>
       </c>
-      <c r="AC34" s="134"/>
-      <c r="AD34" s="134" t="s">
+      <c r="AC34" s="143"/>
+      <c r="AD34" s="143" t="s">
         <v>241</v>
       </c>
-      <c r="AE34" s="134"/>
-      <c r="AF34" s="134" t="s">
+      <c r="AE34" s="143"/>
+      <c r="AF34" s="143" t="s">
         <v>242</v>
       </c>
-      <c r="AG34" s="134"/>
-      <c r="AH34" s="134" t="s">
+      <c r="AG34" s="143"/>
+      <c r="AH34" s="143" t="s">
         <v>243</v>
       </c>
-      <c r="AI34" s="134"/>
-      <c r="AJ34" s="133" t="s">
+      <c r="AI34" s="143"/>
+      <c r="AJ34" s="152" t="s">
         <v>220</v>
       </c>
-      <c r="AK34" s="133"/>
-      <c r="AL34" s="132" t="s">
+      <c r="AK34" s="152"/>
+      <c r="AL34" s="151" t="s">
         <v>228</v>
       </c>
-      <c r="AM34" s="132"/>
-      <c r="AN34" s="132" t="s">
+      <c r="AM34" s="151"/>
+      <c r="AN34" s="151" t="s">
         <v>229</v>
       </c>
-      <c r="AO34" s="132"/>
+      <c r="AO34" s="151"/>
     </row>
     <row r="35" spans="3:41">
-      <c r="D35" s="127"/>
-      <c r="E35" s="131"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="139"/>
-      <c r="H35" s="140"/>
-      <c r="I35" s="140"/>
-      <c r="J35" s="140"/>
-      <c r="K35" s="141"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="141"/>
+      <c r="F35" s="142"/>
+      <c r="G35" s="146"/>
+      <c r="H35" s="147"/>
+      <c r="I35" s="147"/>
+      <c r="J35" s="147"/>
+      <c r="K35" s="148"/>
       <c r="L35" s="114"/>
       <c r="M35" s="115"/>
       <c r="N35" s="115"/>
@@ -52357,44 +52361,25 @@
       <c r="W35" s="118"/>
       <c r="X35" s="118"/>
       <c r="Y35" s="118"/>
-      <c r="Z35" s="135"/>
-      <c r="AA35" s="135"/>
-      <c r="AB35" s="135"/>
-      <c r="AC35" s="135"/>
-      <c r="AD35" s="135"/>
-      <c r="AE35" s="135"/>
-      <c r="AF35" s="135"/>
-      <c r="AG35" s="135"/>
-      <c r="AH35" s="135"/>
-      <c r="AI35" s="135"/>
-      <c r="AJ35" s="130"/>
-      <c r="AK35" s="130"/>
-      <c r="AL35" s="129"/>
-      <c r="AM35" s="129"/>
-      <c r="AN35" s="129"/>
-      <c r="AO35" s="129"/>
+      <c r="Z35" s="144"/>
+      <c r="AA35" s="144"/>
+      <c r="AB35" s="144"/>
+      <c r="AC35" s="144"/>
+      <c r="AD35" s="144"/>
+      <c r="AE35" s="144"/>
+      <c r="AF35" s="144"/>
+      <c r="AG35" s="144"/>
+      <c r="AH35" s="144"/>
+      <c r="AI35" s="144"/>
+      <c r="AJ35" s="150"/>
+      <c r="AK35" s="150"/>
+      <c r="AL35" s="149"/>
+      <c r="AM35" s="149"/>
+      <c r="AN35" s="149"/>
+      <c r="AO35" s="149"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="AD35:AE35"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="AN35:AO35"/>
     <mergeCell ref="AL35:AM35"/>
@@ -52411,6 +52396,25 @@
     <mergeCell ref="AF34:AG34"/>
     <mergeCell ref="AF35:AG35"/>
     <mergeCell ref="AH35:AI35"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="AD35:AE35"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -52645,9 +52649,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
-  <dimension ref="A1:AF407"/>
+  <dimension ref="A1:AF408"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
   <cols>
@@ -52849,14 +52855,14 @@
       <c r="B10" s="86"/>
       <c r="C10" s="87"/>
       <c r="D10" s="87"/>
-      <c r="E10" s="152" t="s">
+      <c r="E10" s="133" t="s">
         <v>212</v>
       </c>
       <c r="F10" s="70"/>
       <c r="G10" s="88" t="s">
         <v>205</v>
       </c>
-      <c r="H10" s="142"/>
+      <c r="H10" s="123"/>
       <c r="I10" s="88" t="s">
         <v>32</v>
       </c>
@@ -52872,7 +52878,7 @@
       <c r="G11" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="143"/>
+      <c r="H11" s="124"/>
       <c r="I11" s="90" t="s">
         <v>32</v>
       </c>
@@ -52888,7 +52894,7 @@
       <c r="G12" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="144"/>
+      <c r="H12" s="125"/>
       <c r="I12" s="92" t="s">
         <v>32</v>
       </c>
@@ -52918,7 +52924,7 @@
       <c r="G14" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="142"/>
+      <c r="H14" s="123"/>
       <c r="I14" s="88" t="s">
         <v>31</v>
       </c>
@@ -52934,7 +52940,7 @@
       <c r="G15" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="143"/>
+      <c r="H15" s="124"/>
       <c r="I15" s="90" t="s">
         <v>31</v>
       </c>
@@ -52950,7 +52956,7 @@
       <c r="G16" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="143"/>
+      <c r="H16" s="124"/>
       <c r="I16" s="90" t="s">
         <v>31</v>
       </c>
@@ -52966,7 +52972,7 @@
       <c r="G17" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="144"/>
+      <c r="H17" s="125"/>
       <c r="I17" s="92" t="s">
         <v>32</v>
       </c>
@@ -53005,14 +53011,14 @@
       <c r="B20" s="97"/>
       <c r="C20" s="98"/>
       <c r="D20" s="98"/>
-      <c r="E20" s="151" t="s">
+      <c r="E20" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F20" s="70"/>
-      <c r="G20" s="145" t="s">
+      <c r="G20" s="126" t="s">
         <v>245</v>
       </c>
-      <c r="H20" s="142" t="s">
+      <c r="H20" s="123" t="s">
         <v>252</v>
       </c>
       <c r="I20" s="88" t="s">
@@ -53025,14 +53031,14 @@
       <c r="B21" s="97"/>
       <c r="C21" s="98"/>
       <c r="D21" s="98"/>
-      <c r="E21" s="151" t="s">
+      <c r="E21" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F21" s="73"/>
-      <c r="G21" s="146" t="s">
+      <c r="G21" s="127" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="143" t="s">
+      <c r="H21" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I21" s="90" t="s">
@@ -53045,14 +53051,14 @@
       <c r="B22" s="97"/>
       <c r="C22" s="98"/>
       <c r="D22" s="98"/>
-      <c r="E22" s="151" t="s">
+      <c r="E22" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F22" s="73"/>
-      <c r="G22" s="146" t="s">
+      <c r="G22" s="127" t="s">
         <v>247</v>
       </c>
-      <c r="H22" s="143" t="s">
+      <c r="H22" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I22" s="90" t="s">
@@ -53065,14 +53071,14 @@
       <c r="B23" s="97"/>
       <c r="C23" s="98"/>
       <c r="D23" s="98"/>
-      <c r="E23" s="151" t="s">
+      <c r="E23" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F23" s="100"/>
-      <c r="G23" s="146" t="s">
+      <c r="G23" s="127" t="s">
         <v>248</v>
       </c>
-      <c r="H23" s="143" t="s">
+      <c r="H23" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I23" s="90" t="s">
@@ -53085,14 +53091,14 @@
       <c r="B24" s="97"/>
       <c r="C24" s="98"/>
       <c r="D24" s="98"/>
-      <c r="E24" s="151" t="s">
+      <c r="E24" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F24" s="100"/>
-      <c r="G24" s="146" t="s">
+      <c r="G24" s="127" t="s">
         <v>244</v>
       </c>
-      <c r="H24" s="143" t="s">
+      <c r="H24" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I24" s="90" t="s">
@@ -53105,14 +53111,14 @@
       <c r="B25" s="97"/>
       <c r="C25" s="98"/>
       <c r="D25" s="98"/>
-      <c r="E25" s="151" t="s">
+      <c r="E25" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F25" s="100"/>
-      <c r="G25" s="146" t="s">
+      <c r="G25" s="127" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="143" t="s">
+      <c r="H25" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I25" s="90" t="s">
@@ -53125,14 +53131,14 @@
       <c r="B26" s="97"/>
       <c r="C26" s="98"/>
       <c r="D26" s="98"/>
-      <c r="E26" s="151" t="s">
+      <c r="E26" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F26" s="100"/>
-      <c r="G26" s="146" t="s">
+      <c r="G26" s="127" t="s">
         <v>249</v>
       </c>
-      <c r="H26" s="143" t="s">
+      <c r="H26" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I26" s="90" t="s">
@@ -53148,7 +53154,7 @@
       <c r="E27" s="98"/>
       <c r="F27" s="73"/>
       <c r="G27" s="90"/>
-      <c r="H27" s="143"/>
+      <c r="H27" s="124"/>
       <c r="I27" s="90"/>
       <c r="J27" s="90"/>
       <c r="K27" s="91"/>
@@ -53162,7 +53168,7 @@
       <c r="G28" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="H28" s="144"/>
+      <c r="H28" s="125"/>
       <c r="I28" s="92" t="s">
         <v>32</v>
       </c>
@@ -53187,14 +53193,14 @@
       <c r="B30" s="97"/>
       <c r="C30" s="98"/>
       <c r="D30" s="98"/>
-      <c r="E30" s="151" t="s">
+      <c r="E30" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F30" s="70"/>
       <c r="G30" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="H30" s="142" t="s">
+      <c r="H30" s="123" t="s">
         <v>250</v>
       </c>
       <c r="I30" s="88" t="s">
@@ -53207,14 +53213,14 @@
       <c r="B31" s="97"/>
       <c r="C31" s="98"/>
       <c r="D31" s="98"/>
-      <c r="E31" s="151" t="s">
+      <c r="E31" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F31" s="73"/>
       <c r="G31" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="H31" s="143" t="s">
+      <c r="H31" s="124" t="s">
         <v>250</v>
       </c>
       <c r="I31" s="90" t="s">
@@ -53227,14 +53233,14 @@
       <c r="B32" s="97"/>
       <c r="C32" s="98"/>
       <c r="D32" s="98"/>
-      <c r="E32" s="151" t="s">
+      <c r="E32" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F32" s="73"/>
       <c r="G32" s="90" t="s">
         <v>251</v>
       </c>
-      <c r="H32" s="143" t="s">
+      <c r="H32" s="124" t="s">
         <v>250</v>
       </c>
       <c r="I32" s="90" t="s">
@@ -53247,14 +53253,14 @@
       <c r="B33" s="97"/>
       <c r="C33" s="98"/>
       <c r="D33" s="98"/>
-      <c r="E33" s="151" t="s">
+      <c r="E33" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F33" s="75"/>
       <c r="G33" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="H33" s="144" t="s">
+      <c r="H33" s="125" t="s">
         <v>250</v>
       </c>
       <c r="I33" s="92" t="s">
@@ -53286,7 +53292,7 @@
       <c r="G35" s="88" t="s">
         <v>253</v>
       </c>
-      <c r="H35" s="142" t="s">
+      <c r="H35" s="123" t="s">
         <v>252</v>
       </c>
       <c r="I35" s="88"/>
@@ -53302,7 +53308,7 @@
       <c r="G36" s="90" t="s">
         <v>254</v>
       </c>
-      <c r="H36" s="143" t="s">
+      <c r="H36" s="124" t="s">
         <v>252</v>
       </c>
       <c r="I36" s="90"/>
@@ -53318,7 +53324,7 @@
       <c r="G37" s="90" t="s">
         <v>255</v>
       </c>
-      <c r="H37" s="143" t="s">
+      <c r="H37" s="124" t="s">
         <v>31</v>
       </c>
       <c r="I37" s="90"/>
@@ -53334,7 +53340,7 @@
       <c r="G38" s="90" t="s">
         <v>261</v>
       </c>
-      <c r="H38" s="143" t="s">
+      <c r="H38" s="124" t="s">
         <v>31</v>
       </c>
       <c r="I38" s="90"/>
@@ -53345,14 +53351,14 @@
       <c r="B39" s="97"/>
       <c r="C39" s="98"/>
       <c r="D39" s="98"/>
-      <c r="E39" s="151" t="s">
+      <c r="E39" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F39" s="77"/>
       <c r="G39" s="90" t="s">
-        <v>256</v>
-      </c>
-      <c r="H39" s="143" t="s">
+        <v>262</v>
+      </c>
+      <c r="H39" s="124" t="s">
         <v>31</v>
       </c>
       <c r="I39" s="90"/>
@@ -53363,14 +53369,14 @@
       <c r="B40" s="97"/>
       <c r="C40" s="98"/>
       <c r="D40" s="98"/>
-      <c r="E40" s="151" t="s">
+      <c r="E40" s="132" t="s">
         <v>212</v>
       </c>
       <c r="F40" s="77"/>
       <c r="G40" s="90" t="s">
-        <v>257</v>
-      </c>
-      <c r="H40" s="143" t="s">
+        <v>256</v>
+      </c>
+      <c r="H40" s="124" t="s">
         <v>31</v>
       </c>
       <c r="I40" s="90"/>
@@ -53381,13 +53387,15 @@
       <c r="B41" s="97"/>
       <c r="C41" s="98"/>
       <c r="D41" s="98"/>
-      <c r="E41" s="98"/>
+      <c r="E41" s="132" t="s">
+        <v>212</v>
+      </c>
       <c r="F41" s="77"/>
       <c r="G41" s="90" t="s">
-        <v>258</v>
-      </c>
-      <c r="H41" s="143" t="s">
-        <v>250</v>
+        <v>257</v>
+      </c>
+      <c r="H41" s="124" t="s">
+        <v>31</v>
       </c>
       <c r="I41" s="90"/>
       <c r="J41" s="90"/>
@@ -53398,12 +53406,12 @@
       <c r="C42" s="98"/>
       <c r="D42" s="98"/>
       <c r="E42" s="98"/>
-      <c r="F42" s="71"/>
+      <c r="F42" s="77"/>
       <c r="G42" s="90" t="s">
-        <v>25</v>
-      </c>
-      <c r="H42" s="143" t="s">
-        <v>252</v>
+        <v>258</v>
+      </c>
+      <c r="H42" s="124" t="s">
+        <v>250</v>
       </c>
       <c r="I42" s="90"/>
       <c r="J42" s="90"/>
@@ -53413,91 +53421,93 @@
       <c r="B43" s="97"/>
       <c r="C43" s="98"/>
       <c r="D43" s="98"/>
-      <c r="E43" s="151" t="s">
-        <v>212</v>
-      </c>
-      <c r="F43" s="147"/>
-      <c r="G43" s="148" t="s">
-        <v>259</v>
-      </c>
-      <c r="H43" s="149" t="s">
+      <c r="E43" s="98"/>
+      <c r="F43" s="71"/>
+      <c r="G43" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="H43" s="124" t="s">
         <v>252</v>
       </c>
-      <c r="I43" s="148"/>
-      <c r="J43" s="148"/>
-      <c r="K43" s="150"/>
+      <c r="I43" s="90"/>
+      <c r="J43" s="90"/>
+      <c r="K43" s="91"/>
     </row>
     <row r="44" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B44" s="97"/>
       <c r="C44" s="98"/>
       <c r="D44" s="98"/>
-      <c r="E44" s="98"/>
-      <c r="F44" s="72"/>
-      <c r="G44" s="92" t="s">
+      <c r="E44" s="132" t="s">
+        <v>212</v>
+      </c>
+      <c r="F44" s="128"/>
+      <c r="G44" s="129" t="s">
+        <v>259</v>
+      </c>
+      <c r="H44" s="130" t="s">
+        <v>252</v>
+      </c>
+      <c r="I44" s="129"/>
+      <c r="J44" s="129"/>
+      <c r="K44" s="131"/>
+    </row>
+    <row r="45" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
+      <c r="B45" s="97"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="98"/>
+      <c r="E45" s="98"/>
+      <c r="F45" s="72"/>
+      <c r="G45" s="92" t="s">
         <v>260</v>
       </c>
-      <c r="H44" s="144" t="s">
+      <c r="H45" s="125" t="s">
         <v>252</v>
       </c>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="93"/>
-    </row>
-    <row r="45" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B45" s="103" t="s">
+      <c r="I45" s="92"/>
+      <c r="J45" s="92"/>
+      <c r="K45" s="93"/>
+    </row>
+    <row r="46" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
+      <c r="B46" s="103" t="s">
         <v>26</v>
       </c>
-      <c r="C45" s="104"/>
-      <c r="D45" s="104"/>
-      <c r="E45" s="104"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="105"/>
-      <c r="I45" s="106"/>
-      <c r="J45" s="106"/>
-      <c r="K45" s="107"/>
-    </row>
-    <row r="46" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B46" s="81" t="s">
+      <c r="C46" s="104"/>
+      <c r="D46" s="104"/>
+      <c r="E46" s="104"/>
+      <c r="F46" s="105"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="106"/>
+      <c r="K46" s="107"/>
+    </row>
+    <row r="47" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
+      <c r="B47" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="C46" s="99"/>
-      <c r="D46" s="99"/>
-      <c r="E46" s="99"/>
-      <c r="F46" s="94"/>
-      <c r="G46" s="95"/>
-      <c r="H46" s="94"/>
-      <c r="I46" s="95"/>
-      <c r="J46" s="95"/>
-      <c r="K46" s="96"/>
-    </row>
-    <row r="47" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B47" s="97"/>
-      <c r="C47" s="98"/>
-      <c r="D47" s="98"/>
-      <c r="E47" s="98"/>
-      <c r="F47" s="70"/>
-      <c r="G47" s="88" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="142"/>
-      <c r="I47" s="88"/>
-      <c r="J47" s="88"/>
-      <c r="K47" s="89"/>
+      <c r="C47" s="99"/>
+      <c r="D47" s="99"/>
+      <c r="E47" s="99"/>
+      <c r="F47" s="94"/>
+      <c r="G47" s="95"/>
+      <c r="H47" s="94"/>
+      <c r="I47" s="95"/>
+      <c r="J47" s="95"/>
+      <c r="K47" s="96"/>
     </row>
     <row r="48" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B48" s="97"/>
       <c r="C48" s="98"/>
       <c r="D48" s="98"/>
       <c r="E48" s="98"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="143"/>
-      <c r="I48" s="90"/>
-      <c r="J48" s="90"/>
-      <c r="K48" s="91"/>
+      <c r="F48" s="70"/>
+      <c r="G48" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="H48" s="123"/>
+      <c r="I48" s="88"/>
+      <c r="J48" s="88"/>
+      <c r="K48" s="89"/>
     </row>
     <row r="49" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B49" s="97"/>
@@ -53506,9 +53516,9 @@
       <c r="E49" s="98"/>
       <c r="F49" s="77"/>
       <c r="G49" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49" s="143"/>
+        <v>28</v>
+      </c>
+      <c r="H49" s="124"/>
       <c r="I49" s="90"/>
       <c r="J49" s="90"/>
       <c r="K49" s="91"/>
@@ -53518,9 +53528,11 @@
       <c r="C50" s="98"/>
       <c r="D50" s="98"/>
       <c r="E50" s="98"/>
-      <c r="F50" s="100"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="143"/>
+      <c r="F50" s="77"/>
+      <c r="G50" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="H50" s="124"/>
       <c r="I50" s="90"/>
       <c r="J50" s="90"/>
       <c r="K50" s="91"/>
@@ -53532,7 +53544,7 @@
       <c r="E51" s="98"/>
       <c r="F51" s="100"/>
       <c r="G51" s="90"/>
-      <c r="H51" s="143"/>
+      <c r="H51" s="124"/>
       <c r="I51" s="90"/>
       <c r="J51" s="90"/>
       <c r="K51" s="91"/>
@@ -53544,7 +53556,7 @@
       <c r="E52" s="98"/>
       <c r="F52" s="100"/>
       <c r="G52" s="90"/>
-      <c r="H52" s="143"/>
+      <c r="H52" s="124"/>
       <c r="I52" s="90"/>
       <c r="J52" s="90"/>
       <c r="K52" s="91"/>
@@ -53556,7 +53568,7 @@
       <c r="E53" s="98"/>
       <c r="F53" s="100"/>
       <c r="G53" s="90"/>
-      <c r="H53" s="143"/>
+      <c r="H53" s="124"/>
       <c r="I53" s="90"/>
       <c r="J53" s="90"/>
       <c r="K53" s="91"/>
@@ -53568,25 +53580,34 @@
       <c r="E54" s="98"/>
       <c r="F54" s="100"/>
       <c r="G54" s="90"/>
-      <c r="H54" s="143"/>
+      <c r="H54" s="124"/>
       <c r="I54" s="90"/>
       <c r="J54" s="90"/>
       <c r="K54" s="91"/>
     </row>
     <row r="55" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="B55" s="108"/>
-      <c r="C55" s="84"/>
-      <c r="D55" s="84"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="109"/>
-      <c r="G55" s="92"/>
-      <c r="H55" s="144"/>
-      <c r="I55" s="92"/>
-      <c r="J55" s="92"/>
-      <c r="K55" s="93"/>
+      <c r="B55" s="97"/>
+      <c r="C55" s="98"/>
+      <c r="D55" s="98"/>
+      <c r="E55" s="98"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="90"/>
+      <c r="H55" s="124"/>
+      <c r="I55" s="90"/>
+      <c r="J55" s="90"/>
+      <c r="K55" s="91"/>
     </row>
     <row r="56" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
-      <c r="F56" s="69"/>
+      <c r="B56" s="108"/>
+      <c r="C56" s="84"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="84"/>
+      <c r="F56" s="109"/>
+      <c r="G56" s="92"/>
+      <c r="H56" s="125"/>
+      <c r="I56" s="92"/>
+      <c r="J56" s="92"/>
+      <c r="K56" s="93"/>
     </row>
     <row r="57" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F57" s="69"/>
@@ -53777,24 +53798,17 @@
     <row r="119" spans="1:8" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F119" s="69"/>
     </row>
-    <row r="120" spans="1:8" s="62" customFormat="1" ht="27" customHeight="1">
+    <row r="120" spans="1:8" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F120" s="69"/>
     </row>
-    <row r="121" spans="1:8" s="62" customFormat="1" ht="26" customHeight="1">
+    <row r="121" spans="1:8" s="62" customFormat="1" ht="27" customHeight="1">
       <c r="F121" s="69"/>
     </row>
     <row r="122" spans="1:8" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F122" s="69"/>
     </row>
-    <row r="123" spans="1:8">
-      <c r="A123" s="62"/>
-      <c r="B123" s="62"/>
-      <c r="C123" s="62"/>
-      <c r="D123" s="62"/>
-      <c r="E123" s="62"/>
+    <row r="123" spans="1:8" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="F123" s="69"/>
-      <c r="G123" s="62"/>
-      <c r="H123" s="62"/>
     </row>
     <row r="124" spans="1:8">
       <c r="A124" s="62"/>
@@ -53907,7 +53921,14 @@
       <c r="H134" s="62"/>
     </row>
     <row r="135" spans="1:8">
+      <c r="A135" s="62"/>
+      <c r="B135" s="62"/>
+      <c r="C135" s="62"/>
+      <c r="D135" s="62"/>
+      <c r="E135" s="62"/>
       <c r="F135" s="69"/>
+      <c r="G135" s="62"/>
+      <c r="H135" s="62"/>
     </row>
     <row r="136" spans="1:8">
       <c r="F136" s="69"/>
@@ -54725,8 +54746,11 @@
     <row r="407" spans="6:6">
       <c r="F407" s="69"/>
     </row>
+    <row r="408" spans="6:6">
+      <c r="F408" s="69"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="F8:F134">
+  <conditionalFormatting sqref="F8:F135">
     <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>$Y$3</formula>
     </cfRule>
@@ -54755,9 +54779,10 @@
     <hyperlink ref="E26" location="Table_WindowsEnrollment" display="🚦" xr:uid="{DE507200-CEB6-3243-BED2-C3C30F98C48F}"/>
     <hyperlink ref="E20:E26" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{3A549D6D-14CB-DF43-9030-B6A5AB6125ED}"/>
     <hyperlink ref="E30:E33" location="Table_EnrollmentDevicePlatformRestrictions" display="🚦" xr:uid="{8E195C76-CEC1-F84A-983C-906F37236965}"/>
-    <hyperlink ref="E39" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{BCBE9148-2D47-3247-822C-0F59830EAB4A}"/>
-    <hyperlink ref="E43" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{926241E4-CD42-474B-8E11-F444A9AA977E}"/>
-    <hyperlink ref="E40" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{DF8D7B5A-DFE1-3C4B-8514-0792D497ADA6}"/>
+    <hyperlink ref="E40" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{BCBE9148-2D47-3247-822C-0F59830EAB4A}"/>
+    <hyperlink ref="E44" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{926241E4-CD42-474B-8E11-F444A9AA977E}"/>
+    <hyperlink ref="E41" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{DF8D7B5A-DFE1-3C4B-8514-0792D497ADA6}"/>
+    <hyperlink ref="E39" location="Table_DeviceCompliancePolicies" display="🚦" xr:uid="{AD8C9AF0-CB43-C044-96A0-ABAAC7B9DB66}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Added app protection policy
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10612"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68FC103-01E5-A84F-AC88-F0CF92AC2D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6142F17-87D2-654A-AA41-0630D2ACFB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-23040" windowWidth="40960" windowHeight="23040" tabRatio="710" activeTab="6" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="0" yWindow="-23040" windowWidth="40960" windowHeight="23040" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -55,6 +55,7 @@
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
     <definedName name="Status">'Identity ✍️'!$AD$3:$AK$3</definedName>
+    <definedName name="Table_AppProtectionPolicies">'Device ⚙️'!$D$44</definedName>
     <definedName name="Table_DeviceCompliancePolicies">'Device ⚙️'!$D$35</definedName>
     <definedName name="Table_EnrollmentDevicePlatformRestrictions">'Device ⚙️'!$D$26</definedName>
     <definedName name="Table_WindowsEnrollment">'Device ⚙️'!$D$18</definedName>
@@ -1195,7 +1196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="289">
   <si>
     <t>Devices: Info</t>
   </si>
@@ -2045,6 +2046,99 @@
   <si>
     <t>macOS - Firewall is enabled</t>
   </si>
+  <si>
+    <t>App protection policies</t>
+  </si>
+  <si>
+    <t>Public apps</t>
+  </si>
+  <si>
+    <t>Custom apps</t>
+  </si>
+  <si>
+    <t>Apps</t>
+  </si>
+  <si>
+    <t>Prevent backups</t>
+  </si>
+  <si>
+    <t>Send org data to other apps</t>
+  </si>
+  <si>
+    <t>Apps to exempt</t>
+  </si>
+  <si>
+    <t>Save copies of org data</t>
+  </si>
+  <si>
+    <t>Allow user to save copies to selected services</t>
+  </si>
+  <si>
+    <t>Transfer telecommunication data to</t>
+  </si>
+  <si>
+    <t>Receive data from other apps</t>
+  </si>
+  <si>
+    <t>Open data into Org documents</t>
+  </si>
+  <si>
+    <t>Allow users to open data from selected services</t>
+  </si>
+  <si>
+    <t>Restrict cut, copy, and paste between other apps</t>
+  </si>
+  <si>
+    <t>Cut and copy character limit for any app</t>
+  </si>
+  <si>
+    <t>Encrypt org data</t>
+  </si>
+  <si>
+    <t>Sync policy managed app data with native apps or add-ins</t>
+  </si>
+  <si>
+    <t>Printing org data</t>
+  </si>
+  <si>
+    <t>Restrict web content transfer with other apps</t>
+  </si>
+  <si>
+    <t>Org data notifications</t>
+  </si>
+  <si>
+    <t>Offline grace period
+Block access (min)</t>
+  </si>
+  <si>
+    <t>Offline grace period
+Wipe data (days)</t>
+  </si>
+  <si>
+    <t>Disabed account</t>
+  </si>
+  <si>
+    <t>Conditional launch - App conditions</t>
+  </si>
+  <si>
+    <t>Primary MTD service</t>
+  </si>
+  <si>
+    <t>Max PIN attempts 
+(Action)</t>
+  </si>
+  <si>
+    <t>Min app version (Action)</t>
+  </si>
+  <si>
+    <t>Max allowed device threat level</t>
+  </si>
+  <si>
+    <t>Conditional launch - Device conditions</t>
+  </si>
+  <si>
+    <t>Assignments</t>
+  </si>
 </sst>
 </file>
 
@@ -2326,7 +2420,7 @@
       <name val="Segoe UI"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2474,8 +2568,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -2833,6 +2933,139 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-4.9989318521683403E-2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2841,7 +3074,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3125,33 +3358,6 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="24" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3205,33 +3411,159 @@
     <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="24" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -40750,6 +41082,126 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5D09937-D45E-CA42-B39D-71054EA0EA0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1663700" y="7988300"/>
+          <a:ext cx="15506700" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>App protection policies (APP) are rules that ensure an organization's data remains safe or contained in a managed app. A policy can be a rule that is enforced when the user attempts to access or move "corporate" data, or a set of actions that are prohibited or monitored when the user is inside the app. A managed app is an app that has app protection policies applied to it, and can be managed by Intune.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>254000</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="635000" cy="635000"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Graphic 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{997D3199-531A-7846-AF43-696045DF02F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId23"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="736600" y="10515600"/>
+          <a:ext cx="635000" cy="635000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -45667,27 +46119,27 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="133"/>
-      <c r="G5" s="133"/>
-      <c r="H5" s="133"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="124"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="134"/>
-      <c r="K5" s="134"/>
-      <c r="L5" s="134"/>
-      <c r="M5" s="134"/>
-      <c r="N5" s="134"/>
-      <c r="O5" s="134"/>
-      <c r="P5" s="134"/>
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="125"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="23"/>
-      <c r="W5" s="134"/>
-      <c r="X5" s="134"/>
-      <c r="Y5" s="134"/>
-      <c r="Z5" s="134"/>
+      <c r="W5" s="125"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="125"/>
+      <c r="Z5" s="125"/>
       <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -49110,8 +49562,8 @@
   <dimension ref="A1:AK154"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="7" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="30" customHeight="1"/>
@@ -49277,27 +49729,27 @@
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="135"/>
-      <c r="H5" s="135"/>
+      <c r="F5" s="126"/>
+      <c r="G5" s="126"/>
+      <c r="H5" s="126"/>
       <c r="I5" s="49"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="136"/>
-      <c r="L5" s="136"/>
-      <c r="M5" s="136"/>
-      <c r="N5" s="136"/>
-      <c r="O5" s="136"/>
-      <c r="P5" s="136"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="127"/>
+      <c r="O5" s="127"/>
+      <c r="P5" s="127"/>
       <c r="Q5" s="50"/>
       <c r="R5" s="50"/>
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
       <c r="V5" s="49"/>
-      <c r="W5" s="136"/>
-      <c r="X5" s="136"/>
-      <c r="Y5" s="136"/>
-      <c r="Z5" s="136"/>
+      <c r="W5" s="127"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="127"/>
       <c r="AA5" s="42"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -51910,10 +52362,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
-  <dimension ref="A1:AO35"/>
+  <dimension ref="A1:AY44"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35:F35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L43" sqref="L43:M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -52115,36 +52568,36 @@
       <c r="D16" s="78"/>
     </row>
     <row r="17" spans="3:21">
-      <c r="D17" s="118" t="s">
+      <c r="D17" s="109" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="137" t="s">
+      <c r="E17" s="131" t="s">
         <v>201</v>
       </c>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137"/>
-      <c r="J17" s="137" t="s">
+      <c r="F17" s="131"/>
+      <c r="G17" s="131"/>
+      <c r="H17" s="131"/>
+      <c r="I17" s="131"/>
+      <c r="J17" s="131" t="s">
         <v>203</v>
       </c>
-      <c r="K17" s="137"/>
-      <c r="L17" s="118" t="s">
+      <c r="K17" s="131"/>
+      <c r="L17" s="109" t="s">
         <v>204</v>
       </c>
-      <c r="M17" s="119"/>
+      <c r="M17" s="110"/>
     </row>
     <row r="18" spans="3:21">
-      <c r="D18" s="119"/>
-      <c r="E18" s="139"/>
-      <c r="F18" s="140"/>
-      <c r="G18" s="140"/>
-      <c r="H18" s="140"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="139"/>
-      <c r="K18" s="141"/>
-      <c r="L18" s="139"/>
-      <c r="M18" s="141"/>
+      <c r="D18" s="110"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="130"/>
+      <c r="G18" s="130"/>
+      <c r="H18" s="130"/>
+      <c r="I18" s="129"/>
+      <c r="J18" s="128"/>
+      <c r="K18" s="129"/>
+      <c r="L18" s="128"/>
+      <c r="M18" s="129"/>
     </row>
     <row r="22" spans="3:21" ht="28">
       <c r="C22"/>
@@ -52161,64 +52614,64 @@
       <c r="D24" s="78"/>
     </row>
     <row r="25" spans="3:21">
-      <c r="D25" s="137" t="s">
+      <c r="D25" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="137"/>
-      <c r="F25" s="137"/>
-      <c r="G25" s="118" t="s">
+      <c r="E25" s="131"/>
+      <c r="F25" s="131"/>
+      <c r="G25" s="109" t="s">
         <v>209</v>
       </c>
-      <c r="H25" s="137" t="s">
+      <c r="H25" s="131" t="s">
         <v>201</v>
       </c>
-      <c r="I25" s="137"/>
-      <c r="J25" s="137"/>
-      <c r="K25" s="137"/>
-      <c r="L25" s="118" t="s">
+      <c r="I25" s="131"/>
+      <c r="J25" s="131"/>
+      <c r="K25" s="131"/>
+      <c r="L25" s="109" t="s">
         <v>210</v>
       </c>
-      <c r="M25" s="118" t="s">
+      <c r="M25" s="109" t="s">
         <v>211</v>
       </c>
-      <c r="N25" s="118" t="s">
+      <c r="N25" s="109" t="s">
         <v>212</v>
       </c>
-      <c r="O25" s="137" t="s">
+      <c r="O25" s="131" t="s">
         <v>213</v>
       </c>
-      <c r="P25" s="137"/>
-      <c r="Q25" s="137" t="s">
+      <c r="P25" s="131"/>
+      <c r="Q25" s="131" t="s">
         <v>216</v>
       </c>
-      <c r="R25" s="137"/>
-      <c r="S25" s="118" t="s">
+      <c r="R25" s="131"/>
+      <c r="S25" s="109" t="s">
         <v>214</v>
       </c>
-      <c r="T25" s="118" t="s">
+      <c r="T25" s="109" t="s">
         <v>215</v>
       </c>
-      <c r="U25" s="119"/>
+      <c r="U25" s="110"/>
     </row>
     <row r="26" spans="3:21">
-      <c r="D26" s="139"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="141"/>
-      <c r="G26" s="120"/>
-      <c r="H26" s="139"/>
-      <c r="I26" s="140"/>
-      <c r="J26" s="140"/>
-      <c r="K26" s="141"/>
-      <c r="L26" s="119"/>
-      <c r="M26" s="121"/>
-      <c r="N26" s="121"/>
-      <c r="O26" s="139"/>
-      <c r="P26" s="141"/>
-      <c r="Q26" s="139"/>
-      <c r="R26" s="141"/>
-      <c r="S26" s="119"/>
-      <c r="T26" s="139"/>
-      <c r="U26" s="141"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="130"/>
+      <c r="F26" s="129"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="128"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="130"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="110"/>
+      <c r="M26" s="112"/>
+      <c r="N26" s="112"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="129"/>
+      <c r="Q26" s="128"/>
+      <c r="R26" s="129"/>
+      <c r="S26" s="110"/>
+      <c r="T26" s="128"/>
+      <c r="U26" s="129"/>
     </row>
     <row r="27" spans="3:21" ht="17" customHeight="1"/>
     <row r="30" spans="3:21" ht="28">
@@ -52235,138 +52688,416 @@
       <c r="C32" s="77"/>
       <c r="D32" s="78"/>
     </row>
-    <row r="33" spans="3:41" ht="16" customHeight="1">
+    <row r="33" spans="1:51" ht="16" customHeight="1">
       <c r="C33" s="77"/>
       <c r="D33" s="78"/>
     </row>
-    <row r="34" spans="3:41" s="79" customFormat="1" ht="68">
-      <c r="D34" s="138" t="s">
+    <row r="34" spans="1:51" s="79" customFormat="1" ht="68">
+      <c r="D34" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="138"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138" t="s">
+      <c r="E34" s="132"/>
+      <c r="F34" s="132"/>
+      <c r="G34" s="132" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="138"/>
-      <c r="I34" s="138"/>
-      <c r="J34" s="138"/>
-      <c r="K34" s="138"/>
-      <c r="L34" s="109" t="s">
+      <c r="H34" s="132"/>
+      <c r="I34" s="132"/>
+      <c r="J34" s="132"/>
+      <c r="K34" s="136"/>
+      <c r="L34" s="149" t="s">
         <v>219</v>
       </c>
-      <c r="M34" s="110" t="s">
+      <c r="M34" s="150" t="s">
         <v>220</v>
       </c>
-      <c r="N34" s="110" t="s">
+      <c r="N34" s="150" t="s">
         <v>221</v>
       </c>
-      <c r="O34" s="111" t="s">
+      <c r="O34" s="151" t="s">
         <v>224</v>
       </c>
-      <c r="P34" s="110" t="s">
+      <c r="P34" s="150" t="s">
         <v>225</v>
       </c>
-      <c r="Q34" s="144" t="s">
+      <c r="Q34" s="152" t="s">
         <v>218</v>
       </c>
-      <c r="R34" s="144"/>
-      <c r="S34" s="110" t="s">
+      <c r="R34" s="152"/>
+      <c r="S34" s="150" t="s">
         <v>226</v>
       </c>
-      <c r="T34" s="110" t="s">
+      <c r="T34" s="150" t="s">
         <v>232</v>
       </c>
-      <c r="U34" s="110" t="s">
+      <c r="U34" s="150" t="s">
         <v>231</v>
       </c>
-      <c r="V34" s="112" t="s">
+      <c r="V34" s="153" t="s">
         <v>227</v>
       </c>
-      <c r="W34" s="112" t="s">
+      <c r="W34" s="153" t="s">
         <v>229</v>
       </c>
-      <c r="X34" s="112" t="s">
+      <c r="X34" s="153" t="s">
         <v>230</v>
       </c>
-      <c r="Y34" s="112" t="s">
+      <c r="Y34" s="153" t="s">
         <v>228</v>
       </c>
-      <c r="Z34" s="142" t="s">
+      <c r="Z34" s="154" t="s">
         <v>233</v>
       </c>
-      <c r="AA34" s="142"/>
-      <c r="AB34" s="142" t="s">
+      <c r="AA34" s="154"/>
+      <c r="AB34" s="154" t="s">
         <v>234</v>
       </c>
-      <c r="AC34" s="142"/>
-      <c r="AD34" s="142" t="s">
+      <c r="AC34" s="154"/>
+      <c r="AD34" s="154" t="s">
         <v>235</v>
       </c>
-      <c r="AE34" s="142"/>
-      <c r="AF34" s="142" t="s">
+      <c r="AE34" s="154"/>
+      <c r="AF34" s="154" t="s">
         <v>236</v>
       </c>
-      <c r="AG34" s="142"/>
-      <c r="AH34" s="142" t="s">
+      <c r="AG34" s="154"/>
+      <c r="AH34" s="154" t="s">
         <v>237</v>
       </c>
-      <c r="AI34" s="142"/>
-      <c r="AJ34" s="151" t="s">
+      <c r="AI34" s="154"/>
+      <c r="AJ34" s="155" t="s">
         <v>214</v>
       </c>
-      <c r="AK34" s="151"/>
-      <c r="AL34" s="150" t="s">
+      <c r="AK34" s="155"/>
+      <c r="AL34" s="156" t="s">
         <v>222</v>
       </c>
-      <c r="AM34" s="150"/>
-      <c r="AN34" s="150" t="s">
+      <c r="AM34" s="156"/>
+      <c r="AN34" s="156" t="s">
         <v>223</v>
       </c>
-      <c r="AO34" s="150"/>
-    </row>
-    <row r="35" spans="3:41">
-      <c r="D35" s="139"/>
-      <c r="E35" s="140"/>
-      <c r="F35" s="141"/>
-      <c r="G35" s="145"/>
-      <c r="H35" s="146"/>
-      <c r="I35" s="146"/>
-      <c r="J35" s="146"/>
-      <c r="K35" s="147"/>
-      <c r="L35" s="113"/>
-      <c r="M35" s="114"/>
-      <c r="N35" s="114"/>
-      <c r="O35" s="115"/>
-      <c r="P35" s="114"/>
-      <c r="Q35" s="116"/>
-      <c r="R35" s="116"/>
-      <c r="S35" s="114"/>
-      <c r="T35" s="114"/>
-      <c r="U35" s="114"/>
-      <c r="V35" s="117"/>
-      <c r="W35" s="117"/>
-      <c r="X35" s="117"/>
-      <c r="Y35" s="117"/>
-      <c r="Z35" s="143"/>
-      <c r="AA35" s="143"/>
-      <c r="AB35" s="143"/>
-      <c r="AC35" s="143"/>
-      <c r="AD35" s="143"/>
-      <c r="AE35" s="143"/>
-      <c r="AF35" s="143"/>
-      <c r="AG35" s="143"/>
-      <c r="AH35" s="143"/>
-      <c r="AI35" s="143"/>
-      <c r="AJ35" s="149"/>
-      <c r="AK35" s="149"/>
+      <c r="AO34" s="156"/>
+    </row>
+    <row r="35" spans="1:51">
+      <c r="D35" s="128"/>
+      <c r="E35" s="130"/>
+      <c r="F35" s="129"/>
+      <c r="G35" s="133"/>
+      <c r="H35" s="134"/>
+      <c r="I35" s="134"/>
+      <c r="J35" s="134"/>
+      <c r="K35" s="135"/>
+      <c r="L35" s="141"/>
+      <c r="M35" s="142"/>
+      <c r="N35" s="142"/>
+      <c r="O35" s="143"/>
+      <c r="P35" s="142"/>
+      <c r="Q35" s="144"/>
+      <c r="R35" s="144"/>
+      <c r="S35" s="142"/>
+      <c r="T35" s="142"/>
+      <c r="U35" s="142"/>
+      <c r="V35" s="145"/>
+      <c r="W35" s="145"/>
+      <c r="X35" s="145"/>
+      <c r="Y35" s="145"/>
+      <c r="Z35" s="146"/>
+      <c r="AA35" s="146"/>
+      <c r="AB35" s="146"/>
+      <c r="AC35" s="146"/>
+      <c r="AD35" s="146"/>
+      <c r="AE35" s="146"/>
+      <c r="AF35" s="146"/>
+      <c r="AG35" s="146"/>
+      <c r="AH35" s="146"/>
+      <c r="AI35" s="146"/>
+      <c r="AJ35" s="147"/>
+      <c r="AK35" s="147"/>
       <c r="AL35" s="148"/>
       <c r="AM35" s="148"/>
       <c r="AN35" s="148"/>
       <c r="AO35" s="148"/>
     </row>
+    <row r="39" spans="1:51" ht="28">
+      <c r="C39"/>
+      <c r="D39" s="78" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="40" spans="1:51" ht="28">
+      <c r="C40" s="77"/>
+      <c r="D40" s="78"/>
+    </row>
+    <row r="41" spans="1:51" ht="28">
+      <c r="C41" s="77"/>
+      <c r="D41" s="78"/>
+    </row>
+    <row r="42" spans="1:51" ht="28">
+      <c r="C42" s="77"/>
+      <c r="D42" s="78"/>
+      <c r="L42" s="158" t="s">
+        <v>262</v>
+      </c>
+      <c r="M42" s="158"/>
+      <c r="N42" s="158"/>
+      <c r="O42" s="159" t="s">
+        <v>118</v>
+      </c>
+      <c r="P42" s="159"/>
+      <c r="Q42" s="159"/>
+      <c r="R42" s="159"/>
+      <c r="S42" s="159"/>
+      <c r="T42" s="159"/>
+      <c r="U42" s="159"/>
+      <c r="V42" s="159"/>
+      <c r="W42" s="159"/>
+      <c r="X42" s="159"/>
+      <c r="Y42" s="159"/>
+      <c r="Z42" s="159"/>
+      <c r="AA42" s="159"/>
+      <c r="AB42" s="159"/>
+      <c r="AC42" s="159"/>
+      <c r="AD42" s="159"/>
+      <c r="AE42" s="161" t="s">
+        <v>282</v>
+      </c>
+      <c r="AF42" s="161"/>
+      <c r="AG42" s="161"/>
+      <c r="AH42" s="161"/>
+      <c r="AI42" s="161"/>
+      <c r="AJ42" s="161"/>
+      <c r="AK42" s="160" t="s">
+        <v>287</v>
+      </c>
+      <c r="AL42" s="160"/>
+      <c r="AM42" s="160"/>
+      <c r="AN42" s="160"/>
+      <c r="AO42" s="160"/>
+      <c r="AP42" s="160"/>
+      <c r="AQ42" s="160"/>
+      <c r="AR42" s="160"/>
+      <c r="AS42" s="160"/>
+      <c r="AT42" s="166" t="s">
+        <v>288</v>
+      </c>
+      <c r="AU42" s="166"/>
+      <c r="AV42" s="166"/>
+      <c r="AW42" s="166"/>
+      <c r="AX42" s="166"/>
+      <c r="AY42" s="166"/>
+    </row>
+    <row r="43" spans="1:51" ht="153">
+      <c r="A43" s="79"/>
+      <c r="B43" s="79"/>
+      <c r="C43" s="79"/>
+      <c r="D43" s="132" t="s">
+        <v>2</v>
+      </c>
+      <c r="E43" s="132"/>
+      <c r="F43" s="136"/>
+      <c r="G43" s="140" t="s">
+        <v>1</v>
+      </c>
+      <c r="H43" s="140"/>
+      <c r="I43" s="140"/>
+      <c r="J43" s="140"/>
+      <c r="K43" s="140"/>
+      <c r="L43" s="169" t="s">
+        <v>260</v>
+      </c>
+      <c r="M43" s="170"/>
+      <c r="N43" s="171" t="s">
+        <v>261</v>
+      </c>
+      <c r="O43" s="172" t="s">
+        <v>263</v>
+      </c>
+      <c r="P43" s="172" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q43" s="172" t="s">
+        <v>265</v>
+      </c>
+      <c r="R43" s="172" t="s">
+        <v>266</v>
+      </c>
+      <c r="S43" s="172" t="s">
+        <v>267</v>
+      </c>
+      <c r="T43" s="172" t="s">
+        <v>268</v>
+      </c>
+      <c r="U43" s="172" t="s">
+        <v>269</v>
+      </c>
+      <c r="V43" s="172" t="s">
+        <v>270</v>
+      </c>
+      <c r="W43" s="172" t="s">
+        <v>271</v>
+      </c>
+      <c r="X43" s="172" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y43" s="172" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z43" s="173" t="s">
+        <v>274</v>
+      </c>
+      <c r="AA43" s="173" t="s">
+        <v>275</v>
+      </c>
+      <c r="AB43" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC43" s="173" t="s">
+        <v>277</v>
+      </c>
+      <c r="AD43" s="173" t="s">
+        <v>278</v>
+      </c>
+      <c r="AE43" s="174" t="s">
+        <v>284</v>
+      </c>
+      <c r="AF43" s="175"/>
+      <c r="AG43" s="176" t="s">
+        <v>279</v>
+      </c>
+      <c r="AH43" s="176" t="s">
+        <v>280</v>
+      </c>
+      <c r="AI43" s="176" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ43" s="176" t="s">
+        <v>285</v>
+      </c>
+      <c r="AK43" s="177" t="s">
+        <v>229</v>
+      </c>
+      <c r="AL43" s="177" t="s">
+        <v>283</v>
+      </c>
+      <c r="AM43" s="177" t="s">
+        <v>286</v>
+      </c>
+      <c r="AN43" s="178" t="s">
+        <v>220</v>
+      </c>
+      <c r="AO43" s="179"/>
+      <c r="AP43" s="180"/>
+      <c r="AQ43" s="178" t="s">
+        <v>221</v>
+      </c>
+      <c r="AR43" s="179"/>
+      <c r="AS43" s="180"/>
+      <c r="AT43" s="162" t="s">
+        <v>214</v>
+      </c>
+      <c r="AU43" s="163"/>
+      <c r="AV43" s="164" t="s">
+        <v>222</v>
+      </c>
+      <c r="AW43" s="165"/>
+      <c r="AX43" s="164" t="s">
+        <v>223</v>
+      </c>
+      <c r="AY43" s="165"/>
+    </row>
+    <row r="44" spans="1:51">
+      <c r="D44" s="128"/>
+      <c r="E44" s="130"/>
+      <c r="F44" s="129"/>
+      <c r="G44" s="137"/>
+      <c r="H44" s="138"/>
+      <c r="I44" s="138"/>
+      <c r="J44" s="138"/>
+      <c r="K44" s="139"/>
+      <c r="L44" s="167"/>
+      <c r="M44" s="168"/>
+      <c r="N44" s="157"/>
+      <c r="O44" s="144"/>
+      <c r="P44" s="144"/>
+      <c r="Q44" s="144"/>
+      <c r="R44" s="144"/>
+      <c r="S44" s="144"/>
+      <c r="T44" s="144"/>
+      <c r="U44" s="144"/>
+      <c r="V44" s="144"/>
+      <c r="W44" s="144"/>
+      <c r="X44" s="144"/>
+      <c r="Y44" s="144"/>
+      <c r="Z44" s="181"/>
+      <c r="AA44" s="181"/>
+      <c r="AB44" s="181"/>
+      <c r="AC44" s="181"/>
+      <c r="AD44" s="181"/>
+      <c r="AE44" s="182"/>
+      <c r="AF44" s="182"/>
+      <c r="AG44" s="182"/>
+      <c r="AH44" s="182"/>
+      <c r="AI44" s="182"/>
+      <c r="AJ44" s="182"/>
+      <c r="AK44" s="183"/>
+      <c r="AL44" s="183"/>
+      <c r="AM44" s="183"/>
+      <c r="AN44" s="184"/>
+      <c r="AO44" s="185"/>
+      <c r="AP44" s="186"/>
+      <c r="AQ44" s="184"/>
+      <c r="AR44" s="185"/>
+      <c r="AS44" s="186"/>
+      <c r="AT44" s="147"/>
+      <c r="AU44" s="147"/>
+      <c r="AV44" s="148"/>
+      <c r="AW44" s="148"/>
+      <c r="AX44" s="148"/>
+      <c r="AY44" s="148"/>
+    </row>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="57">
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="AV43:AW43"/>
+    <mergeCell ref="AX43:AY43"/>
+    <mergeCell ref="AK42:AS42"/>
+    <mergeCell ref="AT42:AY42"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="L42:N42"/>
+    <mergeCell ref="O42:AD42"/>
+    <mergeCell ref="AE43:AF43"/>
+    <mergeCell ref="AE42:AJ42"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="AT44:AU44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:AY44"/>
+    <mergeCell ref="AN43:AP43"/>
+    <mergeCell ref="AN44:AP44"/>
+    <mergeCell ref="AQ43:AS43"/>
+    <mergeCell ref="AQ44:AS44"/>
+    <mergeCell ref="AT43:AU43"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="G43:K43"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="AD35:AE35"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="AN35:AO35"/>
     <mergeCell ref="AL35:AM35"/>
@@ -52383,25 +53114,6 @@
     <mergeCell ref="AF34:AG34"/>
     <mergeCell ref="AF35:AG35"/>
     <mergeCell ref="AH35:AI35"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="AD35:AE35"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="J18:K18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -52638,7 +53350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B279FE6-9E53-40E0-8700-C52FFFC93FCF}">
   <dimension ref="A1:AF403"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -52842,14 +53554,14 @@
       <c r="B10" s="85"/>
       <c r="C10" s="86"/>
       <c r="D10" s="86"/>
-      <c r="E10" s="132" t="s">
+      <c r="E10" s="123" t="s">
         <v>206</v>
       </c>
       <c r="F10" s="69"/>
       <c r="G10" s="87" t="s">
         <v>199</v>
       </c>
-      <c r="H10" s="122"/>
+      <c r="H10" s="113"/>
       <c r="I10" s="87" t="s">
         <v>26</v>
       </c>
@@ -52865,7 +53577,7 @@
       <c r="G11" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="123"/>
+      <c r="H11" s="114"/>
       <c r="I11" s="89" t="s">
         <v>26</v>
       </c>
@@ -52881,7 +53593,7 @@
       <c r="G12" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="H12" s="124"/>
+      <c r="H12" s="115"/>
       <c r="I12" s="91" t="s">
         <v>26</v>
       </c>
@@ -52906,14 +53618,14 @@
       <c r="B14" s="96"/>
       <c r="C14" s="97"/>
       <c r="D14" s="97"/>
-      <c r="E14" s="131" t="s">
+      <c r="E14" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F14" s="69"/>
-      <c r="G14" s="125" t="s">
+      <c r="G14" s="116" t="s">
         <v>239</v>
       </c>
-      <c r="H14" s="122" t="s">
+      <c r="H14" s="113" t="s">
         <v>246</v>
       </c>
       <c r="I14" s="87" t="s">
@@ -52926,14 +53638,14 @@
       <c r="B15" s="96"/>
       <c r="C15" s="97"/>
       <c r="D15" s="97"/>
-      <c r="E15" s="131" t="s">
+      <c r="E15" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F15" s="72"/>
-      <c r="G15" s="126" t="s">
+      <c r="G15" s="117" t="s">
         <v>240</v>
       </c>
-      <c r="H15" s="123" t="s">
+      <c r="H15" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I15" s="89" t="s">
@@ -52946,14 +53658,14 @@
       <c r="B16" s="96"/>
       <c r="C16" s="97"/>
       <c r="D16" s="97"/>
-      <c r="E16" s="131" t="s">
+      <c r="E16" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F16" s="72"/>
-      <c r="G16" s="126" t="s">
+      <c r="G16" s="117" t="s">
         <v>241</v>
       </c>
-      <c r="H16" s="123" t="s">
+      <c r="H16" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I16" s="89" t="s">
@@ -52966,14 +53678,14 @@
       <c r="B17" s="96"/>
       <c r="C17" s="97"/>
       <c r="D17" s="97"/>
-      <c r="E17" s="131" t="s">
+      <c r="E17" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F17" s="99"/>
-      <c r="G17" s="126" t="s">
+      <c r="G17" s="117" t="s">
         <v>242</v>
       </c>
-      <c r="H17" s="123" t="s">
+      <c r="H17" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I17" s="89" t="s">
@@ -52986,14 +53698,14 @@
       <c r="B18" s="96"/>
       <c r="C18" s="97"/>
       <c r="D18" s="97"/>
-      <c r="E18" s="131" t="s">
+      <c r="E18" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F18" s="99"/>
-      <c r="G18" s="126" t="s">
+      <c r="G18" s="117" t="s">
         <v>238</v>
       </c>
-      <c r="H18" s="123" t="s">
+      <c r="H18" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I18" s="89" t="s">
@@ -53006,14 +53718,14 @@
       <c r="B19" s="96"/>
       <c r="C19" s="97"/>
       <c r="D19" s="97"/>
-      <c r="E19" s="131" t="s">
+      <c r="E19" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F19" s="99"/>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="123" t="s">
+      <c r="H19" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I19" s="89" t="s">
@@ -53026,14 +53738,14 @@
       <c r="B20" s="96"/>
       <c r="C20" s="97"/>
       <c r="D20" s="97"/>
-      <c r="E20" s="131" t="s">
+      <c r="E20" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F20" s="99"/>
-      <c r="G20" s="126" t="s">
+      <c r="G20" s="117" t="s">
         <v>243</v>
       </c>
-      <c r="H20" s="123" t="s">
+      <c r="H20" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I20" s="89" t="s">
@@ -53051,7 +53763,7 @@
       <c r="G21" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="H21" s="124"/>
+      <c r="H21" s="115"/>
       <c r="I21" s="91" t="s">
         <v>26</v>
       </c>
@@ -53076,14 +53788,14 @@
       <c r="B23" s="96"/>
       <c r="C23" s="97"/>
       <c r="D23" s="97"/>
-      <c r="E23" s="131" t="s">
+      <c r="E23" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F23" s="69"/>
       <c r="G23" s="87" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="122" t="s">
+      <c r="H23" s="113" t="s">
         <v>244</v>
       </c>
       <c r="I23" s="87" t="s">
@@ -53096,14 +53808,14 @@
       <c r="B24" s="96"/>
       <c r="C24" s="97"/>
       <c r="D24" s="97"/>
-      <c r="E24" s="131" t="s">
+      <c r="E24" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F24" s="72"/>
       <c r="G24" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="H24" s="123" t="s">
+      <c r="H24" s="114" t="s">
         <v>244</v>
       </c>
       <c r="I24" s="89" t="s">
@@ -53116,14 +53828,14 @@
       <c r="B25" s="96"/>
       <c r="C25" s="97"/>
       <c r="D25" s="97"/>
-      <c r="E25" s="131" t="s">
+      <c r="E25" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F25" s="72"/>
       <c r="G25" s="89" t="s">
         <v>245</v>
       </c>
-      <c r="H25" s="123" t="s">
+      <c r="H25" s="114" t="s">
         <v>244</v>
       </c>
       <c r="I25" s="89" t="s">
@@ -53136,14 +53848,14 @@
       <c r="B26" s="96"/>
       <c r="C26" s="97"/>
       <c r="D26" s="97"/>
-      <c r="E26" s="131" t="s">
+      <c r="E26" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F26" s="74"/>
       <c r="G26" s="91" t="s">
         <v>205</v>
       </c>
-      <c r="H26" s="124" t="s">
+      <c r="H26" s="115" t="s">
         <v>244</v>
       </c>
       <c r="I26" s="91" t="s">
@@ -53175,7 +53887,7 @@
       <c r="G28" s="87" t="s">
         <v>247</v>
       </c>
-      <c r="H28" s="122" t="s">
+      <c r="H28" s="113" t="s">
         <v>246</v>
       </c>
       <c r="I28" s="87"/>
@@ -53191,7 +53903,7 @@
       <c r="G29" s="89" t="s">
         <v>248</v>
       </c>
-      <c r="H29" s="123" t="s">
+      <c r="H29" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I29" s="89"/>
@@ -53207,7 +53919,7 @@
       <c r="G30" s="89" t="s">
         <v>249</v>
       </c>
-      <c r="H30" s="123" t="s">
+      <c r="H30" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I30" s="89"/>
@@ -53223,7 +53935,7 @@
       <c r="G31" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="H31" s="123" t="s">
+      <c r="H31" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I31" s="89"/>
@@ -53234,14 +53946,14 @@
       <c r="B32" s="96"/>
       <c r="C32" s="97"/>
       <c r="D32" s="97"/>
-      <c r="E32" s="131" t="s">
+      <c r="E32" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F32" s="76"/>
       <c r="G32" s="89" t="s">
         <v>256</v>
       </c>
-      <c r="H32" s="123" t="s">
+      <c r="H32" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I32" s="89"/>
@@ -53252,14 +53964,14 @@
       <c r="B33" s="96"/>
       <c r="C33" s="97"/>
       <c r="D33" s="97"/>
-      <c r="E33" s="131" t="s">
+      <c r="E33" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F33" s="76"/>
       <c r="G33" s="89" t="s">
         <v>250</v>
       </c>
-      <c r="H33" s="123" t="s">
+      <c r="H33" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I33" s="89"/>
@@ -53270,14 +53982,14 @@
       <c r="B34" s="96"/>
       <c r="C34" s="97"/>
       <c r="D34" s="97"/>
-      <c r="E34" s="131" t="s">
+      <c r="E34" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F34" s="76"/>
       <c r="G34" s="89" t="s">
         <v>251</v>
       </c>
-      <c r="H34" s="123" t="s">
+      <c r="H34" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I34" s="89"/>
@@ -53293,7 +54005,7 @@
       <c r="G35" s="89" t="s">
         <v>252</v>
       </c>
-      <c r="H35" s="123" t="s">
+      <c r="H35" s="114" t="s">
         <v>244</v>
       </c>
       <c r="I35" s="89"/>
@@ -53309,7 +54021,7 @@
       <c r="G36" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="H36" s="123" t="s">
+      <c r="H36" s="114" t="s">
         <v>246</v>
       </c>
       <c r="I36" s="89"/>
@@ -53320,66 +54032,66 @@
       <c r="B37" s="96"/>
       <c r="C37" s="97"/>
       <c r="D37" s="97"/>
-      <c r="E37" s="131" t="s">
+      <c r="E37" s="122" t="s">
         <v>206</v>
       </c>
-      <c r="F37" s="127"/>
-      <c r="G37" s="128" t="s">
+      <c r="F37" s="118"/>
+      <c r="G37" s="119" t="s">
         <v>253</v>
       </c>
-      <c r="H37" s="129" t="s">
+      <c r="H37" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="I37" s="128"/>
-      <c r="J37" s="128"/>
-      <c r="K37" s="130"/>
+      <c r="I37" s="119"/>
+      <c r="J37" s="119"/>
+      <c r="K37" s="121"/>
     </row>
     <row r="38" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B38" s="96"/>
       <c r="C38" s="97"/>
       <c r="D38" s="97"/>
-      <c r="E38" s="131"/>
-      <c r="F38" s="127"/>
-      <c r="G38" s="128" t="s">
+      <c r="E38" s="122"/>
+      <c r="F38" s="118"/>
+      <c r="G38" s="119" t="s">
         <v>254</v>
       </c>
-      <c r="H38" s="129" t="s">
+      <c r="H38" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="I38" s="128"/>
-      <c r="J38" s="128"/>
-      <c r="K38" s="130"/>
+      <c r="I38" s="119"/>
+      <c r="J38" s="119"/>
+      <c r="K38" s="121"/>
     </row>
     <row r="39" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B39" s="96"/>
       <c r="C39" s="97"/>
       <c r="D39" s="97"/>
-      <c r="E39" s="131" t="s">
+      <c r="E39" s="122" t="s">
         <v>206</v>
       </c>
-      <c r="F39" s="127"/>
-      <c r="G39" s="128" t="s">
+      <c r="F39" s="118"/>
+      <c r="G39" s="119" t="s">
         <v>257</v>
       </c>
-      <c r="H39" s="123" t="s">
+      <c r="H39" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="I39" s="128"/>
-      <c r="J39" s="128"/>
-      <c r="K39" s="130"/>
+      <c r="I39" s="119"/>
+      <c r="J39" s="119"/>
+      <c r="K39" s="121"/>
     </row>
     <row r="40" spans="2:11" s="62" customFormat="1" ht="26" customHeight="1">
       <c r="B40" s="96"/>
       <c r="C40" s="97"/>
       <c r="D40" s="97"/>
-      <c r="E40" s="131" t="s">
+      <c r="E40" s="122" t="s">
         <v>206</v>
       </c>
       <c r="F40" s="71"/>
       <c r="G40" s="91" t="s">
         <v>258</v>
       </c>
-      <c r="H40" s="123" t="s">
+      <c r="H40" s="114" t="s">
         <v>25</v>
       </c>
       <c r="I40" s="91"/>
@@ -53423,7 +54135,7 @@
       <c r="G43" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="H43" s="122"/>
+      <c r="H43" s="113"/>
       <c r="I43" s="87"/>
       <c r="J43" s="87"/>
       <c r="K43" s="88"/>
@@ -53437,7 +54149,7 @@
       <c r="G44" s="89" t="s">
         <v>22</v>
       </c>
-      <c r="H44" s="123"/>
+      <c r="H44" s="114"/>
       <c r="I44" s="89"/>
       <c r="J44" s="89"/>
       <c r="K44" s="90"/>
@@ -53451,7 +54163,7 @@
       <c r="G45" s="89" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="123"/>
+      <c r="H45" s="114"/>
       <c r="I45" s="89"/>
       <c r="J45" s="89"/>
       <c r="K45" s="90"/>
@@ -53463,7 +54175,7 @@
       <c r="E46" s="97"/>
       <c r="F46" s="99"/>
       <c r="G46" s="89"/>
-      <c r="H46" s="123"/>
+      <c r="H46" s="114"/>
       <c r="I46" s="89"/>
       <c r="J46" s="89"/>
       <c r="K46" s="90"/>
@@ -53475,7 +54187,7 @@
       <c r="E47" s="97"/>
       <c r="F47" s="99"/>
       <c r="G47" s="89"/>
-      <c r="H47" s="123"/>
+      <c r="H47" s="114"/>
       <c r="I47" s="89"/>
       <c r="J47" s="89"/>
       <c r="K47" s="90"/>
@@ -53487,7 +54199,7 @@
       <c r="E48" s="97"/>
       <c r="F48" s="99"/>
       <c r="G48" s="89"/>
-      <c r="H48" s="123"/>
+      <c r="H48" s="114"/>
       <c r="I48" s="89"/>
       <c r="J48" s="89"/>
       <c r="K48" s="90"/>
@@ -53499,7 +54211,7 @@
       <c r="E49" s="97"/>
       <c r="F49" s="99"/>
       <c r="G49" s="89"/>
-      <c r="H49" s="123"/>
+      <c r="H49" s="114"/>
       <c r="I49" s="89"/>
       <c r="J49" s="89"/>
       <c r="K49" s="90"/>
@@ -53511,7 +54223,7 @@
       <c r="E50" s="97"/>
       <c r="F50" s="99"/>
       <c r="G50" s="89"/>
-      <c r="H50" s="123"/>
+      <c r="H50" s="114"/>
       <c r="I50" s="89"/>
       <c r="J50" s="89"/>
       <c r="K50" s="90"/>
@@ -53523,7 +54235,7 @@
       <c r="E51" s="83"/>
       <c r="F51" s="108"/>
       <c r="G51" s="91"/>
-      <c r="H51" s="124"/>
+      <c r="H51" s="115"/>
       <c r="I51" s="91"/>
       <c r="J51" s="91"/>
       <c r="K51" s="92"/>

</xml_diff>

<commit_message>
Added data out property
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6142F17-87D2-654A-AA41-0630D2ACFB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3771BA26-A0C8-A747-9F90-62AF68AA365E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-23040" windowWidth="40960" windowHeight="23040" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="0" yWindow="-22540" windowWidth="40960" windowHeight="22540" tabRatio="710" activeTab="4" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -3074,7 +3074,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="187">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3399,37 +3399,6 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3445,13 +3414,6 @@
     <xf numFmtId="0" fontId="6" fillId="24" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3467,85 +3429,13 @@
     <xf numFmtId="0" fontId="38" fillId="24" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="22" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="24" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="26" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="26" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="24" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="23" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3557,6 +3447,76 @@
     <xf numFmtId="0" fontId="41" fillId="24" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="24" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="25" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="26" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="26" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="41" fillId="24" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3564,6 +3524,52 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="41" fillId="24" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="18" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="23" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -46119,27 +46125,27 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="124"/>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
+      <c r="F5" s="140"/>
+      <c r="G5" s="140"/>
+      <c r="H5" s="140"/>
       <c r="I5" s="23"/>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="125"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="141"/>
+      <c r="N5" s="141"/>
+      <c r="O5" s="141"/>
+      <c r="P5" s="141"/>
       <c r="Q5" s="24"/>
       <c r="R5" s="24"/>
       <c r="S5" s="24"/>
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
       <c r="V5" s="23"/>
-      <c r="W5" s="125"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="125"/>
-      <c r="Z5" s="125"/>
+      <c r="W5" s="141"/>
+      <c r="X5" s="141"/>
+      <c r="Y5" s="141"/>
+      <c r="Z5" s="141"/>
       <c r="AA5" s="5"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -49729,27 +49735,27 @@
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
+      <c r="F5" s="142"/>
+      <c r="G5" s="142"/>
+      <c r="H5" s="142"/>
       <c r="I5" s="49"/>
-      <c r="J5" s="127"/>
-      <c r="K5" s="127"/>
-      <c r="L5" s="127"/>
-      <c r="M5" s="127"/>
-      <c r="N5" s="127"/>
-      <c r="O5" s="127"/>
-      <c r="P5" s="127"/>
+      <c r="J5" s="143"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="143"/>
+      <c r="M5" s="143"/>
+      <c r="N5" s="143"/>
+      <c r="O5" s="143"/>
+      <c r="P5" s="143"/>
       <c r="Q5" s="50"/>
       <c r="R5" s="50"/>
       <c r="S5" s="50"/>
       <c r="T5" s="50"/>
       <c r="U5" s="50"/>
       <c r="V5" s="49"/>
-      <c r="W5" s="127"/>
-      <c r="X5" s="127"/>
-      <c r="Y5" s="127"/>
-      <c r="Z5" s="127"/>
+      <c r="W5" s="143"/>
+      <c r="X5" s="143"/>
+      <c r="Y5" s="143"/>
+      <c r="Z5" s="143"/>
       <c r="AA5" s="42"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -52362,7 +52368,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10B830-2EC7-4D7B-A783-4C17DFC99A4F}">
-  <dimension ref="A1:AY44"/>
+  <dimension ref="A1:BA44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
       <pane xSplit="11" topLeftCell="L1" activePane="topRight" state="frozen"/>
@@ -52571,17 +52577,17 @@
       <c r="D17" s="109" t="s">
         <v>202</v>
       </c>
-      <c r="E17" s="131" t="s">
+      <c r="E17" s="176" t="s">
         <v>201</v>
       </c>
-      <c r="F17" s="131"/>
-      <c r="G17" s="131"/>
-      <c r="H17" s="131"/>
-      <c r="I17" s="131"/>
-      <c r="J17" s="131" t="s">
+      <c r="F17" s="176"/>
+      <c r="G17" s="176"/>
+      <c r="H17" s="176"/>
+      <c r="I17" s="176"/>
+      <c r="J17" s="176" t="s">
         <v>203</v>
       </c>
-      <c r="K17" s="131"/>
+      <c r="K17" s="176"/>
       <c r="L17" s="109" t="s">
         <v>204</v>
       </c>
@@ -52589,15 +52595,15 @@
     </row>
     <row r="18" spans="3:21">
       <c r="D18" s="110"/>
-      <c r="E18" s="128"/>
-      <c r="F18" s="130"/>
-      <c r="G18" s="130"/>
-      <c r="H18" s="130"/>
-      <c r="I18" s="129"/>
-      <c r="J18" s="128"/>
-      <c r="K18" s="129"/>
-      <c r="L18" s="128"/>
-      <c r="M18" s="129"/>
+      <c r="E18" s="157"/>
+      <c r="F18" s="158"/>
+      <c r="G18" s="158"/>
+      <c r="H18" s="158"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="157"/>
+      <c r="K18" s="159"/>
+      <c r="L18" s="157"/>
+      <c r="M18" s="159"/>
     </row>
     <row r="22" spans="3:21" ht="28">
       <c r="C22"/>
@@ -52614,20 +52620,20 @@
       <c r="D24" s="78"/>
     </row>
     <row r="25" spans="3:21">
-      <c r="D25" s="131" t="s">
+      <c r="D25" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="131"/>
-      <c r="F25" s="131"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="176"/>
       <c r="G25" s="109" t="s">
         <v>209</v>
       </c>
-      <c r="H25" s="131" t="s">
+      <c r="H25" s="176" t="s">
         <v>201</v>
       </c>
-      <c r="I25" s="131"/>
-      <c r="J25" s="131"/>
-      <c r="K25" s="131"/>
+      <c r="I25" s="176"/>
+      <c r="J25" s="176"/>
+      <c r="K25" s="176"/>
       <c r="L25" s="109" t="s">
         <v>210</v>
       </c>
@@ -52637,14 +52643,14 @@
       <c r="N25" s="109" t="s">
         <v>212</v>
       </c>
-      <c r="O25" s="131" t="s">
+      <c r="O25" s="176" t="s">
         <v>213</v>
       </c>
-      <c r="P25" s="131"/>
-      <c r="Q25" s="131" t="s">
+      <c r="P25" s="176"/>
+      <c r="Q25" s="176" t="s">
         <v>216</v>
       </c>
-      <c r="R25" s="131"/>
+      <c r="R25" s="176"/>
       <c r="S25" s="109" t="s">
         <v>214</v>
       </c>
@@ -52654,24 +52660,24 @@
       <c r="U25" s="110"/>
     </row>
     <row r="26" spans="3:21">
-      <c r="D26" s="128"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="129"/>
+      <c r="D26" s="157"/>
+      <c r="E26" s="158"/>
+      <c r="F26" s="159"/>
       <c r="G26" s="111"/>
-      <c r="H26" s="128"/>
-      <c r="I26" s="130"/>
-      <c r="J26" s="130"/>
-      <c r="K26" s="129"/>
+      <c r="H26" s="157"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="159"/>
       <c r="L26" s="110"/>
       <c r="M26" s="112"/>
       <c r="N26" s="112"/>
-      <c r="O26" s="128"/>
-      <c r="P26" s="129"/>
-      <c r="Q26" s="128"/>
-      <c r="R26" s="129"/>
+      <c r="O26" s="157"/>
+      <c r="P26" s="159"/>
+      <c r="Q26" s="157"/>
+      <c r="R26" s="159"/>
       <c r="S26" s="110"/>
-      <c r="T26" s="128"/>
-      <c r="U26" s="129"/>
+      <c r="T26" s="157"/>
+      <c r="U26" s="159"/>
     </row>
     <row r="27" spans="3:21" ht="17" customHeight="1"/>
     <row r="30" spans="3:21" ht="28">
@@ -52688,416 +52694,385 @@
       <c r="C32" s="77"/>
       <c r="D32" s="78"/>
     </row>
-    <row r="33" spans="1:51" ht="16" customHeight="1">
+    <row r="33" spans="1:53" ht="16" customHeight="1">
       <c r="C33" s="77"/>
       <c r="D33" s="78"/>
     </row>
-    <row r="34" spans="1:51" s="79" customFormat="1" ht="68">
-      <c r="D34" s="132" t="s">
+    <row r="34" spans="1:53" s="79" customFormat="1" ht="68">
+      <c r="D34" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="E34" s="132"/>
-      <c r="F34" s="132"/>
-      <c r="G34" s="132" t="s">
+      <c r="E34" s="173"/>
+      <c r="F34" s="173"/>
+      <c r="G34" s="173" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="132"/>
-      <c r="I34" s="132"/>
-      <c r="J34" s="132"/>
-      <c r="K34" s="136"/>
-      <c r="L34" s="149" t="s">
+      <c r="H34" s="173"/>
+      <c r="I34" s="173"/>
+      <c r="J34" s="173"/>
+      <c r="K34" s="174"/>
+      <c r="L34" s="129" t="s">
         <v>219</v>
       </c>
-      <c r="M34" s="150" t="s">
+      <c r="M34" s="130" t="s">
         <v>220</v>
       </c>
-      <c r="N34" s="150" t="s">
+      <c r="N34" s="130" t="s">
         <v>221</v>
       </c>
-      <c r="O34" s="151" t="s">
+      <c r="O34" s="131" t="s">
         <v>224</v>
       </c>
-      <c r="P34" s="150" t="s">
+      <c r="P34" s="130" t="s">
         <v>225</v>
       </c>
-      <c r="Q34" s="152" t="s">
+      <c r="Q34" s="179" t="s">
         <v>218</v>
       </c>
-      <c r="R34" s="152"/>
-      <c r="S34" s="150" t="s">
+      <c r="R34" s="179"/>
+      <c r="S34" s="130" t="s">
         <v>226</v>
       </c>
-      <c r="T34" s="150" t="s">
+      <c r="T34" s="130" t="s">
         <v>232</v>
       </c>
-      <c r="U34" s="150" t="s">
+      <c r="U34" s="130" t="s">
         <v>231</v>
       </c>
-      <c r="V34" s="153" t="s">
+      <c r="V34" s="133" t="s">
         <v>227</v>
       </c>
-      <c r="W34" s="153" t="s">
+      <c r="W34" s="133" t="s">
         <v>229</v>
       </c>
-      <c r="X34" s="153" t="s">
+      <c r="X34" s="133" t="s">
         <v>230</v>
       </c>
-      <c r="Y34" s="153" t="s">
+      <c r="Y34" s="133" t="s">
         <v>228</v>
       </c>
-      <c r="Z34" s="154" t="s">
+      <c r="Z34" s="177" t="s">
         <v>233</v>
       </c>
-      <c r="AA34" s="154"/>
-      <c r="AB34" s="154" t="s">
+      <c r="AA34" s="177"/>
+      <c r="AB34" s="177" t="s">
         <v>234</v>
       </c>
-      <c r="AC34" s="154"/>
-      <c r="AD34" s="154" t="s">
+      <c r="AC34" s="177"/>
+      <c r="AD34" s="177" t="s">
         <v>235</v>
       </c>
-      <c r="AE34" s="154"/>
-      <c r="AF34" s="154" t="s">
+      <c r="AE34" s="177"/>
+      <c r="AF34" s="177" t="s">
         <v>236</v>
       </c>
-      <c r="AG34" s="154"/>
-      <c r="AH34" s="154" t="s">
+      <c r="AG34" s="177"/>
+      <c r="AH34" s="177" t="s">
         <v>237</v>
       </c>
-      <c r="AI34" s="154"/>
-      <c r="AJ34" s="155" t="s">
+      <c r="AI34" s="177"/>
+      <c r="AJ34" s="184" t="s">
         <v>214</v>
       </c>
-      <c r="AK34" s="155"/>
-      <c r="AL34" s="156" t="s">
+      <c r="AK34" s="184"/>
+      <c r="AL34" s="183" t="s">
         <v>222</v>
       </c>
-      <c r="AM34" s="156"/>
-      <c r="AN34" s="156" t="s">
+      <c r="AM34" s="183"/>
+      <c r="AN34" s="183" t="s">
         <v>223</v>
       </c>
-      <c r="AO34" s="156"/>
-    </row>
-    <row r="35" spans="1:51">
-      <c r="D35" s="128"/>
-      <c r="E35" s="130"/>
-      <c r="F35" s="129"/>
-      <c r="G35" s="133"/>
-      <c r="H35" s="134"/>
-      <c r="I35" s="134"/>
-      <c r="J35" s="134"/>
-      <c r="K35" s="135"/>
-      <c r="L35" s="141"/>
-      <c r="M35" s="142"/>
-      <c r="N35" s="142"/>
-      <c r="O35" s="143"/>
-      <c r="P35" s="142"/>
-      <c r="Q35" s="144"/>
-      <c r="R35" s="144"/>
-      <c r="S35" s="142"/>
-      <c r="T35" s="142"/>
-      <c r="U35" s="142"/>
-      <c r="V35" s="145"/>
-      <c r="W35" s="145"/>
-      <c r="X35" s="145"/>
-      <c r="Y35" s="145"/>
-      <c r="Z35" s="146"/>
-      <c r="AA35" s="146"/>
-      <c r="AB35" s="146"/>
-      <c r="AC35" s="146"/>
-      <c r="AD35" s="146"/>
-      <c r="AE35" s="146"/>
-      <c r="AF35" s="146"/>
-      <c r="AG35" s="146"/>
-      <c r="AH35" s="146"/>
-      <c r="AI35" s="146"/>
-      <c r="AJ35" s="147"/>
-      <c r="AK35" s="147"/>
-      <c r="AL35" s="148"/>
-      <c r="AM35" s="148"/>
-      <c r="AN35" s="148"/>
-      <c r="AO35" s="148"/>
-    </row>
-    <row r="39" spans="1:51" ht="28">
+      <c r="AO34" s="183"/>
+    </row>
+    <row r="35" spans="1:53">
+      <c r="D35" s="157"/>
+      <c r="E35" s="158"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="180"/>
+      <c r="H35" s="181"/>
+      <c r="I35" s="181"/>
+      <c r="J35" s="181"/>
+      <c r="K35" s="182"/>
+      <c r="L35" s="124"/>
+      <c r="M35" s="125"/>
+      <c r="N35" s="125"/>
+      <c r="O35" s="126"/>
+      <c r="P35" s="125"/>
+      <c r="Q35" s="127"/>
+      <c r="R35" s="127"/>
+      <c r="S35" s="125"/>
+      <c r="T35" s="125"/>
+      <c r="U35" s="125"/>
+      <c r="V35" s="128"/>
+      <c r="W35" s="128"/>
+      <c r="X35" s="128"/>
+      <c r="Y35" s="128"/>
+      <c r="Z35" s="178"/>
+      <c r="AA35" s="178"/>
+      <c r="AB35" s="178"/>
+      <c r="AC35" s="178"/>
+      <c r="AD35" s="178"/>
+      <c r="AE35" s="178"/>
+      <c r="AF35" s="178"/>
+      <c r="AG35" s="178"/>
+      <c r="AH35" s="178"/>
+      <c r="AI35" s="178"/>
+      <c r="AJ35" s="163"/>
+      <c r="AK35" s="163"/>
+      <c r="AL35" s="164"/>
+      <c r="AM35" s="164"/>
+      <c r="AN35" s="164"/>
+      <c r="AO35" s="164"/>
+    </row>
+    <row r="39" spans="1:53" ht="28">
       <c r="C39"/>
       <c r="D39" s="78" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="40" spans="1:51" ht="28">
+    <row r="40" spans="1:53" ht="28">
       <c r="C40" s="77"/>
       <c r="D40" s="78"/>
     </row>
-    <row r="41" spans="1:51" ht="28">
+    <row r="41" spans="1:53" ht="28">
       <c r="C41" s="77"/>
       <c r="D41" s="78"/>
     </row>
-    <row r="42" spans="1:51" ht="28">
+    <row r="42" spans="1:53" ht="28">
       <c r="C42" s="77"/>
       <c r="D42" s="78"/>
-      <c r="L42" s="158" t="s">
+      <c r="L42" s="152" t="s">
         <v>262</v>
       </c>
-      <c r="M42" s="158"/>
-      <c r="N42" s="158"/>
-      <c r="O42" s="159" t="s">
+      <c r="M42" s="152"/>
+      <c r="N42" s="152"/>
+      <c r="O42" s="152"/>
+      <c r="P42" s="153" t="s">
         <v>118</v>
       </c>
-      <c r="P42" s="159"/>
-      <c r="Q42" s="159"/>
-      <c r="R42" s="159"/>
-      <c r="S42" s="159"/>
-      <c r="T42" s="159"/>
-      <c r="U42" s="159"/>
-      <c r="V42" s="159"/>
-      <c r="W42" s="159"/>
-      <c r="X42" s="159"/>
-      <c r="Y42" s="159"/>
-      <c r="Z42" s="159"/>
-      <c r="AA42" s="159"/>
-      <c r="AB42" s="159"/>
-      <c r="AC42" s="159"/>
-      <c r="AD42" s="159"/>
-      <c r="AE42" s="161" t="s">
+      <c r="Q42" s="153"/>
+      <c r="R42" s="153"/>
+      <c r="S42" s="153"/>
+      <c r="T42" s="153"/>
+      <c r="U42" s="153"/>
+      <c r="V42" s="153"/>
+      <c r="W42" s="153"/>
+      <c r="X42" s="153"/>
+      <c r="Y42" s="153"/>
+      <c r="Z42" s="153"/>
+      <c r="AA42" s="153"/>
+      <c r="AB42" s="153"/>
+      <c r="AC42" s="153"/>
+      <c r="AD42" s="153"/>
+      <c r="AE42" s="153"/>
+      <c r="AF42" s="153"/>
+      <c r="AG42" s="156" t="s">
         <v>282</v>
       </c>
-      <c r="AF42" s="161"/>
-      <c r="AG42" s="161"/>
-      <c r="AH42" s="161"/>
-      <c r="AI42" s="161"/>
-      <c r="AJ42" s="161"/>
-      <c r="AK42" s="160" t="s">
+      <c r="AH42" s="156"/>
+      <c r="AI42" s="156"/>
+      <c r="AJ42" s="156"/>
+      <c r="AK42" s="156"/>
+      <c r="AL42" s="156"/>
+      <c r="AM42" s="148" t="s">
         <v>287</v>
       </c>
-      <c r="AL42" s="160"/>
-      <c r="AM42" s="160"/>
-      <c r="AN42" s="160"/>
-      <c r="AO42" s="160"/>
-      <c r="AP42" s="160"/>
-      <c r="AQ42" s="160"/>
-      <c r="AR42" s="160"/>
-      <c r="AS42" s="160"/>
-      <c r="AT42" s="166" t="s">
+      <c r="AN42" s="148"/>
+      <c r="AO42" s="148"/>
+      <c r="AP42" s="148"/>
+      <c r="AQ42" s="148"/>
+      <c r="AR42" s="148"/>
+      <c r="AS42" s="148"/>
+      <c r="AT42" s="148"/>
+      <c r="AU42" s="148"/>
+      <c r="AV42" s="149" t="s">
         <v>288</v>
       </c>
-      <c r="AU42" s="166"/>
-      <c r="AV42" s="166"/>
-      <c r="AW42" s="166"/>
-      <c r="AX42" s="166"/>
-      <c r="AY42" s="166"/>
-    </row>
-    <row r="43" spans="1:51" ht="153">
+      <c r="AW42" s="149"/>
+      <c r="AX42" s="149"/>
+      <c r="AY42" s="149"/>
+      <c r="AZ42" s="149"/>
+      <c r="BA42" s="149"/>
+    </row>
+    <row r="43" spans="1:53" ht="153">
       <c r="A43" s="79"/>
       <c r="B43" s="79"/>
       <c r="C43" s="79"/>
-      <c r="D43" s="132" t="s">
+      <c r="D43" s="173" t="s">
         <v>2</v>
       </c>
-      <c r="E43" s="132"/>
-      <c r="F43" s="136"/>
-      <c r="G43" s="140" t="s">
+      <c r="E43" s="173"/>
+      <c r="F43" s="174"/>
+      <c r="G43" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="H43" s="140"/>
-      <c r="I43" s="140"/>
-      <c r="J43" s="140"/>
-      <c r="K43" s="140"/>
-      <c r="L43" s="169" t="s">
+      <c r="H43" s="175"/>
+      <c r="I43" s="175"/>
+      <c r="J43" s="175"/>
+      <c r="K43" s="175"/>
+      <c r="L43" s="150" t="s">
         <v>260</v>
       </c>
-      <c r="M43" s="170"/>
-      <c r="N43" s="171" t="s">
+      <c r="M43" s="151"/>
+      <c r="N43" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="O43" s="172" t="s">
+      <c r="O43" s="151"/>
+      <c r="P43" s="131" t="s">
         <v>263</v>
       </c>
-      <c r="P43" s="172" t="s">
+      <c r="Q43" s="185" t="s">
         <v>264</v>
       </c>
-      <c r="Q43" s="172" t="s">
+      <c r="R43" s="186"/>
+      <c r="S43" s="132" t="s">
         <v>265</v>
       </c>
-      <c r="R43" s="172" t="s">
+      <c r="T43" s="132" t="s">
         <v>266</v>
       </c>
-      <c r="S43" s="172" t="s">
+      <c r="U43" s="132" t="s">
         <v>267</v>
       </c>
-      <c r="T43" s="172" t="s">
+      <c r="V43" s="132" t="s">
         <v>268</v>
       </c>
-      <c r="U43" s="172" t="s">
+      <c r="W43" s="132" t="s">
         <v>269</v>
       </c>
-      <c r="V43" s="172" t="s">
+      <c r="X43" s="132" t="s">
         <v>270</v>
       </c>
-      <c r="W43" s="172" t="s">
+      <c r="Y43" s="132" t="s">
         <v>271</v>
       </c>
-      <c r="X43" s="172" t="s">
+      <c r="Z43" s="132" t="s">
         <v>272</v>
       </c>
-      <c r="Y43" s="172" t="s">
+      <c r="AA43" s="132" t="s">
         <v>273</v>
       </c>
-      <c r="Z43" s="173" t="s">
+      <c r="AB43" s="134" t="s">
         <v>274</v>
       </c>
-      <c r="AA43" s="173" t="s">
+      <c r="AC43" s="134" t="s">
         <v>275</v>
       </c>
-      <c r="AB43" s="173" t="s">
+      <c r="AD43" s="134" t="s">
         <v>276</v>
       </c>
-      <c r="AC43" s="173" t="s">
+      <c r="AE43" s="134" t="s">
         <v>277</v>
       </c>
-      <c r="AD43" s="173" t="s">
+      <c r="AF43" s="134" t="s">
         <v>278</v>
       </c>
-      <c r="AE43" s="174" t="s">
+      <c r="AG43" s="154" t="s">
         <v>284</v>
       </c>
-      <c r="AF43" s="175"/>
-      <c r="AG43" s="176" t="s">
+      <c r="AH43" s="155"/>
+      <c r="AI43" s="135" t="s">
         <v>279</v>
       </c>
-      <c r="AH43" s="176" t="s">
+      <c r="AJ43" s="135" t="s">
         <v>280</v>
       </c>
-      <c r="AI43" s="176" t="s">
+      <c r="AK43" s="135" t="s">
         <v>281</v>
       </c>
-      <c r="AJ43" s="176" t="s">
+      <c r="AL43" s="135" t="s">
         <v>285</v>
       </c>
-      <c r="AK43" s="177" t="s">
+      <c r="AM43" s="136" t="s">
         <v>229</v>
       </c>
-      <c r="AL43" s="177" t="s">
+      <c r="AN43" s="136" t="s">
         <v>283</v>
       </c>
-      <c r="AM43" s="177" t="s">
+      <c r="AO43" s="136" t="s">
         <v>286</v>
       </c>
-      <c r="AN43" s="178" t="s">
+      <c r="AP43" s="165" t="s">
         <v>220</v>
       </c>
-      <c r="AO43" s="179"/>
-      <c r="AP43" s="180"/>
-      <c r="AQ43" s="178" t="s">
+      <c r="AQ43" s="166"/>
+      <c r="AR43" s="167"/>
+      <c r="AS43" s="165" t="s">
         <v>221</v>
       </c>
-      <c r="AR43" s="179"/>
-      <c r="AS43" s="180"/>
-      <c r="AT43" s="162" t="s">
+      <c r="AT43" s="166"/>
+      <c r="AU43" s="167"/>
+      <c r="AV43" s="171" t="s">
         <v>214</v>
       </c>
-      <c r="AU43" s="163"/>
-      <c r="AV43" s="164" t="s">
+      <c r="AW43" s="172"/>
+      <c r="AX43" s="146" t="s">
         <v>222</v>
       </c>
-      <c r="AW43" s="165"/>
-      <c r="AX43" s="164" t="s">
+      <c r="AY43" s="147"/>
+      <c r="AZ43" s="146" t="s">
         <v>223</v>
       </c>
-      <c r="AY43" s="165"/>
-    </row>
-    <row r="44" spans="1:51">
-      <c r="D44" s="128"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="129"/>
-      <c r="G44" s="137"/>
-      <c r="H44" s="138"/>
-      <c r="I44" s="138"/>
-      <c r="J44" s="138"/>
-      <c r="K44" s="139"/>
-      <c r="L44" s="167"/>
-      <c r="M44" s="168"/>
-      <c r="N44" s="157"/>
-      <c r="O44" s="144"/>
-      <c r="P44" s="144"/>
-      <c r="Q44" s="144"/>
-      <c r="R44" s="144"/>
-      <c r="S44" s="144"/>
-      <c r="T44" s="144"/>
-      <c r="U44" s="144"/>
-      <c r="V44" s="144"/>
-      <c r="W44" s="144"/>
-      <c r="X44" s="144"/>
-      <c r="Y44" s="144"/>
-      <c r="Z44" s="181"/>
-      <c r="AA44" s="181"/>
-      <c r="AB44" s="181"/>
-      <c r="AC44" s="181"/>
-      <c r="AD44" s="181"/>
-      <c r="AE44" s="182"/>
-      <c r="AF44" s="182"/>
-      <c r="AG44" s="182"/>
-      <c r="AH44" s="182"/>
-      <c r="AI44" s="182"/>
-      <c r="AJ44" s="182"/>
-      <c r="AK44" s="183"/>
-      <c r="AL44" s="183"/>
-      <c r="AM44" s="183"/>
-      <c r="AN44" s="184"/>
-      <c r="AO44" s="185"/>
-      <c r="AP44" s="186"/>
-      <c r="AQ44" s="184"/>
-      <c r="AR44" s="185"/>
-      <c r="AS44" s="186"/>
-      <c r="AT44" s="147"/>
-      <c r="AU44" s="147"/>
-      <c r="AV44" s="148"/>
-      <c r="AW44" s="148"/>
-      <c r="AX44" s="148"/>
-      <c r="AY44" s="148"/>
+      <c r="BA43" s="147"/>
+    </row>
+    <row r="44" spans="1:53">
+      <c r="D44" s="157"/>
+      <c r="E44" s="158"/>
+      <c r="F44" s="159"/>
+      <c r="G44" s="160"/>
+      <c r="H44" s="161"/>
+      <c r="I44" s="161"/>
+      <c r="J44" s="161"/>
+      <c r="K44" s="162"/>
+      <c r="L44" s="144"/>
+      <c r="M44" s="145"/>
+      <c r="N44" s="144"/>
+      <c r="O44" s="145"/>
+      <c r="P44" s="126"/>
+      <c r="Q44" s="187"/>
+      <c r="R44" s="188"/>
+      <c r="S44" s="127"/>
+      <c r="T44" s="127"/>
+      <c r="U44" s="127"/>
+      <c r="V44" s="127"/>
+      <c r="W44" s="127"/>
+      <c r="X44" s="127"/>
+      <c r="Y44" s="127"/>
+      <c r="Z44" s="127"/>
+      <c r="AA44" s="127"/>
+      <c r="AB44" s="137"/>
+      <c r="AC44" s="137"/>
+      <c r="AD44" s="137"/>
+      <c r="AE44" s="137"/>
+      <c r="AF44" s="137"/>
+      <c r="AG44" s="138"/>
+      <c r="AH44" s="138"/>
+      <c r="AI44" s="138"/>
+      <c r="AJ44" s="138"/>
+      <c r="AK44" s="138"/>
+      <c r="AL44" s="138"/>
+      <c r="AM44" s="139"/>
+      <c r="AN44" s="139"/>
+      <c r="AO44" s="139"/>
+      <c r="AP44" s="168"/>
+      <c r="AQ44" s="169"/>
+      <c r="AR44" s="170"/>
+      <c r="AS44" s="168"/>
+      <c r="AT44" s="169"/>
+      <c r="AU44" s="170"/>
+      <c r="AV44" s="163"/>
+      <c r="AW44" s="163"/>
+      <c r="AX44" s="164"/>
+      <c r="AY44" s="164"/>
+      <c r="AZ44" s="164"/>
+      <c r="BA44" s="164"/>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="AV43:AW43"/>
-    <mergeCell ref="AX43:AY43"/>
-    <mergeCell ref="AK42:AS42"/>
-    <mergeCell ref="AT42:AY42"/>
-    <mergeCell ref="L43:M43"/>
-    <mergeCell ref="L42:N42"/>
-    <mergeCell ref="O42:AD42"/>
-    <mergeCell ref="AE43:AF43"/>
-    <mergeCell ref="AE42:AJ42"/>
-    <mergeCell ref="D44:F44"/>
-    <mergeCell ref="G44:K44"/>
-    <mergeCell ref="AT44:AU44"/>
-    <mergeCell ref="AV44:AW44"/>
-    <mergeCell ref="AX44:AY44"/>
-    <mergeCell ref="AN43:AP43"/>
-    <mergeCell ref="AN44:AP44"/>
-    <mergeCell ref="AQ43:AS43"/>
-    <mergeCell ref="AQ44:AS44"/>
-    <mergeCell ref="AT43:AU43"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="G43:K43"/>
-    <mergeCell ref="E17:I17"/>
-    <mergeCell ref="G34:K34"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="D25:F25"/>
-    <mergeCell ref="H25:K25"/>
-    <mergeCell ref="E18:I18"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="AD34:AE34"/>
-    <mergeCell ref="AB34:AC34"/>
-    <mergeCell ref="Z34:AA34"/>
-    <mergeCell ref="Z35:AA35"/>
-    <mergeCell ref="AB35:AC35"/>
-    <mergeCell ref="AD35:AE35"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="D35:F35"/>
-    <mergeCell ref="G35:K35"/>
+  <mergeCells count="61">
+    <mergeCell ref="AG42:AL42"/>
+    <mergeCell ref="AM42:AU42"/>
+    <mergeCell ref="AV42:BA42"/>
+    <mergeCell ref="P42:AF42"/>
     <mergeCell ref="L18:M18"/>
     <mergeCell ref="AN35:AO35"/>
     <mergeCell ref="AL35:AM35"/>
@@ -53114,6 +53089,47 @@
     <mergeCell ref="AF34:AG34"/>
     <mergeCell ref="AF35:AG35"/>
     <mergeCell ref="AH35:AI35"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="D35:F35"/>
+    <mergeCell ref="G35:K35"/>
+    <mergeCell ref="AD34:AE34"/>
+    <mergeCell ref="AB34:AC34"/>
+    <mergeCell ref="Z34:AA34"/>
+    <mergeCell ref="Z35:AA35"/>
+    <mergeCell ref="AB35:AC35"/>
+    <mergeCell ref="AD35:AE35"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="G43:K43"/>
+    <mergeCell ref="E17:I17"/>
+    <mergeCell ref="G34:K34"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="H25:K25"/>
+    <mergeCell ref="E18:I18"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="D44:F44"/>
+    <mergeCell ref="G44:K44"/>
+    <mergeCell ref="AV44:AW44"/>
+    <mergeCell ref="AX44:AY44"/>
+    <mergeCell ref="AZ44:BA44"/>
+    <mergeCell ref="AP44:AR44"/>
+    <mergeCell ref="AS44:AU44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="AX43:AY43"/>
+    <mergeCell ref="AZ43:BA43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="AG43:AH43"/>
+    <mergeCell ref="AP43:AR43"/>
+    <mergeCell ref="AS43:AU43"/>
+    <mergeCell ref="AV43:AW43"/>
+    <mergeCell ref="Q43:R43"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="L42:O42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added phish resistant MFA
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D523BD-187E-F644-866D-B2F7A4520F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D535607E-B816-8541-8315-405BC7E2246E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="5" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
@@ -59,6 +59,7 @@
     <definedName name="HeaderTitle">Home!$E$3</definedName>
     <definedName name="I00001_Workload_Exists">'Identity ☑️'!$E$11:$E$11</definedName>
     <definedName name="I00002_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$E$12</definedName>
+    <definedName name="I00003_GlobalAdminPhishingResistantAuthStrength">'Identity ☑️'!$E$15</definedName>
     <definedName name="ListStatus" localSheetId="2">'Device ✍️'!$G$97:$G$104</definedName>
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
@@ -53440,7 +53441,7 @@
   <dimension ref="A1:AP26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="26" customHeight="1"/>

</xml_diff>

<commit_message>
Added cloud only account
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9C6C05-7F4C-E841-8459-11FC56216313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06FC72D-8964-394E-8D18-145063EB02D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="5" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
@@ -63,6 +63,7 @@
     <definedName name="I00004_BasicMfaUsageInsteadOfAuthStrength">'Identity ☑️'!$E$18</definedName>
     <definedName name="I00005_BasicMfaInUse">'Identity ☑️'!$E$24</definedName>
     <definedName name="I00006_SecureRegistrationOfSecurityInfo">'Identity ☑️'!$E$20</definedName>
+    <definedName name="I00007_CloudOnlyCloudPrivilege">'Identity ☑️'!$E$16</definedName>
     <definedName name="ListStatus" localSheetId="2">'Device ✍️'!$G$97:$G$104</definedName>
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
     <definedName name="Status" localSheetId="2">'Device ✍️'!$AD$3:$AK$3</definedName>
@@ -53408,7 +53409,7 @@
   <dimension ref="A1:AP26"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="26" customHeight="1"/>

</xml_diff>

<commit_message>
Added weak auth check
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049CF9F4-5B22-2641-9F60-2D0C7AE9F0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9172B8-1AD8-2E4A-AD76-8565F4F7BAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="5" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
@@ -59,6 +59,7 @@
     <definedName name="HeaderTitle">Home!$E$3</definedName>
     <definedName name="I00001_R_Workload_Exists">'Identity ☑️'!$C$27:$C$36</definedName>
     <definedName name="I00001_Workload_Exists">'Identity ☑️'!$E$9:$E$9</definedName>
+    <definedName name="I000010_WeakAuthMethods">'Identity ☑️'!$E$21</definedName>
     <definedName name="I00002_R_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$C$40:$C$49</definedName>
     <definedName name="I00002_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$E$10</definedName>
     <definedName name="I00003_GlobalAdminPhishingResistantAuthStrength">'Identity ☑️'!$E$13</definedName>
@@ -54040,7 +54041,7 @@
   <dimension ref="A1:AP24"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="26" customHeight="1"/>

</xml_diff>

<commit_message>
Added approved client check
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CDD76FE-0D2B-8E49-BDB6-FBBB3C61E871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3C652-E8BA-4940-8831-8F9FA9425199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-42880" yWindow="-17200" windowWidth="28800" windowHeight="16520" tabRatio="710" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="-46660" yWindow="-15740" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="5" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,9 @@
     <definedName name="HeaderAssessedOn">Home!$E$7</definedName>
     <definedName name="HeaderTenantId">Home!$E$5</definedName>
     <definedName name="HeaderTitle">Home!$E$3</definedName>
-    <definedName name="I00001_R_Workload_Exists">'Identity ☑️'!$C$26:$C$35</definedName>
+    <definedName name="I00001_R_Workload_Exists">'Identity ☑️'!$C$29:$C$38</definedName>
     <definedName name="I00001_Workload_Exists">'Identity ☑️'!$E$9:$E$9</definedName>
-    <definedName name="I00002_R_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$C$39:$C$48</definedName>
+    <definedName name="I00002_R_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$C$42:$C$51</definedName>
     <definedName name="I00002_Workload_TenantAppMgmtPolicy">'Identity ☑️'!$E$10</definedName>
     <definedName name="I00003_GlobalAdminPhishingResistantAuthStrength">'Identity ☑️'!$E$13</definedName>
     <definedName name="I00004_BasicMfaUsageInsteadOfAuthStrength">'Identity ☑️'!$E$16</definedName>
@@ -72,6 +72,8 @@
     <definedName name="I00011_PasswordProtectOnPrem">'Identity ☑️'!$E$22</definedName>
     <definedName name="I00012_BannedPasswordList">'Identity ☑️'!$E$23</definedName>
     <definedName name="I00013_PIM_JIT_CriticalRoles">'Identity ☑️'!$E$12</definedName>
+    <definedName name="I00014_CA_AppProtection">'Identity ☑️'!$E$25</definedName>
+    <definedName name="I00015_CA_CompliantDevice">'Identity ☑️'!$E$26</definedName>
     <definedName name="IdentityCP">'Identity ☑️'!$A$1</definedName>
     <definedName name="ListStatus" localSheetId="2">'Device ✍️'!$G$97:$G$104</definedName>
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
@@ -1218,7 +1220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="295">
   <si>
     <t>Policy name</t>
   </si>
@@ -2169,6 +2171,15 @@
   </si>
   <si>
     <t>Identity Zero Trust Roadmap</t>
+  </si>
+  <si>
+    <t>Conditional access</t>
+  </si>
+  <si>
+    <t>Mobile Application Management enforcement</t>
+  </si>
+  <si>
+    <t>Compliant device enforcement</t>
   </si>
 </sst>
 </file>
@@ -3690,7 +3701,57 @@
     <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="150">
+  <dxfs count="155">
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF76FC79"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBADC6A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF941100"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="1"/>
@@ -42097,7 +42158,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -42277,13 +42338,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -42344,13 +42405,13 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -42398,7 +42459,7 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="11112500" cy="3644900"/>
@@ -42578,13 +42639,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -42645,7 +42706,7 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="495300" cy="495300"/>
@@ -46523,7 +46584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6C57C3-010E-3649-B978-A4ACB529691A}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
@@ -49998,417 +50059,417 @@
     <mergeCell ref="W5:Z5"/>
   </mergeCells>
   <conditionalFormatting sqref="A24:K25">
-    <cfRule type="cellIs" dxfId="149" priority="97" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="97" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="98" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="98" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="99" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="99" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="100" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="100" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="101" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="101" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="102" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="102" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="103" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="103" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="104" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="104" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:O47 A67:AA73 A9:AA10 O11 Q11 A11:K12 M11:M12 S11:W12 AA11:AA12 L12 N12:R12 A13:AA13 Q14:AA14 A14:M15 O14:O15 N15 P15:Q15 S15 U15:AA15 A16:AA16 A17:K18 M17:M18 O17:O18 Q17:Q18 S17:S18 U17:AA18 L18 N18 P18 R18 T18 A19:AA19 M20 O20:Q20 R20:S21 A20:K22 U20:AA22 A23:AA23 O24:O25 S24:W25 Y24:Y25 AA24:AA25 A26:AA26 A27:W28 Y27:AA28 A29:AA29 A30:F31 H30:AA31 A32:AA32 A33:Q34 U33:AA34 A35:AA35 A36:F37 H36:AA37 A38:AA38 H39:O40 Q39:AA40 A39:F43 H41:AA43 A44:AA45 A48:AA48 A49:O50 Q49:AA50 A53:O54 Q53:AA54 A55:AA55 A56:O57 S56:AA57 A58:AA58 A59:M60 Q59:AA60 A61:AA61 A64:AA64 A65:F66 H65:M66 S65:AA66 AA74:AA115 A116:K207 S116:AA207 L124:R215">
-    <cfRule type="cellIs" dxfId="141" priority="120" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="120" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:P63">
-    <cfRule type="cellIs" dxfId="140" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="9" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="10" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="11" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="12" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="13" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="14" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="15" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="16" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="16" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:AA10 O11 Q11 A11:K12 M11:M12 S11:W12 AA11:AA12 L12 N12:R12 A13:AA13 Q14:AA14 A14:M15 O14:O15 N15 P15:Q15 S15 U15:AA15 A16:AA16 A17:K18 M17:M18 O17:O18 Q17:Q18 S17:S18 U17:AA18 L18 N18 P18 R18 T18 A19:AA19 M20 O20:Q20 R20:S21 A20:K22 U20:AA22 A23:AA23 O24:O25 S24:W25 Y24:Y25 AA24:AA25 A26:AA26 A27:W28 Y27:AA28 A29:AA29 A30:F31 H30:AA31 A32:AA32 A33:Q34 U33:AA34 A35:AA35 A36:F37 H36:AA37 A38:AA38 H39:O40 Q39:AA40 A39:F43 H41:AA43 A44:AA45 A46:O47 A48:AA48 A49:O50 Q49:AA50 A53:O54 Q53:AA54 A55:AA55 A56:O57 S56:AA57 A58:AA58 A59:M60 Q59:AA60 A61:AA61 A64:AA64 A65:F66 H65:M66 S65:AA66 A67:AA73 AA74:AA115 A116:K207 S116:AA207 L124:R215">
-    <cfRule type="cellIs" dxfId="132" priority="121" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="121" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="122" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="122" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="123" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="123" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="124" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="124" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="125" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="125" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="126" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="126" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="127" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="127" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:AA52">
-    <cfRule type="cellIs" dxfId="125" priority="17" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="17" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="124" priority="18" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="18" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="19" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="19" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="20" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="20" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="21" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="21" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="22" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="22" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="23" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="23" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="24" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="24" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47 G69">
-    <cfRule type="cellIs" dxfId="117" priority="113" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="113" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="114" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="114" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="115" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="115" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="114" priority="116" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="116" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="117" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="117" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="118" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="118" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="119" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="119" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25">
-    <cfRule type="cellIs" dxfId="110" priority="89" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="89" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="90" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="90" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="91" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="91" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="92" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="92" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="93" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="93" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="94" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="94" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="95" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="95" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="96" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="96" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L21:Q21">
-    <cfRule type="cellIs" dxfId="102" priority="105" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="105" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="106" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="106" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="107" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="107" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="108" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="108" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="109" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="109" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="110" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="110" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="111" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="111" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="112" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="112" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25">
-    <cfRule type="cellIs" dxfId="94" priority="73" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="73" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="74" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="74" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="75" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="75" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="76" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="76" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="77" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="77" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="78" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="78" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="79" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="79" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="80" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="80" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="cellIs" dxfId="86" priority="65" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="65" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="66" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="66" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="67" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="67" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="68" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="69" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="69" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="70" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="70" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="71" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="71" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="72" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="72" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P46:P47">
-    <cfRule type="cellIs" dxfId="78" priority="33" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="33" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="34" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="34" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="35" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="35" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="36" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="36" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="37" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="37" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="38" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="38" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="39" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="39" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="40" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="40" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R46:AA47">
-    <cfRule type="cellIs" dxfId="70" priority="25" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="25" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="26" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="26" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="27" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="27" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="28" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="28" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="29" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="29" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="30" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="30" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="31" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="31" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="32" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="32" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R62:AA63">
-    <cfRule type="cellIs" dxfId="62" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="1" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="2" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="3" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="4" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="5" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="6" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="7" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="8" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T21">
-    <cfRule type="cellIs" dxfId="54" priority="81" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="81" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="82" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="82" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="83" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="83" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="84" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="84" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="85" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="85" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="86" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="86" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="87" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="87" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="88" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="88" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X25">
-    <cfRule type="cellIs" dxfId="46" priority="57" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="57" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="58" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="58" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="59" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="59" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="60" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="60" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="61" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="61" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="62" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="62" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="63" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="63" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="64" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="64" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X28">
-    <cfRule type="cellIs" dxfId="38" priority="41" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="41" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="42" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="42" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="43" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="43" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="44" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="44" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="45" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="45" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="46" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="46" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="47" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="48" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z25">
-    <cfRule type="cellIs" dxfId="30" priority="49" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="49" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="50" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="50" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="51" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="51" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="52" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="52" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="53" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="53" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="54" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="54" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="55" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="55" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="56" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="56" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52943,53 +53004,53 @@
     <mergeCell ref="W5:Z5"/>
   </mergeCells>
   <conditionalFormatting sqref="A9:AA11 A12:R12 U12:AA12 A13:AA15 A16:Q16 S16 U16:AA16 A17:AA29 A30:Q30 V30:AA30 A31:AA42 A43:Q43 S43:AA43 A44:T44 V44:AA44 A45:AA63 A64:S64 U64:AA64 A65:AA83 A84:T84 V84:AA84 A85:AA211">
-    <cfRule type="cellIs" dxfId="22" priority="9" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="9" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="10" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="12" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="13" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="14" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="14" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="15" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:AA63 A65:AA83 A84:T84 V84:AA84 A85:AA211 A9:AA11 A12:R12 U12:AA12 A13:AA15 A16:Q16 S16 U16:AA16 A17:AA29 A30:Q30 V30:AA30 A31:AA42 A43:Q43 S43:AA43 A44:T44 V44:AA44 A64:S64 U64:AA64">
-    <cfRule type="cellIs" dxfId="15" priority="8" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="8" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50 G70 G73 L84 R84 X84 L87 N87 P87 R87 X87 G90 L90 N90 P90 R90 X90 G93 L93 N93 P93 R93 X93 G96 L96 N96 G99 G102 L105 N105 P105 R105 L108 N108">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="1" stopIfTrue="1" operator="equal">
       <formula>$AD$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="2" stopIfTrue="1" operator="equal">
       <formula>$AE$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="3" stopIfTrue="1" operator="equal">
       <formula>$AF$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="4" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="4" stopIfTrue="1" operator="equal">
       <formula>$AG$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="5" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" stopIfTrue="1" operator="equal">
       <formula>$AH$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="6" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="6" stopIfTrue="1" operator="equal">
       <formula>$AI$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="7" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" stopIfTrue="1" operator="equal">
       <formula>$AJ$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53930,9 +53991,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B22CC3-1E7C-46FC-913F-FE980CD50DF3}">
-  <dimension ref="A1:AP23"/>
+  <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="26" customHeight="1"/>
   <cols>
@@ -54627,8 +54690,98 @@
       </c>
       <c r="V23" s="202"/>
     </row>
+    <row r="24" spans="2:22" ht="26" customHeight="1">
+      <c r="B24" s="198" t="s">
+        <v>292</v>
+      </c>
+      <c r="C24" s="199"/>
+      <c r="D24" s="199"/>
+      <c r="E24" s="199"/>
+      <c r="F24" s="199"/>
+      <c r="G24" s="199"/>
+      <c r="H24" s="199"/>
+      <c r="I24" s="199"/>
+      <c r="J24" s="199"/>
+      <c r="K24" s="199"/>
+      <c r="L24" s="199"/>
+      <c r="M24" s="199"/>
+      <c r="N24" s="199"/>
+      <c r="O24" s="199"/>
+      <c r="P24" s="199"/>
+      <c r="Q24" s="199"/>
+      <c r="R24" s="199"/>
+      <c r="S24" s="199"/>
+      <c r="T24" s="199"/>
+      <c r="U24" s="199"/>
+      <c r="V24" s="200"/>
+    </row>
+    <row r="25" spans="2:22" ht="26" customHeight="1">
+      <c r="B25" s="134"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="137"/>
+      <c r="F25" s="197" t="s">
+        <v>293</v>
+      </c>
+      <c r="G25" s="197"/>
+      <c r="H25" s="197"/>
+      <c r="I25" s="197"/>
+      <c r="J25" s="197"/>
+      <c r="K25" s="197"/>
+      <c r="L25" s="197"/>
+      <c r="M25" s="197"/>
+      <c r="N25" s="197"/>
+      <c r="O25" s="197"/>
+      <c r="P25" s="197"/>
+      <c r="Q25" s="197"/>
+      <c r="R25" s="197"/>
+      <c r="S25" s="212" t="s">
+        <v>228</v>
+      </c>
+      <c r="T25" s="212"/>
+      <c r="U25" s="212" t="s">
+        <v>228</v>
+      </c>
+      <c r="V25" s="214"/>
+    </row>
+    <row r="26" spans="2:22" ht="26" customHeight="1">
+      <c r="B26" s="133"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="136"/>
+      <c r="F26" s="196" t="s">
+        <v>294</v>
+      </c>
+      <c r="G26" s="196"/>
+      <c r="H26" s="196"/>
+      <c r="I26" s="196"/>
+      <c r="J26" s="196"/>
+      <c r="K26" s="196"/>
+      <c r="L26" s="196"/>
+      <c r="M26" s="196"/>
+      <c r="N26" s="196"/>
+      <c r="O26" s="196"/>
+      <c r="P26" s="196"/>
+      <c r="Q26" s="196"/>
+      <c r="R26" s="196"/>
+      <c r="S26" s="201" t="s">
+        <v>13</v>
+      </c>
+      <c r="T26" s="201"/>
+      <c r="U26" s="201" t="s">
+        <v>228</v>
+      </c>
+      <c r="V26" s="202"/>
+    </row>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="51">
+    <mergeCell ref="B24:V24"/>
+    <mergeCell ref="F25:R25"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="F26:R26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
     <mergeCell ref="U20:V20"/>
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="U18:V18"/>
@@ -54675,19 +54828,36 @@
     <mergeCell ref="F23:R23"/>
   </mergeCells>
   <conditionalFormatting sqref="E7 E9:E10 E12:E14 E16:E23">
-    <cfRule type="cellIs" dxfId="7" priority="129" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="134" stopIfTrue="1" operator="equal">
       <formula>$AI$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="130" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="135" stopIfTrue="1" operator="equal">
       <formula>$AJ$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="131" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="136" stopIfTrue="1" operator="equal">
       <formula>$AK$6</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="132" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="137" stopIfTrue="1" operator="equal">
       <formula>$AK$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="133" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="138" stopIfTrue="1" operator="equal">
+      <formula>$AL$3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E26">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+      <formula>$AI$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" stopIfTrue="1" operator="equal">
+      <formula>$AJ$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+      <formula>$AK$6</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" stopIfTrue="1" operator="equal">
+      <formula>$AK$3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" stopIfTrue="1" operator="equal">
       <formula>$AL$3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56509,13 +56679,13 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <conditionalFormatting sqref="F8:F115">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>$Y$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" stopIfTrue="1" operator="equal">
       <formula>$AA$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="equal">
       <formula>$AB$3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Workload Identity ca policy view
</commit_message>
<xml_diff>
--- a/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
+++ b/src/documentgenerator/Assets/ZeroTrustTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/merill/Projects/zt/src/documentgenerator/Assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3C652-E8BA-4940-8831-8F9FA9425199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE77711-6BFA-5548-B628-CBC46378AFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46660" yWindow="-15740" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="5" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
+    <workbookView xWindow="-45060" yWindow="-19260" windowWidth="28800" windowHeight="16520" tabRatio="710" activeTab="3" xr2:uid="{5EA7E585-8CA3-BF47-B9B9-48D1FF6D96B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Home" sheetId="1" r:id="rId1"/>
@@ -74,6 +74,7 @@
     <definedName name="I00013_PIM_JIT_CriticalRoles">'Identity ☑️'!$E$12</definedName>
     <definedName name="I00014_CA_AppProtection">'Identity ☑️'!$E$25</definedName>
     <definedName name="I00015_CA_CompliantDevice">'Identity ☑️'!$E$26</definedName>
+    <definedName name="IC_Table_WorkloadCA">'Identity ⚙️'!$D$12</definedName>
     <definedName name="IdentityCP">'Identity ☑️'!$A$1</definedName>
     <definedName name="ListStatus" localSheetId="2">'Device ✍️'!$G$97:$G$104</definedName>
     <definedName name="ListStatus">'Identity ✍️'!$G$93:$G$100</definedName>
@@ -1220,7 +1221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="299">
   <si>
     <t>Policy name</t>
   </si>
@@ -2173,13 +2174,25 @@
     <t>Identity Zero Trust Roadmap</t>
   </si>
   <si>
-    <t>Conditional access</t>
-  </si>
-  <si>
     <t>Mobile Application Management enforcement</t>
   </si>
   <si>
     <t>Compliant device enforcement</t>
+  </si>
+  <si>
+    <t>Device and app (MAM) compliance</t>
+  </si>
+  <si>
+    <t>Workload identity: Conditional access policies</t>
+  </si>
+  <si>
+    <t>Conditional access policy name</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Policy Json</t>
   </si>
 </sst>
 </file>
@@ -3116,7 +3129,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="216">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3505,6 +3518,7 @@
     <xf numFmtId="0" fontId="16" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3692,6 +3706,18 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -40105,6 +40131,128 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>215900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B50275CB-4080-8547-8718-C58F77F64ECE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1676400" y="2171700"/>
+          <a:ext cx="6134100" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Conditional Access for workload identities enables blocking service principals from outside of trusted public IP ranges, or based on risk detected by Azure AD Identity Protection.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>288200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>8800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Graphic 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBBC84D6-4A5A-EAA3-1434-5D69B61F7776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId14"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="558800" y="2146300"/>
+          <a:ext cx="720000" cy="720000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -47051,27 +47199,27 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
-      <c r="H5" s="146"/>
+      <c r="F5" s="147"/>
+      <c r="G5" s="147"/>
+      <c r="H5" s="147"/>
       <c r="I5" s="21"/>
-      <c r="J5" s="147"/>
-      <c r="K5" s="147"/>
-      <c r="L5" s="147"/>
-      <c r="M5" s="147"/>
-      <c r="N5" s="147"/>
-      <c r="O5" s="147"/>
-      <c r="P5" s="147"/>
+      <c r="J5" s="148"/>
+      <c r="K5" s="148"/>
+      <c r="L5" s="148"/>
+      <c r="M5" s="148"/>
+      <c r="N5" s="148"/>
+      <c r="O5" s="148"/>
+      <c r="P5" s="148"/>
       <c r="Q5" s="22"/>
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
       <c r="T5" s="22"/>
       <c r="U5" s="22"/>
       <c r="V5" s="21"/>
-      <c r="W5" s="147"/>
-      <c r="X5" s="147"/>
-      <c r="Y5" s="147"/>
-      <c r="Z5" s="147"/>
+      <c r="W5" s="148"/>
+      <c r="X5" s="148"/>
+      <c r="Y5" s="148"/>
+      <c r="Z5" s="148"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -50661,27 +50809,27 @@
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
       <c r="E5" s="40"/>
-      <c r="F5" s="148"/>
-      <c r="G5" s="148"/>
-      <c r="H5" s="148"/>
+      <c r="F5" s="149"/>
+      <c r="G5" s="149"/>
+      <c r="H5" s="149"/>
       <c r="I5" s="46"/>
-      <c r="J5" s="149"/>
-      <c r="K5" s="149"/>
-      <c r="L5" s="149"/>
-      <c r="M5" s="149"/>
-      <c r="N5" s="149"/>
-      <c r="O5" s="149"/>
-      <c r="P5" s="149"/>
+      <c r="J5" s="150"/>
+      <c r="K5" s="150"/>
+      <c r="L5" s="150"/>
+      <c r="M5" s="150"/>
+      <c r="N5" s="150"/>
+      <c r="O5" s="150"/>
+      <c r="P5" s="150"/>
       <c r="Q5" s="47"/>
       <c r="R5" s="47"/>
       <c r="S5" s="47"/>
       <c r="T5" s="47"/>
       <c r="U5" s="47"/>
       <c r="V5" s="46"/>
-      <c r="W5" s="149"/>
-      <c r="X5" s="149"/>
-      <c r="Y5" s="149"/>
-      <c r="Z5" s="149"/>
+      <c r="W5" s="150"/>
+      <c r="X5" s="150"/>
+      <c r="Y5" s="150"/>
+      <c r="Z5" s="150"/>
       <c r="AA5" s="40"/>
     </row>
     <row r="6" spans="1:37" ht="5" customHeight="1">
@@ -53070,9 +53218,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8363E681-A1AE-4887-9EC0-161837175EE7}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12:N12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16"/>
   <cols>
@@ -53249,7 +53399,110 @@
       <c r="AE5" s="55"/>
       <c r="AF5" s="55"/>
     </row>
+    <row r="8" spans="1:32" ht="28">
+      <c r="B8" s="3"/>
+      <c r="D8" s="72" t="s">
+        <v>295</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:32" ht="28">
+      <c r="B9" s="3"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:32" ht="28">
+      <c r="B10" s="3"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:32">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="166" t="s">
+        <v>296</v>
+      </c>
+      <c r="E11" s="167"/>
+      <c r="F11" s="167"/>
+      <c r="G11" s="167"/>
+      <c r="H11" s="167"/>
+      <c r="I11" s="168"/>
+      <c r="J11" s="146" t="s">
+        <v>297</v>
+      </c>
+      <c r="K11" s="166" t="s">
+        <v>298</v>
+      </c>
+      <c r="L11" s="167"/>
+      <c r="M11" s="167"/>
+      <c r="N11" s="168"/>
+    </row>
+    <row r="12" spans="1:32">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="217"/>
+      <c r="E12" s="218"/>
+      <c r="F12" s="218"/>
+      <c r="G12" s="218"/>
+      <c r="H12" s="218"/>
+      <c r="I12" s="219"/>
+      <c r="J12" s="220"/>
+      <c r="K12" s="217"/>
+      <c r="L12" s="218"/>
+      <c r="M12" s="218"/>
+      <c r="N12" s="219"/>
+    </row>
+    <row r="13" spans="1:32">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="D11:I11"/>
+    <mergeCell ref="D12:I12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
@@ -53264,7 +53517,7 @@
       <pane xSplit="11" ySplit="5" topLeftCell="L6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16"/>
@@ -53428,33 +53681,33 @@
       <c r="D13" s="91" t="s">
         <v>184</v>
       </c>
-      <c r="E13" s="158" t="s">
+      <c r="E13" s="159" t="s">
         <v>183</v>
       </c>
-      <c r="F13" s="158"/>
-      <c r="G13" s="158"/>
-      <c r="H13" s="158"/>
-      <c r="I13" s="158"/>
-      <c r="J13" s="158" t="s">
+      <c r="F13" s="159"/>
+      <c r="G13" s="159"/>
+      <c r="H13" s="159"/>
+      <c r="I13" s="159"/>
+      <c r="J13" s="159" t="s">
         <v>185</v>
       </c>
-      <c r="K13" s="158"/>
-      <c r="L13" s="91" t="s">
+      <c r="K13" s="159"/>
+      <c r="L13" s="166" t="s">
         <v>186</v>
       </c>
-      <c r="M13" s="92"/>
+      <c r="M13" s="168"/>
     </row>
     <row r="14" spans="1:32">
       <c r="D14" s="92"/>
-      <c r="E14" s="150"/>
-      <c r="F14" s="163"/>
-      <c r="G14" s="163"/>
-      <c r="H14" s="163"/>
-      <c r="I14" s="151"/>
-      <c r="J14" s="150"/>
-      <c r="K14" s="151"/>
-      <c r="L14" s="150"/>
-      <c r="M14" s="151"/>
+      <c r="E14" s="151"/>
+      <c r="F14" s="164"/>
+      <c r="G14" s="164"/>
+      <c r="H14" s="164"/>
+      <c r="I14" s="152"/>
+      <c r="J14" s="151"/>
+      <c r="K14" s="152"/>
+      <c r="L14" s="151"/>
+      <c r="M14" s="152"/>
     </row>
     <row r="18" spans="3:41" ht="28">
       <c r="C18"/>
@@ -53471,20 +53724,20 @@
       <c r="D20" s="72"/>
     </row>
     <row r="21" spans="3:41">
-      <c r="D21" s="158" t="s">
+      <c r="D21" s="159" t="s">
         <v>1</v>
       </c>
-      <c r="E21" s="158"/>
-      <c r="F21" s="158"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
       <c r="G21" s="91" t="s">
         <v>191</v>
       </c>
-      <c r="H21" s="158" t="s">
+      <c r="H21" s="159" t="s">
         <v>183</v>
       </c>
-      <c r="I21" s="158"/>
-      <c r="J21" s="158"/>
-      <c r="K21" s="158"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="159"/>
+      <c r="K21" s="159"/>
       <c r="L21" s="91" t="s">
         <v>192</v>
       </c>
@@ -53494,14 +53747,14 @@
       <c r="N21" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="O21" s="158" t="s">
+      <c r="O21" s="159" t="s">
         <v>195</v>
       </c>
-      <c r="P21" s="158"/>
-      <c r="Q21" s="158" t="s">
+      <c r="P21" s="159"/>
+      <c r="Q21" s="159" t="s">
         <v>198</v>
       </c>
-      <c r="R21" s="158"/>
+      <c r="R21" s="159"/>
       <c r="S21" s="91" t="s">
         <v>196</v>
       </c>
@@ -53511,24 +53764,24 @@
       <c r="U21" s="92"/>
     </row>
     <row r="22" spans="3:41">
-      <c r="D22" s="150"/>
-      <c r="E22" s="163"/>
-      <c r="F22" s="151"/>
+      <c r="D22" s="151"/>
+      <c r="E22" s="164"/>
+      <c r="F22" s="152"/>
       <c r="G22" s="93"/>
-      <c r="H22" s="150"/>
-      <c r="I22" s="163"/>
-      <c r="J22" s="163"/>
-      <c r="K22" s="151"/>
+      <c r="H22" s="151"/>
+      <c r="I22" s="164"/>
+      <c r="J22" s="164"/>
+      <c r="K22" s="152"/>
       <c r="L22" s="92"/>
       <c r="M22" s="94"/>
       <c r="N22" s="94"/>
-      <c r="O22" s="150"/>
-      <c r="P22" s="151"/>
-      <c r="Q22" s="150"/>
-      <c r="R22" s="151"/>
+      <c r="O22" s="151"/>
+      <c r="P22" s="152"/>
+      <c r="Q22" s="151"/>
+      <c r="R22" s="152"/>
       <c r="S22" s="92"/>
-      <c r="T22" s="150"/>
-      <c r="U22" s="151"/>
+      <c r="T22" s="151"/>
+      <c r="U22" s="152"/>
     </row>
     <row r="23" spans="3:41" ht="17" customHeight="1"/>
     <row r="26" spans="3:41" ht="28">
@@ -53550,18 +53803,18 @@
       <c r="D29" s="72"/>
     </row>
     <row r="30" spans="3:41" s="73" customFormat="1" ht="68">
-      <c r="D30" s="160" t="s">
+      <c r="D30" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="160"/>
-      <c r="F30" s="160"/>
-      <c r="G30" s="160" t="s">
+      <c r="E30" s="161"/>
+      <c r="F30" s="161"/>
+      <c r="G30" s="161" t="s">
         <v>0</v>
       </c>
-      <c r="H30" s="160"/>
-      <c r="I30" s="160"/>
-      <c r="J30" s="160"/>
-      <c r="K30" s="161"/>
+      <c r="H30" s="161"/>
+      <c r="I30" s="161"/>
+      <c r="J30" s="161"/>
+      <c r="K30" s="162"/>
       <c r="L30" s="107" t="s">
         <v>201</v>
       </c>
@@ -53577,10 +53830,10 @@
       <c r="P30" s="108" t="s">
         <v>207</v>
       </c>
-      <c r="Q30" s="159" t="s">
+      <c r="Q30" s="160" t="s">
         <v>200</v>
       </c>
-      <c r="R30" s="159"/>
+      <c r="R30" s="160"/>
       <c r="S30" s="108" t="s">
         <v>208</v>
       </c>
@@ -53602,48 +53855,48 @@
       <c r="Y30" s="111" t="s">
         <v>210</v>
       </c>
-      <c r="Z30" s="156" t="s">
+      <c r="Z30" s="157" t="s">
         <v>215</v>
       </c>
-      <c r="AA30" s="156"/>
-      <c r="AB30" s="156" t="s">
+      <c r="AA30" s="157"/>
+      <c r="AB30" s="157" t="s">
         <v>216</v>
       </c>
-      <c r="AC30" s="156"/>
-      <c r="AD30" s="156" t="s">
+      <c r="AC30" s="157"/>
+      <c r="AD30" s="157" t="s">
         <v>217</v>
       </c>
-      <c r="AE30" s="156"/>
-      <c r="AF30" s="156" t="s">
+      <c r="AE30" s="157"/>
+      <c r="AF30" s="157" t="s">
         <v>218</v>
       </c>
-      <c r="AG30" s="156"/>
-      <c r="AH30" s="156" t="s">
+      <c r="AG30" s="157"/>
+      <c r="AH30" s="157" t="s">
         <v>219</v>
       </c>
-      <c r="AI30" s="156"/>
-      <c r="AJ30" s="155" t="s">
+      <c r="AI30" s="157"/>
+      <c r="AJ30" s="156" t="s">
         <v>196</v>
       </c>
-      <c r="AK30" s="155"/>
-      <c r="AL30" s="154" t="s">
+      <c r="AK30" s="156"/>
+      <c r="AL30" s="155" t="s">
         <v>204</v>
       </c>
-      <c r="AM30" s="154"/>
-      <c r="AN30" s="154" t="s">
+      <c r="AM30" s="155"/>
+      <c r="AN30" s="155" t="s">
         <v>205</v>
       </c>
-      <c r="AO30" s="154"/>
+      <c r="AO30" s="155"/>
     </row>
     <row r="31" spans="3:41">
-      <c r="D31" s="150"/>
-      <c r="E31" s="163"/>
-      <c r="F31" s="151"/>
-      <c r="G31" s="165"/>
-      <c r="H31" s="166"/>
-      <c r="I31" s="166"/>
-      <c r="J31" s="166"/>
-      <c r="K31" s="167"/>
+      <c r="D31" s="151"/>
+      <c r="E31" s="164"/>
+      <c r="F31" s="152"/>
+      <c r="G31" s="166"/>
+      <c r="H31" s="167"/>
+      <c r="I31" s="167"/>
+      <c r="J31" s="167"/>
+      <c r="K31" s="168"/>
       <c r="L31" s="102"/>
       <c r="M31" s="103"/>
       <c r="N31" s="103"/>
@@ -53658,22 +53911,22 @@
       <c r="W31" s="106"/>
       <c r="X31" s="106"/>
       <c r="Y31" s="106"/>
-      <c r="Z31" s="157"/>
-      <c r="AA31" s="157"/>
-      <c r="AB31" s="157"/>
-      <c r="AC31" s="157"/>
-      <c r="AD31" s="157"/>
-      <c r="AE31" s="157"/>
-      <c r="AF31" s="157"/>
-      <c r="AG31" s="157"/>
-      <c r="AH31" s="157"/>
-      <c r="AI31" s="157"/>
-      <c r="AJ31" s="153"/>
-      <c r="AK31" s="153"/>
-      <c r="AL31" s="152"/>
-      <c r="AM31" s="152"/>
-      <c r="AN31" s="152"/>
-      <c r="AO31" s="152"/>
+      <c r="Z31" s="158"/>
+      <c r="AA31" s="158"/>
+      <c r="AB31" s="158"/>
+      <c r="AC31" s="158"/>
+      <c r="AD31" s="158"/>
+      <c r="AE31" s="158"/>
+      <c r="AF31" s="158"/>
+      <c r="AG31" s="158"/>
+      <c r="AH31" s="158"/>
+      <c r="AI31" s="158"/>
+      <c r="AJ31" s="154"/>
+      <c r="AK31" s="154"/>
+      <c r="AL31" s="153"/>
+      <c r="AM31" s="153"/>
+      <c r="AN31" s="153"/>
+      <c r="AO31" s="153"/>
     </row>
     <row r="35" spans="1:53" ht="28">
       <c r="C35"/>
@@ -53692,90 +53945,90 @@
     <row r="38" spans="1:53" ht="28">
       <c r="C38" s="71"/>
       <c r="D38" s="72"/>
-      <c r="L38" s="164" t="s">
+      <c r="L38" s="165" t="s">
         <v>244</v>
       </c>
-      <c r="M38" s="164"/>
-      <c r="N38" s="164"/>
-      <c r="O38" s="164"/>
-      <c r="P38" s="192" t="s">
+      <c r="M38" s="165"/>
+      <c r="N38" s="165"/>
+      <c r="O38" s="165"/>
+      <c r="P38" s="193" t="s">
         <v>105</v>
       </c>
-      <c r="Q38" s="192"/>
-      <c r="R38" s="192"/>
-      <c r="S38" s="192"/>
-      <c r="T38" s="192"/>
-      <c r="U38" s="192"/>
-      <c r="V38" s="192"/>
-      <c r="W38" s="192"/>
-      <c r="X38" s="192"/>
-      <c r="Y38" s="192"/>
-      <c r="Z38" s="192"/>
-      <c r="AA38" s="192"/>
-      <c r="AB38" s="192"/>
-      <c r="AC38" s="192"/>
-      <c r="AD38" s="192"/>
-      <c r="AE38" s="192"/>
-      <c r="AF38" s="192"/>
-      <c r="AG38" s="189" t="s">
+      <c r="Q38" s="193"/>
+      <c r="R38" s="193"/>
+      <c r="S38" s="193"/>
+      <c r="T38" s="193"/>
+      <c r="U38" s="193"/>
+      <c r="V38" s="193"/>
+      <c r="W38" s="193"/>
+      <c r="X38" s="193"/>
+      <c r="Y38" s="193"/>
+      <c r="Z38" s="193"/>
+      <c r="AA38" s="193"/>
+      <c r="AB38" s="193"/>
+      <c r="AC38" s="193"/>
+      <c r="AD38" s="193"/>
+      <c r="AE38" s="193"/>
+      <c r="AF38" s="193"/>
+      <c r="AG38" s="190" t="s">
         <v>263</v>
       </c>
-      <c r="AH38" s="189"/>
-      <c r="AI38" s="189"/>
-      <c r="AJ38" s="189"/>
-      <c r="AK38" s="189"/>
-      <c r="AL38" s="189"/>
-      <c r="AM38" s="190" t="s">
+      <c r="AH38" s="190"/>
+      <c r="AI38" s="190"/>
+      <c r="AJ38" s="190"/>
+      <c r="AK38" s="190"/>
+      <c r="AL38" s="190"/>
+      <c r="AM38" s="191" t="s">
         <v>268</v>
       </c>
-      <c r="AN38" s="190"/>
-      <c r="AO38" s="190"/>
-      <c r="AP38" s="190"/>
-      <c r="AQ38" s="190"/>
-      <c r="AR38" s="190"/>
-      <c r="AS38" s="190"/>
-      <c r="AT38" s="190"/>
-      <c r="AU38" s="190"/>
-      <c r="AV38" s="191" t="s">
+      <c r="AN38" s="191"/>
+      <c r="AO38" s="191"/>
+      <c r="AP38" s="191"/>
+      <c r="AQ38" s="191"/>
+      <c r="AR38" s="191"/>
+      <c r="AS38" s="191"/>
+      <c r="AT38" s="191"/>
+      <c r="AU38" s="191"/>
+      <c r="AV38" s="192" t="s">
         <v>269</v>
       </c>
-      <c r="AW38" s="191"/>
-      <c r="AX38" s="191"/>
-      <c r="AY38" s="191"/>
-      <c r="AZ38" s="191"/>
-      <c r="BA38" s="191"/>
+      <c r="AW38" s="192"/>
+      <c r="AX38" s="192"/>
+      <c r="AY38" s="192"/>
+      <c r="AZ38" s="192"/>
+      <c r="BA38" s="192"/>
     </row>
     <row r="39" spans="1:53" ht="153">
       <c r="A39" s="73"/>
       <c r="B39" s="73"/>
       <c r="C39" s="73"/>
-      <c r="D39" s="160" t="s">
+      <c r="D39" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="160"/>
-      <c r="F39" s="161"/>
-      <c r="G39" s="162" t="s">
+      <c r="E39" s="161"/>
+      <c r="F39" s="162"/>
+      <c r="G39" s="163" t="s">
         <v>0</v>
       </c>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
-      <c r="J39" s="162"/>
-      <c r="K39" s="162"/>
-      <c r="L39" s="178" t="s">
+      <c r="H39" s="163"/>
+      <c r="I39" s="163"/>
+      <c r="J39" s="163"/>
+      <c r="K39" s="163"/>
+      <c r="L39" s="179" t="s">
         <v>242</v>
       </c>
-      <c r="M39" s="179"/>
-      <c r="N39" s="178" t="s">
+      <c r="M39" s="180"/>
+      <c r="N39" s="179" t="s">
         <v>243</v>
       </c>
-      <c r="O39" s="179"/>
+      <c r="O39" s="180"/>
       <c r="P39" s="109" t="s">
         <v>270</v>
       </c>
-      <c r="Q39" s="187" t="s">
+      <c r="Q39" s="188" t="s">
         <v>245</v>
       </c>
-      <c r="R39" s="188"/>
+      <c r="R39" s="189"/>
       <c r="S39" s="110" t="s">
         <v>246</v>
       </c>
@@ -53818,10 +54071,10 @@
       <c r="AF39" s="112" t="s">
         <v>259</v>
       </c>
-      <c r="AG39" s="180" t="s">
+      <c r="AG39" s="181" t="s">
         <v>265</v>
       </c>
-      <c r="AH39" s="181"/>
+      <c r="AH39" s="182"/>
       <c r="AI39" s="113" t="s">
         <v>260</v>
       </c>
@@ -53843,45 +54096,45 @@
       <c r="AO39" s="114" t="s">
         <v>267</v>
       </c>
-      <c r="AP39" s="182" t="s">
+      <c r="AP39" s="183" t="s">
         <v>202</v>
       </c>
-      <c r="AQ39" s="183"/>
-      <c r="AR39" s="184"/>
-      <c r="AS39" s="182" t="s">
+      <c r="AQ39" s="184"/>
+      <c r="AR39" s="185"/>
+      <c r="AS39" s="183" t="s">
         <v>203</v>
       </c>
-      <c r="AT39" s="183"/>
-      <c r="AU39" s="184"/>
-      <c r="AV39" s="185" t="s">
+      <c r="AT39" s="184"/>
+      <c r="AU39" s="185"/>
+      <c r="AV39" s="186" t="s">
         <v>196</v>
       </c>
-      <c r="AW39" s="186"/>
-      <c r="AX39" s="193" t="s">
+      <c r="AW39" s="187"/>
+      <c r="AX39" s="194" t="s">
         <v>204</v>
       </c>
-      <c r="AY39" s="194"/>
-      <c r="AZ39" s="193" t="s">
+      <c r="AY39" s="195"/>
+      <c r="AZ39" s="194" t="s">
         <v>205</v>
       </c>
-      <c r="BA39" s="194"/>
+      <c r="BA39" s="195"/>
     </row>
     <row r="40" spans="1:53">
-      <c r="D40" s="150"/>
-      <c r="E40" s="163"/>
-      <c r="F40" s="151"/>
-      <c r="G40" s="168"/>
-      <c r="H40" s="169"/>
-      <c r="I40" s="169"/>
-      <c r="J40" s="169"/>
-      <c r="K40" s="170"/>
-      <c r="L40" s="176"/>
-      <c r="M40" s="177"/>
-      <c r="N40" s="176"/>
-      <c r="O40" s="177"/>
+      <c r="D40" s="151"/>
+      <c r="E40" s="164"/>
+      <c r="F40" s="152"/>
+      <c r="G40" s="169"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
+      <c r="J40" s="170"/>
+      <c r="K40" s="171"/>
+      <c r="L40" s="177"/>
+      <c r="M40" s="178"/>
+      <c r="N40" s="177"/>
+      <c r="O40" s="178"/>
       <c r="P40" s="104"/>
-      <c r="Q40" s="174"/>
-      <c r="R40" s="175"/>
+      <c r="Q40" s="175"/>
+      <c r="R40" s="176"/>
       <c r="S40" s="105"/>
       <c r="T40" s="105"/>
       <c r="U40" s="105"/>
@@ -53905,21 +54158,22 @@
       <c r="AM40" s="117"/>
       <c r="AN40" s="117"/>
       <c r="AO40" s="117"/>
-      <c r="AP40" s="171"/>
-      <c r="AQ40" s="172"/>
-      <c r="AR40" s="173"/>
-      <c r="AS40" s="171"/>
-      <c r="AT40" s="172"/>
-      <c r="AU40" s="173"/>
-      <c r="AV40" s="153"/>
-      <c r="AW40" s="153"/>
-      <c r="AX40" s="152"/>
-      <c r="AY40" s="152"/>
-      <c r="AZ40" s="152"/>
-      <c r="BA40" s="152"/>
+      <c r="AP40" s="172"/>
+      <c r="AQ40" s="173"/>
+      <c r="AR40" s="174"/>
+      <c r="AS40" s="172"/>
+      <c r="AT40" s="173"/>
+      <c r="AU40" s="174"/>
+      <c r="AV40" s="154"/>
+      <c r="AW40" s="154"/>
+      <c r="AX40" s="153"/>
+      <c r="AY40" s="153"/>
+      <c r="AZ40" s="153"/>
+      <c r="BA40" s="153"/>
     </row>
   </sheetData>
-  <mergeCells count="61">
+  <mergeCells count="62">
+    <mergeCell ref="L13:M13"/>
     <mergeCell ref="AG38:AL38"/>
     <mergeCell ref="AM38:AU38"/>
     <mergeCell ref="AV38:BA38"/>
@@ -53993,8 +54247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07B22CC3-1E7C-46FC-913F-FE980CD50DF3}">
   <dimension ref="A1:AP26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="26" customHeight="1"/>
@@ -54231,547 +54485,547 @@
       <c r="P7" s="128"/>
       <c r="Q7" s="128"/>
       <c r="R7" s="128"/>
-      <c r="S7" s="208" t="s">
+      <c r="S7" s="209" t="s">
         <v>5</v>
       </c>
-      <c r="T7" s="208"/>
-      <c r="U7" s="208" t="s">
+      <c r="T7" s="209"/>
+      <c r="U7" s="209" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="209"/>
+      <c r="V7" s="210"/>
     </row>
     <row r="8" spans="1:42" ht="26" customHeight="1">
-      <c r="B8" s="198" t="s">
+      <c r="B8" s="199" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="199"/>
-      <c r="D8" s="199"/>
-      <c r="E8" s="199"/>
-      <c r="F8" s="199"/>
-      <c r="G8" s="199"/>
-      <c r="H8" s="199"/>
-      <c r="I8" s="199"/>
-      <c r="J8" s="199"/>
-      <c r="K8" s="199"/>
-      <c r="L8" s="199"/>
-      <c r="M8" s="199"/>
-      <c r="N8" s="199"/>
-      <c r="O8" s="199"/>
-      <c r="P8" s="199"/>
-      <c r="Q8" s="199"/>
-      <c r="R8" s="199"/>
-      <c r="S8" s="199"/>
-      <c r="T8" s="199"/>
-      <c r="U8" s="199"/>
-      <c r="V8" s="200"/>
+      <c r="C8" s="200"/>
+      <c r="D8" s="200"/>
+      <c r="E8" s="200"/>
+      <c r="F8" s="200"/>
+      <c r="G8" s="200"/>
+      <c r="H8" s="200"/>
+      <c r="I8" s="200"/>
+      <c r="J8" s="200"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="200"/>
+      <c r="M8" s="200"/>
+      <c r="N8" s="200"/>
+      <c r="O8" s="200"/>
+      <c r="P8" s="200"/>
+      <c r="Q8" s="200"/>
+      <c r="R8" s="200"/>
+      <c r="S8" s="200"/>
+      <c r="T8" s="200"/>
+      <c r="U8" s="200"/>
+      <c r="V8" s="201"/>
     </row>
     <row r="9" spans="1:42" ht="26" customHeight="1">
       <c r="B9" s="132"/>
       <c r="C9" s="86"/>
       <c r="D9" s="86"/>
       <c r="E9" s="135"/>
-      <c r="F9" s="210" t="s">
+      <c r="F9" s="211" t="s">
         <v>272</v>
       </c>
-      <c r="G9" s="210"/>
-      <c r="H9" s="210"/>
-      <c r="I9" s="210"/>
-      <c r="J9" s="210"/>
-      <c r="K9" s="210"/>
-      <c r="L9" s="210"/>
-      <c r="M9" s="210"/>
-      <c r="N9" s="210"/>
-      <c r="O9" s="210"/>
-      <c r="P9" s="210"/>
-      <c r="Q9" s="210"/>
-      <c r="R9" s="210"/>
-      <c r="S9" s="206" t="s">
+      <c r="G9" s="211"/>
+      <c r="H9" s="211"/>
+      <c r="I9" s="211"/>
+      <c r="J9" s="211"/>
+      <c r="K9" s="211"/>
+      <c r="L9" s="211"/>
+      <c r="M9" s="211"/>
+      <c r="N9" s="211"/>
+      <c r="O9" s="211"/>
+      <c r="P9" s="211"/>
+      <c r="Q9" s="211"/>
+      <c r="R9" s="211"/>
+      <c r="S9" s="207" t="s">
         <v>226</v>
       </c>
-      <c r="T9" s="206"/>
-      <c r="U9" s="206" t="s">
+      <c r="T9" s="207"/>
+      <c r="U9" s="207" t="s">
         <v>228</v>
       </c>
-      <c r="V9" s="207"/>
+      <c r="V9" s="208"/>
     </row>
     <row r="10" spans="1:42" ht="26" customHeight="1">
       <c r="B10" s="132"/>
       <c r="C10" s="86"/>
       <c r="D10" s="86"/>
       <c r="E10" s="136"/>
-      <c r="F10" s="203" t="s">
+      <c r="F10" s="204" t="s">
         <v>273</v>
       </c>
-      <c r="G10" s="203"/>
-      <c r="H10" s="203"/>
-      <c r="I10" s="203"/>
-      <c r="J10" s="203"/>
-      <c r="K10" s="203"/>
-      <c r="L10" s="203"/>
-      <c r="M10" s="203"/>
-      <c r="N10" s="203"/>
-      <c r="O10" s="203"/>
-      <c r="P10" s="203"/>
-      <c r="Q10" s="203"/>
-      <c r="R10" s="203"/>
-      <c r="S10" s="201" t="s">
+      <c r="G10" s="204"/>
+      <c r="H10" s="204"/>
+      <c r="I10" s="204"/>
+      <c r="J10" s="204"/>
+      <c r="K10" s="204"/>
+      <c r="L10" s="204"/>
+      <c r="M10" s="204"/>
+      <c r="N10" s="204"/>
+      <c r="O10" s="204"/>
+      <c r="P10" s="204"/>
+      <c r="Q10" s="204"/>
+      <c r="R10" s="204"/>
+      <c r="S10" s="202" t="s">
         <v>228</v>
       </c>
-      <c r="T10" s="201"/>
-      <c r="U10" s="201" t="s">
+      <c r="T10" s="202"/>
+      <c r="U10" s="202" t="s">
         <v>228</v>
       </c>
-      <c r="V10" s="202"/>
+      <c r="V10" s="203"/>
     </row>
     <row r="11" spans="1:42" ht="26" customHeight="1">
-      <c r="B11" s="198" t="s">
+      <c r="B11" s="199" t="s">
         <v>274</v>
       </c>
-      <c r="C11" s="199"/>
-      <c r="D11" s="199"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="199"/>
-      <c r="H11" s="199"/>
-      <c r="I11" s="199"/>
-      <c r="J11" s="199"/>
-      <c r="K11" s="199"/>
-      <c r="L11" s="199"/>
-      <c r="M11" s="199"/>
-      <c r="N11" s="199"/>
-      <c r="O11" s="199"/>
-      <c r="P11" s="199"/>
-      <c r="Q11" s="199"/>
-      <c r="R11" s="199"/>
-      <c r="S11" s="199"/>
-      <c r="T11" s="199"/>
-      <c r="U11" s="199"/>
-      <c r="V11" s="200"/>
+      <c r="C11" s="200"/>
+      <c r="D11" s="200"/>
+      <c r="E11" s="200"/>
+      <c r="F11" s="200"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="200"/>
+      <c r="I11" s="200"/>
+      <c r="J11" s="200"/>
+      <c r="K11" s="200"/>
+      <c r="L11" s="200"/>
+      <c r="M11" s="200"/>
+      <c r="N11" s="200"/>
+      <c r="O11" s="200"/>
+      <c r="P11" s="200"/>
+      <c r="Q11" s="200"/>
+      <c r="R11" s="200"/>
+      <c r="S11" s="200"/>
+      <c r="T11" s="200"/>
+      <c r="U11" s="200"/>
+      <c r="V11" s="201"/>
     </row>
     <row r="12" spans="1:42" ht="26" customHeight="1">
       <c r="B12" s="132"/>
       <c r="C12" s="86"/>
       <c r="D12" s="86"/>
       <c r="E12" s="137"/>
-      <c r="F12" s="197" t="s">
+      <c r="F12" s="198" t="s">
         <v>275</v>
       </c>
-      <c r="G12" s="197"/>
-      <c r="H12" s="197"/>
-      <c r="I12" s="197"/>
-      <c r="J12" s="197"/>
-      <c r="K12" s="197"/>
-      <c r="L12" s="197"/>
-      <c r="M12" s="197"/>
-      <c r="N12" s="197"/>
-      <c r="O12" s="197"/>
-      <c r="P12" s="197"/>
-      <c r="Q12" s="197"/>
-      <c r="R12" s="197"/>
-      <c r="S12" s="206" t="s">
+      <c r="G12" s="198"/>
+      <c r="H12" s="198"/>
+      <c r="I12" s="198"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="198"/>
+      <c r="L12" s="198"/>
+      <c r="M12" s="198"/>
+      <c r="N12" s="198"/>
+      <c r="O12" s="198"/>
+      <c r="P12" s="198"/>
+      <c r="Q12" s="198"/>
+      <c r="R12" s="198"/>
+      <c r="S12" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="T12" s="206"/>
-      <c r="U12" s="206" t="s">
+      <c r="T12" s="207"/>
+      <c r="U12" s="207" t="s">
         <v>13</v>
       </c>
-      <c r="V12" s="207"/>
+      <c r="V12" s="208"/>
     </row>
     <row r="13" spans="1:42" ht="26" customHeight="1">
       <c r="B13" s="132"/>
       <c r="C13" s="86"/>
       <c r="D13" s="86"/>
       <c r="E13" s="138"/>
-      <c r="F13" s="195" t="s">
+      <c r="F13" s="196" t="s">
         <v>276</v>
       </c>
-      <c r="G13" s="195"/>
-      <c r="H13" s="195"/>
-      <c r="I13" s="195"/>
-      <c r="J13" s="195"/>
-      <c r="K13" s="195"/>
-      <c r="L13" s="195"/>
-      <c r="M13" s="195"/>
-      <c r="N13" s="195"/>
-      <c r="O13" s="195"/>
-      <c r="P13" s="195"/>
-      <c r="Q13" s="195"/>
-      <c r="R13" s="195"/>
-      <c r="S13" s="204" t="s">
+      <c r="G13" s="196"/>
+      <c r="H13" s="196"/>
+      <c r="I13" s="196"/>
+      <c r="J13" s="196"/>
+      <c r="K13" s="196"/>
+      <c r="L13" s="196"/>
+      <c r="M13" s="196"/>
+      <c r="N13" s="196"/>
+      <c r="O13" s="196"/>
+      <c r="P13" s="196"/>
+      <c r="Q13" s="196"/>
+      <c r="R13" s="196"/>
+      <c r="S13" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="T13" s="204"/>
-      <c r="U13" s="204"/>
-      <c r="V13" s="205"/>
+      <c r="T13" s="205"/>
+      <c r="U13" s="205"/>
+      <c r="V13" s="206"/>
     </row>
     <row r="14" spans="1:42" ht="26" customHeight="1">
       <c r="B14" s="132"/>
       <c r="C14" s="86"/>
       <c r="D14" s="86"/>
       <c r="E14" s="139"/>
-      <c r="F14" s="196" t="s">
+      <c r="F14" s="197" t="s">
         <v>277</v>
       </c>
-      <c r="G14" s="196"/>
-      <c r="H14" s="196"/>
-      <c r="I14" s="196"/>
-      <c r="J14" s="196"/>
-      <c r="K14" s="196"/>
-      <c r="L14" s="196"/>
-      <c r="M14" s="196"/>
-      <c r="N14" s="196"/>
-      <c r="O14" s="196"/>
-      <c r="P14" s="196"/>
-      <c r="Q14" s="196"/>
-      <c r="R14" s="196"/>
-      <c r="S14" s="201" t="s">
+      <c r="G14" s="197"/>
+      <c r="H14" s="197"/>
+      <c r="I14" s="197"/>
+      <c r="J14" s="197"/>
+      <c r="K14" s="197"/>
+      <c r="L14" s="197"/>
+      <c r="M14" s="197"/>
+      <c r="N14" s="197"/>
+      <c r="O14" s="197"/>
+      <c r="P14" s="197"/>
+      <c r="Q14" s="197"/>
+      <c r="R14" s="197"/>
+      <c r="S14" s="202" t="s">
         <v>228</v>
       </c>
-      <c r="T14" s="201"/>
-      <c r="U14" s="201" t="s">
+      <c r="T14" s="202"/>
+      <c r="U14" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="V14" s="202"/>
+      <c r="V14" s="203"/>
     </row>
     <row r="15" spans="1:42" ht="26" customHeight="1">
-      <c r="B15" s="198" t="s">
+      <c r="B15" s="199" t="s">
         <v>278</v>
       </c>
-      <c r="C15" s="199"/>
-      <c r="D15" s="199"/>
-      <c r="E15" s="199"/>
-      <c r="F15" s="199"/>
-      <c r="G15" s="199"/>
-      <c r="H15" s="199"/>
-      <c r="I15" s="199"/>
-      <c r="J15" s="199"/>
-      <c r="K15" s="199"/>
-      <c r="L15" s="199"/>
-      <c r="M15" s="199"/>
-      <c r="N15" s="199"/>
-      <c r="O15" s="199"/>
-      <c r="P15" s="199"/>
-      <c r="Q15" s="199"/>
-      <c r="R15" s="199"/>
-      <c r="S15" s="199"/>
-      <c r="T15" s="199"/>
-      <c r="U15" s="199"/>
-      <c r="V15" s="200"/>
+      <c r="C15" s="200"/>
+      <c r="D15" s="200"/>
+      <c r="E15" s="200"/>
+      <c r="F15" s="200"/>
+      <c r="G15" s="200"/>
+      <c r="H15" s="200"/>
+      <c r="I15" s="200"/>
+      <c r="J15" s="200"/>
+      <c r="K15" s="200"/>
+      <c r="L15" s="200"/>
+      <c r="M15" s="200"/>
+      <c r="N15" s="200"/>
+      <c r="O15" s="200"/>
+      <c r="P15" s="200"/>
+      <c r="Q15" s="200"/>
+      <c r="R15" s="200"/>
+      <c r="S15" s="200"/>
+      <c r="T15" s="200"/>
+      <c r="U15" s="200"/>
+      <c r="V15" s="201"/>
     </row>
     <row r="16" spans="1:42" ht="26" customHeight="1">
       <c r="B16" s="134"/>
       <c r="C16" s="89"/>
       <c r="D16" s="89"/>
       <c r="E16" s="137"/>
-      <c r="F16" s="197" t="s">
+      <c r="F16" s="198" t="s">
         <v>279</v>
       </c>
-      <c r="G16" s="197"/>
-      <c r="H16" s="197"/>
-      <c r="I16" s="197"/>
-      <c r="J16" s="197"/>
-      <c r="K16" s="197"/>
-      <c r="L16" s="197"/>
-      <c r="M16" s="197"/>
-      <c r="N16" s="197"/>
-      <c r="O16" s="197"/>
-      <c r="P16" s="197"/>
-      <c r="Q16" s="197"/>
-      <c r="R16" s="197"/>
-      <c r="S16" s="212" t="s">
+      <c r="G16" s="198"/>
+      <c r="H16" s="198"/>
+      <c r="I16" s="198"/>
+      <c r="J16" s="198"/>
+      <c r="K16" s="198"/>
+      <c r="L16" s="198"/>
+      <c r="M16" s="198"/>
+      <c r="N16" s="198"/>
+      <c r="O16" s="198"/>
+      <c r="P16" s="198"/>
+      <c r="Q16" s="198"/>
+      <c r="R16" s="198"/>
+      <c r="S16" s="213" t="s">
         <v>13</v>
       </c>
-      <c r="T16" s="212"/>
-      <c r="U16" s="212" t="s">
+      <c r="T16" s="213"/>
+      <c r="U16" s="213" t="s">
         <v>228</v>
       </c>
-      <c r="V16" s="214"/>
+      <c r="V16" s="215"/>
     </row>
     <row r="17" spans="2:22" ht="26" customHeight="1">
       <c r="B17" s="132"/>
       <c r="C17" s="86"/>
       <c r="D17" s="86"/>
       <c r="E17" s="140"/>
-      <c r="F17" s="195" t="s">
+      <c r="F17" s="196" t="s">
         <v>280</v>
       </c>
-      <c r="G17" s="195"/>
-      <c r="H17" s="195"/>
-      <c r="I17" s="195"/>
-      <c r="J17" s="195"/>
-      <c r="K17" s="195"/>
-      <c r="L17" s="195"/>
-      <c r="M17" s="195"/>
-      <c r="N17" s="195"/>
-      <c r="O17" s="195"/>
-      <c r="P17" s="195"/>
-      <c r="Q17" s="195"/>
-      <c r="R17" s="195"/>
-      <c r="S17" s="204" t="s">
+      <c r="G17" s="196"/>
+      <c r="H17" s="196"/>
+      <c r="I17" s="196"/>
+      <c r="J17" s="196"/>
+      <c r="K17" s="196"/>
+      <c r="L17" s="196"/>
+      <c r="M17" s="196"/>
+      <c r="N17" s="196"/>
+      <c r="O17" s="196"/>
+      <c r="P17" s="196"/>
+      <c r="Q17" s="196"/>
+      <c r="R17" s="196"/>
+      <c r="S17" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="T17" s="204"/>
-      <c r="U17" s="204" t="s">
+      <c r="T17" s="205"/>
+      <c r="U17" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="V17" s="205"/>
+      <c r="V17" s="206"/>
     </row>
     <row r="18" spans="2:22" ht="26" customHeight="1">
       <c r="B18" s="132"/>
       <c r="C18" s="86"/>
       <c r="D18" s="86"/>
       <c r="E18" s="140"/>
-      <c r="F18" s="195" t="s">
+      <c r="F18" s="196" t="s">
         <v>286</v>
       </c>
-      <c r="G18" s="195"/>
-      <c r="H18" s="195"/>
-      <c r="I18" s="195"/>
-      <c r="J18" s="195"/>
-      <c r="K18" s="195"/>
-      <c r="L18" s="195"/>
-      <c r="M18" s="195"/>
-      <c r="N18" s="195"/>
-      <c r="O18" s="195"/>
-      <c r="P18" s="195"/>
-      <c r="Q18" s="195"/>
-      <c r="R18" s="195"/>
-      <c r="S18" s="204" t="s">
+      <c r="G18" s="196"/>
+      <c r="H18" s="196"/>
+      <c r="I18" s="196"/>
+      <c r="J18" s="196"/>
+      <c r="K18" s="196"/>
+      <c r="L18" s="196"/>
+      <c r="M18" s="196"/>
+      <c r="N18" s="196"/>
+      <c r="O18" s="196"/>
+      <c r="P18" s="196"/>
+      <c r="Q18" s="196"/>
+      <c r="R18" s="196"/>
+      <c r="S18" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="T18" s="204"/>
-      <c r="U18" s="204" t="s">
+      <c r="T18" s="205"/>
+      <c r="U18" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="V18" s="205"/>
+      <c r="V18" s="206"/>
     </row>
     <row r="19" spans="2:22" ht="26" customHeight="1">
       <c r="B19" s="132"/>
       <c r="C19" s="86"/>
       <c r="D19" s="86"/>
       <c r="E19" s="140"/>
-      <c r="F19" s="195" t="s">
+      <c r="F19" s="196" t="s">
         <v>281</v>
       </c>
-      <c r="G19" s="195"/>
-      <c r="H19" s="195"/>
-      <c r="I19" s="195"/>
-      <c r="J19" s="195"/>
-      <c r="K19" s="195"/>
-      <c r="L19" s="195"/>
-      <c r="M19" s="195"/>
-      <c r="N19" s="195"/>
-      <c r="O19" s="195"/>
-      <c r="P19" s="195"/>
-      <c r="Q19" s="195"/>
-      <c r="R19" s="195"/>
-      <c r="S19" s="204" t="s">
+      <c r="G19" s="196"/>
+      <c r="H19" s="196"/>
+      <c r="I19" s="196"/>
+      <c r="J19" s="196"/>
+      <c r="K19" s="196"/>
+      <c r="L19" s="196"/>
+      <c r="M19" s="196"/>
+      <c r="N19" s="196"/>
+      <c r="O19" s="196"/>
+      <c r="P19" s="196"/>
+      <c r="Q19" s="196"/>
+      <c r="R19" s="196"/>
+      <c r="S19" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="T19" s="204"/>
-      <c r="U19" s="204" t="s">
+      <c r="T19" s="205"/>
+      <c r="U19" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="V19" s="205"/>
+      <c r="V19" s="206"/>
     </row>
     <row r="20" spans="2:22" ht="26" customHeight="1">
       <c r="B20" s="132"/>
       <c r="C20" s="129"/>
       <c r="D20" s="129"/>
       <c r="E20" s="138"/>
-      <c r="F20" s="195" t="s">
+      <c r="F20" s="196" t="s">
         <v>282</v>
       </c>
-      <c r="G20" s="195"/>
-      <c r="H20" s="195"/>
-      <c r="I20" s="195"/>
-      <c r="J20" s="195"/>
-      <c r="K20" s="195"/>
-      <c r="L20" s="195"/>
-      <c r="M20" s="195"/>
-      <c r="N20" s="195"/>
-      <c r="O20" s="195"/>
-      <c r="P20" s="195"/>
-      <c r="Q20" s="195"/>
-      <c r="R20" s="195"/>
-      <c r="S20" s="211" t="s">
+      <c r="G20" s="196"/>
+      <c r="H20" s="196"/>
+      <c r="I20" s="196"/>
+      <c r="J20" s="196"/>
+      <c r="K20" s="196"/>
+      <c r="L20" s="196"/>
+      <c r="M20" s="196"/>
+      <c r="N20" s="196"/>
+      <c r="O20" s="196"/>
+      <c r="P20" s="196"/>
+      <c r="Q20" s="196"/>
+      <c r="R20" s="196"/>
+      <c r="S20" s="212" t="s">
         <v>228</v>
       </c>
-      <c r="T20" s="211"/>
-      <c r="U20" s="211" t="s">
+      <c r="T20" s="212"/>
+      <c r="U20" s="212" t="s">
         <v>228</v>
       </c>
-      <c r="V20" s="213"/>
+      <c r="V20" s="214"/>
     </row>
     <row r="21" spans="2:22" ht="26" customHeight="1">
       <c r="B21" s="132"/>
       <c r="C21" s="86"/>
       <c r="D21" s="86"/>
       <c r="E21" s="141"/>
-      <c r="F21" s="195" t="s">
+      <c r="F21" s="196" t="s">
         <v>283</v>
       </c>
-      <c r="G21" s="195"/>
-      <c r="H21" s="195"/>
-      <c r="I21" s="195"/>
-      <c r="J21" s="195"/>
-      <c r="K21" s="195"/>
-      <c r="L21" s="195"/>
-      <c r="M21" s="195"/>
-      <c r="N21" s="195"/>
-      <c r="O21" s="195"/>
-      <c r="P21" s="195"/>
-      <c r="Q21" s="195"/>
-      <c r="R21" s="195"/>
-      <c r="S21" s="204" t="s">
+      <c r="G21" s="196"/>
+      <c r="H21" s="196"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="196"/>
+      <c r="K21" s="196"/>
+      <c r="L21" s="196"/>
+      <c r="M21" s="196"/>
+      <c r="N21" s="196"/>
+      <c r="O21" s="196"/>
+      <c r="P21" s="196"/>
+      <c r="Q21" s="196"/>
+      <c r="R21" s="196"/>
+      <c r="S21" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="T21" s="204"/>
-      <c r="U21" s="204" t="s">
+      <c r="T21" s="205"/>
+      <c r="U21" s="205" t="s">
         <v>13</v>
       </c>
-      <c r="V21" s="205"/>
+      <c r="V21" s="206"/>
     </row>
     <row r="22" spans="2:22" ht="26" customHeight="1">
       <c r="B22" s="132"/>
       <c r="C22" s="86"/>
       <c r="D22" s="86"/>
       <c r="E22" s="141"/>
-      <c r="F22" s="195" t="s">
+      <c r="F22" s="196" t="s">
         <v>285</v>
       </c>
-      <c r="G22" s="195"/>
-      <c r="H22" s="195"/>
-      <c r="I22" s="195"/>
-      <c r="J22" s="195"/>
-      <c r="K22" s="195"/>
-      <c r="L22" s="195"/>
-      <c r="M22" s="195"/>
-      <c r="N22" s="195"/>
-      <c r="O22" s="195"/>
-      <c r="P22" s="195"/>
-      <c r="Q22" s="195"/>
-      <c r="R22" s="195"/>
-      <c r="S22" s="204" t="s">
+      <c r="G22" s="196"/>
+      <c r="H22" s="196"/>
+      <c r="I22" s="196"/>
+      <c r="J22" s="196"/>
+      <c r="K22" s="196"/>
+      <c r="L22" s="196"/>
+      <c r="M22" s="196"/>
+      <c r="N22" s="196"/>
+      <c r="O22" s="196"/>
+      <c r="P22" s="196"/>
+      <c r="Q22" s="196"/>
+      <c r="R22" s="196"/>
+      <c r="S22" s="205" t="s">
         <v>228</v>
       </c>
-      <c r="T22" s="204"/>
-      <c r="U22" s="204" t="s">
+      <c r="T22" s="205"/>
+      <c r="U22" s="205" t="s">
         <v>14</v>
       </c>
-      <c r="V22" s="205"/>
+      <c r="V22" s="206"/>
     </row>
     <row r="23" spans="2:22" ht="26" customHeight="1">
       <c r="B23" s="133"/>
       <c r="C23" s="77"/>
       <c r="D23" s="77"/>
       <c r="E23" s="142"/>
-      <c r="F23" s="196" t="s">
+      <c r="F23" s="197" t="s">
         <v>284</v>
       </c>
-      <c r="G23" s="196"/>
-      <c r="H23" s="196"/>
-      <c r="I23" s="196"/>
-      <c r="J23" s="196"/>
-      <c r="K23" s="196"/>
-      <c r="L23" s="196"/>
-      <c r="M23" s="196"/>
-      <c r="N23" s="196"/>
-      <c r="O23" s="196"/>
-      <c r="P23" s="196"/>
-      <c r="Q23" s="196"/>
-      <c r="R23" s="196"/>
-      <c r="S23" s="201" t="s">
+      <c r="G23" s="197"/>
+      <c r="H23" s="197"/>
+      <c r="I23" s="197"/>
+      <c r="J23" s="197"/>
+      <c r="K23" s="197"/>
+      <c r="L23" s="197"/>
+      <c r="M23" s="197"/>
+      <c r="N23" s="197"/>
+      <c r="O23" s="197"/>
+      <c r="P23" s="197"/>
+      <c r="Q23" s="197"/>
+      <c r="R23" s="197"/>
+      <c r="S23" s="202" t="s">
         <v>228</v>
       </c>
-      <c r="T23" s="201"/>
-      <c r="U23" s="201" t="s">
+      <c r="T23" s="202"/>
+      <c r="U23" s="202" t="s">
         <v>14</v>
       </c>
-      <c r="V23" s="202"/>
+      <c r="V23" s="203"/>
     </row>
     <row r="24" spans="2:22" ht="26" customHeight="1">
-      <c r="B24" s="198" t="s">
-        <v>292</v>
-      </c>
-      <c r="C24" s="199"/>
-      <c r="D24" s="199"/>
-      <c r="E24" s="199"/>
-      <c r="F24" s="199"/>
-      <c r="G24" s="199"/>
-      <c r="H24" s="199"/>
-      <c r="I24" s="199"/>
-      <c r="J24" s="199"/>
-      <c r="K24" s="199"/>
-      <c r="L24" s="199"/>
-      <c r="M24" s="199"/>
-      <c r="N24" s="199"/>
-      <c r="O24" s="199"/>
-      <c r="P24" s="199"/>
-      <c r="Q24" s="199"/>
-      <c r="R24" s="199"/>
-      <c r="S24" s="199"/>
-      <c r="T24" s="199"/>
-      <c r="U24" s="199"/>
-      <c r="V24" s="200"/>
+      <c r="B24" s="199" t="s">
+        <v>294</v>
+      </c>
+      <c r="C24" s="200"/>
+      <c r="D24" s="200"/>
+      <c r="E24" s="200"/>
+      <c r="F24" s="200"/>
+      <c r="G24" s="200"/>
+      <c r="H24" s="200"/>
+      <c r="I24" s="200"/>
+      <c r="J24" s="200"/>
+      <c r="K24" s="200"/>
+      <c r="L24" s="200"/>
+      <c r="M24" s="200"/>
+      <c r="N24" s="200"/>
+      <c r="O24" s="200"/>
+      <c r="P24" s="200"/>
+      <c r="Q24" s="200"/>
+      <c r="R24" s="200"/>
+      <c r="S24" s="200"/>
+      <c r="T24" s="200"/>
+      <c r="U24" s="200"/>
+      <c r="V24" s="201"/>
     </row>
     <row r="25" spans="2:22" ht="26" customHeight="1">
       <c r="B25" s="134"/>
       <c r="C25" s="89"/>
       <c r="D25" s="89"/>
       <c r="E25" s="137"/>
-      <c r="F25" s="197" t="s">
-        <v>293</v>
-      </c>
-      <c r="G25" s="197"/>
-      <c r="H25" s="197"/>
-      <c r="I25" s="197"/>
-      <c r="J25" s="197"/>
-      <c r="K25" s="197"/>
-      <c r="L25" s="197"/>
-      <c r="M25" s="197"/>
-      <c r="N25" s="197"/>
-      <c r="O25" s="197"/>
-      <c r="P25" s="197"/>
-      <c r="Q25" s="197"/>
-      <c r="R25" s="197"/>
-      <c r="S25" s="212" t="s">
+      <c r="F25" s="198" t="s">
+        <v>292</v>
+      </c>
+      <c r="G25" s="198"/>
+      <c r="H25" s="198"/>
+      <c r="I25" s="198"/>
+      <c r="J25" s="198"/>
+      <c r="K25" s="198"/>
+      <c r="L25" s="198"/>
+      <c r="M25" s="198"/>
+      <c r="N25" s="198"/>
+      <c r="O25" s="198"/>
+      <c r="P25" s="198"/>
+      <c r="Q25" s="198"/>
+      <c r="R25" s="198"/>
+      <c r="S25" s="213" t="s">
         <v>228</v>
       </c>
-      <c r="T25" s="212"/>
-      <c r="U25" s="212" t="s">
+      <c r="T25" s="213"/>
+      <c r="U25" s="213" t="s">
         <v>228</v>
       </c>
-      <c r="V25" s="214"/>
+      <c r="V25" s="215"/>
     </row>
     <row r="26" spans="2:22" ht="26" customHeight="1">
       <c r="B26" s="133"/>
       <c r="C26" s="77"/>
       <c r="D26" s="77"/>
       <c r="E26" s="136"/>
-      <c r="F26" s="196" t="s">
-        <v>294</v>
-      </c>
-      <c r="G26" s="196"/>
-      <c r="H26" s="196"/>
-      <c r="I26" s="196"/>
-      <c r="J26" s="196"/>
-      <c r="K26" s="196"/>
-      <c r="L26" s="196"/>
-      <c r="M26" s="196"/>
-      <c r="N26" s="196"/>
-      <c r="O26" s="196"/>
-      <c r="P26" s="196"/>
-      <c r="Q26" s="196"/>
-      <c r="R26" s="196"/>
-      <c r="S26" s="201" t="s">
+      <c r="F26" s="197" t="s">
+        <v>293</v>
+      </c>
+      <c r="G26" s="197"/>
+      <c r="H26" s="197"/>
+      <c r="I26" s="197"/>
+      <c r="J26" s="197"/>
+      <c r="K26" s="197"/>
+      <c r="L26" s="197"/>
+      <c r="M26" s="197"/>
+      <c r="N26" s="197"/>
+      <c r="O26" s="197"/>
+      <c r="P26" s="197"/>
+      <c r="Q26" s="197"/>
+      <c r="R26" s="197"/>
+      <c r="S26" s="202" t="s">
         <v>13</v>
       </c>
-      <c r="T26" s="201"/>
-      <c r="U26" s="201" t="s">
+      <c r="T26" s="202"/>
+      <c r="U26" s="202" t="s">
         <v>228</v>
       </c>
-      <c r="V26" s="202"/>
+      <c r="V26" s="203"/>
     </row>
   </sheetData>
   <mergeCells count="51">
@@ -54945,8 +55199,8 @@
       <c r="C3" s="55"/>
       <c r="D3" s="55"/>
       <c r="E3" s="55"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
+      <c r="F3" s="216"/>
+      <c r="G3" s="216"/>
       <c r="H3" s="56"/>
       <c r="I3" s="55"/>
       <c r="J3" s="55"/>

</xml_diff>